<commit_message>
refactor: :recycle: adding a time tree do handle date occurrences
</commit_message>
<xml_diff>
--- a/poc.xlsx
+++ b/poc.xlsx
@@ -8,22 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\renatospaka\dev\heykid\draft\poc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FD7983-A8FB-4EE6-91C0-F8F485300185}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC5408D-7F1A-4E6D-8C46-B722A4543D77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="complication" sheetId="1" r:id="rId1"/>
-    <sheet name="specialty" sheetId="2" r:id="rId2"/>
-    <sheet name="disease" sheetId="3" r:id="rId3"/>
-    <sheet name="allergy" sheetId="4" r:id="rId4"/>
-    <sheet name="intolerance" sheetId="5" r:id="rId5"/>
-    <sheet name="vaccine" sheetId="6" r:id="rId6"/>
-    <sheet name="vaccine dose" sheetId="7" r:id="rId7"/>
+    <sheet name="disease" sheetId="3" r:id="rId2"/>
+    <sheet name="measurement" sheetId="8" r:id="rId3"/>
+    <sheet name="specialty" sheetId="2" r:id="rId4"/>
+    <sheet name="allergy" sheetId="4" r:id="rId5"/>
+    <sheet name="intolerance" sheetId="5" r:id="rId6"/>
+    <sheet name="vaccine" sheetId="6" r:id="rId7"/>
+    <sheet name="vaccine dose" sheetId="7" r:id="rId8"/>
+    <sheet name="Date Range" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">disease!$A$1:$D$74</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'vaccine dose'!$A$1:$F$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">disease!$A$1:$D$74</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'vaccine dose'!$A$1:$F$55</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="373">
   <si>
     <t>Tipos</t>
   </si>
@@ -1154,6 +1156,88 @@
   </si>
   <si>
     <t>Query Relationship</t>
+  </si>
+  <si>
+    <t>MERGE (r:TimeTreeRoot)
+WITH r, range(2010, 2020) AS years, range(1,12) as months
+FOREACH(year IN years |
+  MERGE (y:Year {value: year})
+  MERGE (r)-[:CHILD]-&gt;(y)
+  FOREACH(month IN months |
+    CREATE (m:Month {value: month})
+    MERGE (y)-[:CHILD]-&gt;(m)
+    FOREACH(day IN (CASE
+                      WHEN month IN [1,3,5,7,8,10,12] THEN range(1,31)
+                      WHEN month = 2 THEN
+                        CASE
+                          WHEN year % 4 &lt;&gt; 0 THEN range(1,28)
+                          WHEN year % 100 &lt;&gt; 0 THEN range(1,29)
+                          WHEN year % 400 &lt;&gt; 0 THEN range(1,29)
+                          ELSE range(1,28)
+                        END
+                      ELSE range(1,30)
+                    END) |
+      CREATE (d:Day {value: day})
+      MERGE (m)-[:CHILD]-&gt;(d))))
+WITH *
+//Create years linked list
+MATCH (root:TimeTreeRoot)--&gt;(year:Year)
+WITH root, year ORDER BY year.value
+WITH root, collect(year) as years
+WITH root, years, years[0] AS first, years[size(years)-1] AS last
+MERGE (root)-[:FIRST]-&gt;(first)
+MERGE (root)-[:LAST]-&gt;(last)
+FOREACH(i in RANGE(0, size(years)-2) |
+    FOREACH(year1 in [years[i]] |
+        FOREACH(year2 in [years[i+1]] |
+            MERGE (year1)-[:NEXT]-&gt;(year2))))
+WITH *
+//Create months linked list
+MATCH (year:Year)
+WITH collect(year) as years
+UNWIND years AS year
+	MATCH (year)--(first:Month {value: 1}), (year)--(last:Month {value: 12})
+	MERGE (year)-[:FIRST]-&gt;(first)
+	MERGE (year)-[:LAST]-&gt;(last)
+WITH *
+MATCH (year:Year)-[:CHILD]-&gt;(month:Month)
+WITH year, month
+ORDER BY year.value, month.value
+WITH collect(month) as months
+FOREACH(i in RANGE(0, size(months)-2) |
+    FOREACH(month1 in [months[i]] |
+        FOREACH(month2 in [months[i+1]] |
+            MERGE (month1)-[:NEXT]-&gt;(month2))))
+WITH *
+//Create days linked list
+MATCH (month:Month)
+WITH collect(month) as months
+UNWIND months AS month
+	MATCH (month)-[:CHILD]-&gt;(day:Day)
+	WITH month, collect(day) AS days
+	WITH month, days[0] AS first, days[size(days)-1] AS last
+	MERGE (month)-[:FIRST]-&gt;(first)
+	MERGE (month)-[:LAST]-&gt;(last)
+WITH *
+MATCH (year:Year)-[:CHILD]-&gt;(month:Month)-[:CHILD]-&gt;(day:Day)
+WITH year,month,day
+ORDER BY year.value, month.value, day.value
+WITH collect(day) as days
+FOREACH(i in RANGE(0, size(days)-2) |
+    FOREACH(day1 in [days[i]] |
+        FOREACH(day2 in [days[i+1]] |
+            MERGE (day1)-[:NEXT]-&gt;(day2))))
+;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATCH (year:Year)-[:CHILD]-&gt;(month:Month)-[:CHILD]-&gt;(day:Day)
+WHERE year.value &gt;=2018
+RETURN year.value AS Year, month.value AS Month, day.value AS Day
+ORDER BY Year, Month, Day
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creates a Date structure to allow connecting date nodes to other nodes instead of pure properties </t>
   </si>
 </sst>
 </file>
@@ -1189,11 +1273,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1478,6 +1565,1235 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.44140625" customWidth="1"/>
+    <col min="3" max="3" width="30.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C18" si="0">"(:Complication {name: '" &amp; B2 &amp;"', inPortuguese: '" &amp; A2 &amp;"'}),"</f>
+        <v>(:Complication {name: 'Cry', inPortuguese: 'Choro'}),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>292</v>
+      </c>
+      <c r="B3" t="s">
+        <v>309</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Complication {name: 'Fever', inPortuguese: 'Febre'}),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B4" t="s">
+        <v>310</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Complication {name: 'Vomiting', inPortuguese: 'Vômito'}),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>294</v>
+      </c>
+      <c r="B5" t="s">
+        <v>311</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Complication {name: 'Diarrhea', inPortuguese: 'Diarreia'}),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>295</v>
+      </c>
+      <c r="B6" t="s">
+        <v>312</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Complication {name: 'Coryza', inPortuguese: 'Coriza'}),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>296</v>
+      </c>
+      <c r="B7" t="s">
+        <v>313</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Complication {name: 'Stress', inPortuguese: 'Estresse'}),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>297</v>
+      </c>
+      <c r="B8" t="s">
+        <v>314</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Complication {name: 'Cough', inPortuguese: 'Tosse'}),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>298</v>
+      </c>
+      <c r="B9" t="s">
+        <v>315</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Complication {name: 'Sneeze', inPortuguese: 'Espirro'}),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>299</v>
+      </c>
+      <c r="B10" t="s">
+        <v>316</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Complication {name: 'Nausea', inPortuguese: 'Náusea'}),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>300</v>
+      </c>
+      <c r="B11" t="s">
+        <v>317</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Complication {name: 'Fall', inPortuguese: 'Queda'}),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>301</v>
+      </c>
+      <c r="B12" t="s">
+        <v>318</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Complication {name: 'Vertigo', inPortuguese: 'Vertigem'}),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>302</v>
+      </c>
+      <c r="B13" t="s">
+        <v>319</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Complication {name: 'Twist', inPortuguese: 'Torção'}),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>303</v>
+      </c>
+      <c r="B14" t="s">
+        <v>320</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Complication {name: 'Cut', inPortuguese: 'Corte'}),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>304</v>
+      </c>
+      <c r="B15" t="s">
+        <v>321</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Complication {name: 'Shock', inPortuguese: 'Choque'}),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>305</v>
+      </c>
+      <c r="B16" t="s">
+        <v>322</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Complication {name: 'Weakness', inPortuguese: 'Fraqueza'}),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>306</v>
+      </c>
+      <c r="B17" t="s">
+        <v>323</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Complication {name: 'Ingestion', inPortuguese: 'Ingestão'}),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>307</v>
+      </c>
+      <c r="B18" t="s">
+        <v>324</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Complication {name: 'Ache', inPortuguese: 'Dor'}),</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16822055-6D7C-4562-869B-B3AD28812FB9}">
+  <dimension ref="A1:D81"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D33" si="0">"(:Disease {name: '" &amp; B2 &amp;"', inPortuguese: '" &amp; A2 &amp;"'}),"</f>
+        <v>(:Disease {name: 'Headache', inPortuguese: 'Cefaleia'}),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Disease {name: 'Migraine', inPortuguese: 'Enxaqueca'}),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Disease {name: 'Rhinitis', inPortuguese: 'Rinite'}),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Disease {name: 'Sinusitis', inPortuguese: 'Sinusite'}),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Disease {name: 'Asthma', inPortuguese: 'Asma'}),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Disease {name: 'Diabetes', inPortuguese: 'Diabetes'}),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Disease {name: 'Hepatitis', inPortuguese: 'Hepatite'}),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Disease {name: 'Depression', inPortuguese: 'Depressão'}),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Disease {name: 'Anemia', inPortuguese: 'Anemia'}),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Disease {name: 'Obesity', inPortuguese: 'Obesidade'}),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Disease {name: 'Hypertension', inPortuguese: 'Hipertensão Arterial'}),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Disease {name: 'Astigmatism', inPortuguese: 'Astigmatismo'}),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Disease {name: 'Myopia', inPortuguese: 'Miopia'}),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" t="s">
+        <v>99</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Disease {name: 'Hyperopia', inPortuguese: 'Hipermetropia'}),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Disease {name: 'Blindness', inPortuguese: 'Cegueira'}),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Disease {name: 'Presbyopia', inPortuguese: 'Presbiopia'}),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Disease {name: 'Cataract', inPortuguese: 'Catarata'}),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Disease {name: 'Glaucoma', inPortuguese: 'Glaucoma'}),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Disease {name: 'Conjunctivitis', inPortuguese: 'Conjuntivite'}),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>142</v>
+      </c>
+      <c r="B21" t="s">
+        <v>149</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Disease {name: 'Diabetic Retinopathy', inPortuguese: 'Retinopatia Diabética'}),</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" t="s">
+        <v>104</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Disease {name: 'Deafness', inPortuguese: 'Surdez'}),</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" t="s">
+        <v>105</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Disease {name: 'Otitis', inPortuguese: 'Otite'}),</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" t="s">
+        <v>106</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Disease {name: 'Labyrinthitis', inPortuguese: 'Labirintite'}),</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Disease {name: 'Tinnutus', inPortuguese: 'Tinnutus'}),</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" t="s">
+        <v>107</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Disease {name: 'Otosclerosis', inPortuguese: 'Otosclerose'}),</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" t="s">
+        <v>108</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Disease {name: 'Ototoxicity', inPortuguese: 'Ototoxicidade'}),</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" t="s">
+        <v>150</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Disease {name: 'Usher Syndrome', inPortuguese: 'Síndrome de Usher'}),</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" t="s">
+        <v>109</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Disease {name: 'Acoustic Neuroma', inPortuguese: 'Neuroma do Acústico'}),</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" t="s">
+        <v>151</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Disease {name: 'Meniere Disease', inPortuguese: 'Doença de Ménière'}),</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" t="s">
+        <v>110</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Disease {name: 'Stuttering', inPortuguese: 'Gagueira'}),</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" t="s">
+        <v>111</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Disease {name: 'Mute', inPortuguese: 'Mudez'}),</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" t="s">
+        <v>112</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Disease {name: 'Aphasia', inPortuguese: 'Afasia'}),</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" t="s">
+        <v>113</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" ref="D34:D65" si="1">"(:Disease {name: '" &amp; B34 &amp;"', inPortuguese: '" &amp; A34 &amp;"'}),"</f>
+        <v>(:Disease {name: 'Dysarthria', inPortuguese: 'Disartria'}),</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" t="s">
+        <v>114</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {name: 'Dystonia', inPortuguese: 'Distonia'}),</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" t="s">
+        <v>115</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {name: 'Cancer', inPortuguese: 'Câncer'}),</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37" t="s">
+        <v>116</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {name: 'Bipolarity', inPortuguese: 'Bipolaridade'}),</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" t="s">
+        <v>117</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {name: 'Schizophrenia', inPortuguese: 'Esquizifrenia'}),</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>143</v>
+      </c>
+      <c r="B39" t="s">
+        <v>152</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {name: 'Gastroesophageal Reflux', inPortuguese: 'Refluxo Gastroesofágico'}),</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>144</v>
+      </c>
+      <c r="B40" t="s">
+        <v>118</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {name: 'Gallstone', inPortuguese: 'Cálculo Biliar'}),</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" t="s">
+        <v>119</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {name: 'Pancreatitis', inPortuguese: 'Pancreatite'}),</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>145</v>
+      </c>
+      <c r="B42" t="s">
+        <v>153</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {name: 'Abdominal Hernia', inPortuguese: 'Hérnia Abdominal'}),</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>146</v>
+      </c>
+      <c r="B43" t="s">
+        <v>154</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {name: 'Hepatic Steatosis', inPortuguese: 'Esteatose Hepática'}),</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>78</v>
+      </c>
+      <c r="B44" t="s">
+        <v>120</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {name: 'Gastritis', inPortuguese: 'Gastrite'}),</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>79</v>
+      </c>
+      <c r="B45" t="s">
+        <v>121</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {name: 'Ulcer', inPortuguese: 'Úlcera'}),</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>147</v>
+      </c>
+      <c r="B46" t="s">
+        <v>122</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {name: 'Constipation', inPortuguese: 'Prisão de Ventre'}),</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>80</v>
+      </c>
+      <c r="B47" t="s">
+        <v>123</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {name: 'Appendicitis', inPortuguese: 'Apendicite'}),</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>81</v>
+      </c>
+      <c r="B48" t="s">
+        <v>124</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {name: 'Diverticulitis', inPortuguese: 'Diverticulite'}),</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>82</v>
+      </c>
+      <c r="B49" t="s">
+        <v>125</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {name: 'Heartburn', inPortuguese: 'Azia'}),</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>83</v>
+      </c>
+      <c r="B50" t="s">
+        <v>126</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {name: 'Dyspepsia', inPortuguese: 'Dispepsia'}),</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>84</v>
+      </c>
+      <c r="B51" t="s">
+        <v>84</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {name: 'Alzheimer', inPortuguese: 'Alzheimer'}),</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>148</v>
+      </c>
+      <c r="B52" t="s">
+        <v>148</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {name: 'Aids', inPortuguese: 'Aids'}),</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>85</v>
+      </c>
+      <c r="B53" t="s">
+        <v>127</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {name: 'Stroke', inPortuguese: 'Acidente Vascular Cerebral'}),</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>86</v>
+      </c>
+      <c r="B54" t="s">
+        <v>86</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {name: 'Parkinson', inPortuguese: 'Parkinson'}),</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>87</v>
+      </c>
+      <c r="B55" t="s">
+        <v>155</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {name: 'Polio', inPortuguese: 'Poliomielite'}),</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>128</v>
+      </c>
+      <c r="B56" t="s">
+        <v>134</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {name: 'Dyslipidemia', inPortuguese: 'Dislipidemia'}),</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>172</v>
+      </c>
+      <c r="B57" t="s">
+        <v>135</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {name: 'Ischemic Heart Disease', inPortuguese: 'Cardiopatia Isquêmica'}),</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>129</v>
+      </c>
+      <c r="B58" t="s">
+        <v>136</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {name: 'Cardiac Insufficiency', inPortuguese: 'Insuficiência Cardíaca'}),</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>173</v>
+      </c>
+      <c r="B59" t="s">
+        <v>137</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {name: 'Atrial Fibrillation', inPortuguese: 'Fibrilação Atrial'}),</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>130</v>
+      </c>
+      <c r="B60" t="s">
+        <v>138</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {name: 'Stomatitis', inPortuguese: 'Estomatite'}),</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>131</v>
+      </c>
+      <c r="B61" t="s">
+        <v>139</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {name: 'Crohn Disease', inPortuguese: 'Doença de Crohn'}),</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>132</v>
+      </c>
+      <c r="B62" t="s">
+        <v>140</v>
+      </c>
+      <c r="D62" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {name: 'Irritable Bowel Syndrome', inPortuguese: 'Síndrome do Intestino Irritável'}),</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>174</v>
+      </c>
+      <c r="B63" t="s">
+        <v>141</v>
+      </c>
+      <c r="D63" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {name: 'Ulcerative Colitis', inPortuguese: 'Retocolite Ulcerativa'}),</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>133</v>
+      </c>
+      <c r="B64" t="s">
+        <v>122</v>
+      </c>
+      <c r="D64" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {name: 'Constipation', inPortuguese: 'Obstipação'}),</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>156</v>
+      </c>
+      <c r="B65" t="s">
+        <v>164</v>
+      </c>
+      <c r="D65" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {name: 'Arthrosis', inPortuguese: 'Artrose'}),</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>157</v>
+      </c>
+      <c r="B66" t="s">
+        <v>165</v>
+      </c>
+      <c r="D66" t="str">
+        <f t="shared" ref="D66:D81" si="2">"(:Disease {name: '" &amp; B66 &amp;"', inPortuguese: '" &amp; A66 &amp;"'}),"</f>
+        <v>(:Disease {name: 'Flat Feet', inPortuguese: 'Pé Chato'}),</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>158</v>
+      </c>
+      <c r="B67" t="s">
+        <v>166</v>
+      </c>
+      <c r="D67" t="str">
+        <f t="shared" si="2"/>
+        <v>(:Disease {name: 'Tendonitis', inPortuguese: 'Tendinite'}),</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>159</v>
+      </c>
+      <c r="B68" t="s">
+        <v>167</v>
+      </c>
+      <c r="D68" t="str">
+        <f t="shared" si="2"/>
+        <v>(:Disease {name: 'Bursitis', inPortuguese: 'Bursite'}),</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>160</v>
+      </c>
+      <c r="B69" t="s">
+        <v>168</v>
+      </c>
+      <c r="D69" t="str">
+        <f t="shared" si="2"/>
+        <v>(:Disease {name: 'Ligament Rupture', inPortuguese: 'Ruptura de Ligamento'}),</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>161</v>
+      </c>
+      <c r="B70" t="s">
+        <v>169</v>
+      </c>
+      <c r="D70" t="str">
+        <f t="shared" si="2"/>
+        <v>(:Disease {name: 'Backache', inPortuguese: 'Lombalgia'}),</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>162</v>
+      </c>
+      <c r="B71" t="s">
+        <v>170</v>
+      </c>
+      <c r="D71" t="str">
+        <f t="shared" si="2"/>
+        <v>(:Disease {name: 'Plantar Fasciitis', inPortuguese: 'Fascite Plantar'}),</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>163</v>
+      </c>
+      <c r="B72" t="s">
+        <v>171</v>
+      </c>
+      <c r="D72" t="str">
+        <f t="shared" si="2"/>
+        <v>(:Disease {name: 'Osteoporosis', inPortuguese: 'Osteoporose'}),</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>175</v>
+      </c>
+      <c r="B73" t="s">
+        <v>180</v>
+      </c>
+      <c r="D73" t="str">
+        <f t="shared" si="2"/>
+        <v>(:Disease {name: 'Pulmonary Emphysema', inPortuguese: 'Enfisema Pulmonar'}),</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>176</v>
+      </c>
+      <c r="B74" t="s">
+        <v>181</v>
+      </c>
+      <c r="D74" t="str">
+        <f t="shared" si="2"/>
+        <v>(:Disease {name: 'Bronchitis', inPortuguese: 'Bronquite'}),</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>177</v>
+      </c>
+      <c r="B75" t="s">
+        <v>182</v>
+      </c>
+      <c r="D75" t="str">
+        <f t="shared" si="2"/>
+        <v>(:Disease {name: 'Tuberculosis', inPortuguese: 'Tuberculose'}),</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>178</v>
+      </c>
+      <c r="B76" t="s">
+        <v>183</v>
+      </c>
+      <c r="D76" t="str">
+        <f t="shared" si="2"/>
+        <v>(:Disease {name: 'Pharyngitis', inPortuguese: 'Faringite'}),</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>179</v>
+      </c>
+      <c r="B77" t="s">
+        <v>179</v>
+      </c>
+      <c r="D77" t="str">
+        <f t="shared" si="2"/>
+        <v>(:Disease {name: 'Pneumonia', inPortuguese: 'Pneumonia'}),</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>185</v>
+      </c>
+      <c r="B78" t="s">
+        <v>189</v>
+      </c>
+      <c r="D78" t="str">
+        <f t="shared" si="2"/>
+        <v>(:Disease {name: 'Allergic Urticaria', inPortuguese: 'Urticária Alérgica'}),</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>186</v>
+      </c>
+      <c r="B79" t="s">
+        <v>186</v>
+      </c>
+      <c r="D79" t="str">
+        <f t="shared" si="2"/>
+        <v>(:Disease {name: 'Angioedema', inPortuguese: 'Angioedema'}),</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>187</v>
+      </c>
+      <c r="B80" t="s">
+        <v>190</v>
+      </c>
+      <c r="D80" t="str">
+        <f t="shared" si="2"/>
+        <v>(:Disease {name: 'Contact Dermatitis', inPortuguese: 'Dermatite de Contato'}),</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>188</v>
+      </c>
+      <c r="B81" t="s">
+        <v>191</v>
+      </c>
+      <c r="D81" t="str">
+        <f t="shared" si="2"/>
+        <v>(:Disease {name: 'Atopic Dermatitis', inPortuguese: 'Dermatite Atópica'}),</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D74" xr:uid="{B2FAB676-2031-4EBE-8374-605422BD9A7E}"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F5CDE23-EAB5-47A7-B33D-96F18BE56CCE}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C18"/>
     </sheetView>
   </sheetViews>
@@ -1506,8 +2822,8 @@
         <v>308</v>
       </c>
       <c r="C2" t="str">
-        <f>"(:Complication {name: '" &amp; B2 &amp;"', inPortuguese: '" &amp; A2 &amp;"'}),"</f>
-        <v>(:Complication {name: 'Cry', inPortuguese: 'Choro'}),</v>
+        <f>"(:Measurement {name: '" &amp; B2 &amp;"', inPortuguese: '" &amp; A2 &amp;"'}),"</f>
+        <v>(:Measurement {name: 'Cry', inPortuguese: 'Choro'}),</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1518,8 +2834,8 @@
         <v>309</v>
       </c>
       <c r="C3" t="str">
-        <f>"(:Complication {name: '" &amp; B3 &amp;"', inPortuguese: '" &amp; A3 &amp;"'}),"</f>
-        <v>(:Complication {name: 'Fever', inPortuguese: 'Febre'}),</v>
+        <f t="shared" ref="C3:C18" si="0">"(:Measurement {name: '" &amp; B3 &amp;"', inPortuguese: '" &amp; A3 &amp;"'}),"</f>
+        <v>(:Measurement {name: 'Fever', inPortuguese: 'Febre'}),</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1530,8 +2846,8 @@
         <v>310</v>
       </c>
       <c r="C4" t="str">
-        <f>"(:Complication {name: '" &amp; B4 &amp;"', inPortuguese: '" &amp; A4 &amp;"'}),"</f>
-        <v>(:Complication {name: 'Vomiting', inPortuguese: 'Vômito'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Measurement {name: 'Vomiting', inPortuguese: 'Vômito'}),</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1542,8 +2858,8 @@
         <v>311</v>
       </c>
       <c r="C5" t="str">
-        <f>"(:Complication {name: '" &amp; B5 &amp;"', inPortuguese: '" &amp; A5 &amp;"'}),"</f>
-        <v>(:Complication {name: 'Diarrhea', inPortuguese: 'Diarreia'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Measurement {name: 'Diarrhea', inPortuguese: 'Diarreia'}),</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1554,8 +2870,8 @@
         <v>312</v>
       </c>
       <c r="C6" t="str">
-        <f>"(:Complication {name: '" &amp; B6 &amp;"', inPortuguese: '" &amp; A6 &amp;"'}),"</f>
-        <v>(:Complication {name: 'Coryza', inPortuguese: 'Coriza'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Measurement {name: 'Coryza', inPortuguese: 'Coriza'}),</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1566,8 +2882,8 @@
         <v>313</v>
       </c>
       <c r="C7" t="str">
-        <f>"(:Complication {name: '" &amp; B7 &amp;"', inPortuguese: '" &amp; A7 &amp;"'}),"</f>
-        <v>(:Complication {name: 'Stress', inPortuguese: 'Estresse'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Measurement {name: 'Stress', inPortuguese: 'Estresse'}),</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1578,8 +2894,8 @@
         <v>314</v>
       </c>
       <c r="C8" t="str">
-        <f>"(:Complication {name: '" &amp; B8 &amp;"', inPortuguese: '" &amp; A8 &amp;"'}),"</f>
-        <v>(:Complication {name: 'Cough', inPortuguese: 'Tosse'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Measurement {name: 'Cough', inPortuguese: 'Tosse'}),</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1590,8 +2906,8 @@
         <v>315</v>
       </c>
       <c r="C9" t="str">
-        <f>"(:Complication {name: '" &amp; B9 &amp;"', inPortuguese: '" &amp; A9 &amp;"'}),"</f>
-        <v>(:Complication {name: 'Sneeze', inPortuguese: 'Espirro'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Measurement {name: 'Sneeze', inPortuguese: 'Espirro'}),</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1602,8 +2918,8 @@
         <v>316</v>
       </c>
       <c r="C10" t="str">
-        <f>"(:Complication {name: '" &amp; B10 &amp;"', inPortuguese: '" &amp; A10 &amp;"'}),"</f>
-        <v>(:Complication {name: 'Nausea', inPortuguese: 'Náusea'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Measurement {name: 'Nausea', inPortuguese: 'Náusea'}),</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1614,8 +2930,8 @@
         <v>317</v>
       </c>
       <c r="C11" t="str">
-        <f>"(:Complication {name: '" &amp; B11 &amp;"', inPortuguese: '" &amp; A11 &amp;"'}),"</f>
-        <v>(:Complication {name: 'Fall', inPortuguese: 'Queda'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Measurement {name: 'Fall', inPortuguese: 'Queda'}),</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1626,8 +2942,8 @@
         <v>318</v>
       </c>
       <c r="C12" t="str">
-        <f>"(:Complication {name: '" &amp; B12 &amp;"', inPortuguese: '" &amp; A12 &amp;"'}),"</f>
-        <v>(:Complication {name: 'Vertigo', inPortuguese: 'Vertigem'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Measurement {name: 'Vertigo', inPortuguese: 'Vertigem'}),</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1638,8 +2954,8 @@
         <v>319</v>
       </c>
       <c r="C13" t="str">
-        <f>"(:Complication {name: '" &amp; B13 &amp;"', inPortuguese: '" &amp; A13 &amp;"'}),"</f>
-        <v>(:Complication {name: 'Twist', inPortuguese: 'Torção'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Measurement {name: 'Twist', inPortuguese: 'Torção'}),</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -1650,8 +2966,8 @@
         <v>320</v>
       </c>
       <c r="C14" t="str">
-        <f>"(:Complication {name: '" &amp; B14 &amp;"', inPortuguese: '" &amp; A14 &amp;"'}),"</f>
-        <v>(:Complication {name: 'Cut', inPortuguese: 'Corte'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Measurement {name: 'Cut', inPortuguese: 'Corte'}),</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -1662,8 +2978,8 @@
         <v>321</v>
       </c>
       <c r="C15" t="str">
-        <f>"(:Complication {name: '" &amp; B15 &amp;"', inPortuguese: '" &amp; A15 &amp;"'}),"</f>
-        <v>(:Complication {name: 'Shock', inPortuguese: 'Choque'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Measurement {name: 'Shock', inPortuguese: 'Choque'}),</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -1674,8 +2990,8 @@
         <v>322</v>
       </c>
       <c r="C16" t="str">
-        <f>"(:Complication {name: '" &amp; B16 &amp;"', inPortuguese: '" &amp; A16 &amp;"'}),"</f>
-        <v>(:Complication {name: 'Weakness', inPortuguese: 'Fraqueza'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Measurement {name: 'Weakness', inPortuguese: 'Fraqueza'}),</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -1686,8 +3002,8 @@
         <v>323</v>
       </c>
       <c r="C17" t="str">
-        <f>"(:Complication {name: '" &amp; B17 &amp;"', inPortuguese: '" &amp; A17 &amp;"'}),"</f>
-        <v>(:Complication {name: 'Ingestion', inPortuguese: 'Ingestão'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Measurement {name: 'Ingestion', inPortuguese: 'Ingestão'}),</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -1698,8 +3014,8 @@
         <v>324</v>
       </c>
       <c r="C18" t="str">
-        <f>"(:Complication {name: '" &amp; B18 &amp;"', inPortuguese: '" &amp; A18 &amp;"'}),"</f>
-        <v>(:Complication {name: 'Ache', inPortuguese: 'Dor'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Measurement {name: 'Ache', inPortuguese: 'Dor'}),</v>
       </c>
     </row>
   </sheetData>
@@ -1707,7 +3023,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8BE5788-872A-43B9-9E25-E8C1A583BFB6}">
   <dimension ref="A1:C20"/>
   <sheetViews>
@@ -1740,7 +3056,7 @@
         <v>22</v>
       </c>
       <c r="C2" t="str">
-        <f>"(:Specialty {name: '" &amp; B2 &amp;"', inPortuguese: '" &amp; A2 &amp;"'}),"</f>
+        <f t="shared" ref="C2:C20" si="0">"(:Specialty {name: '" &amp; B2 &amp;"', inPortuguese: '" &amp; A2 &amp;"'}),"</f>
         <v>(:Specialty {name: 'Pediatrician', inPortuguese: 'Pediatra'}),</v>
       </c>
     </row>
@@ -1752,7 +3068,7 @@
         <v>23</v>
       </c>
       <c r="C3" t="str">
-        <f>"(:Specialty {name: '" &amp; B3 &amp;"', inPortuguese: '" &amp; A3 &amp;"'}),"</f>
+        <f t="shared" si="0"/>
         <v>(:Specialty {name: 'Otolaryngologist', inPortuguese: 'Otorrinolaringologista'}),</v>
       </c>
     </row>
@@ -1764,7 +3080,7 @@
         <v>24</v>
       </c>
       <c r="C4" t="str">
-        <f>"(:Specialty {name: '" &amp; B4 &amp;"', inPortuguese: '" &amp; A4 &amp;"'}),"</f>
+        <f t="shared" si="0"/>
         <v>(:Specialty {name: 'Ophthalmologist', inPortuguese: 'Oftalmologista'}),</v>
       </c>
     </row>
@@ -1776,7 +3092,7 @@
         <v>25</v>
       </c>
       <c r="C5" t="str">
-        <f>"(:Specialty {name: '" &amp; B5 &amp;"', inPortuguese: '" &amp; A5 &amp;"'}),"</f>
+        <f t="shared" si="0"/>
         <v>(:Specialty {name: 'Allergist', inPortuguese: 'Alergologista'}),</v>
       </c>
     </row>
@@ -1788,7 +3104,7 @@
         <v>26</v>
       </c>
       <c r="C6" t="str">
-        <f>"(:Specialty {name: '" &amp; B6 &amp;"', inPortuguese: '" &amp; A6 &amp;"'}),"</f>
+        <f t="shared" si="0"/>
         <v>(:Specialty {name: 'Dentist', inPortuguese: 'Dentista'}),</v>
       </c>
     </row>
@@ -1800,7 +3116,7 @@
         <v>27</v>
       </c>
       <c r="C7" t="str">
-        <f>"(:Specialty {name: '" &amp; B7 &amp;"', inPortuguese: '" &amp; A7 &amp;"'}),"</f>
+        <f t="shared" si="0"/>
         <v>(:Specialty {name: 'Endocrinologist', inPortuguese: 'Endocrinologista'}),</v>
       </c>
     </row>
@@ -1812,7 +3128,7 @@
         <v>28</v>
       </c>
       <c r="C8" t="str">
-        <f>"(:Specialty {name: '" &amp; B8 &amp;"', inPortuguese: '" &amp; A8 &amp;"'}),"</f>
+        <f t="shared" si="0"/>
         <v>(:Specialty {name: 'Orthopedist', inPortuguese: 'Ortopedista'}),</v>
       </c>
     </row>
@@ -1824,7 +3140,7 @@
         <v>29</v>
       </c>
       <c r="C9" t="str">
-        <f>"(:Specialty {name: '" &amp; B9 &amp;"', inPortuguese: '" &amp; A9 &amp;"'}),"</f>
+        <f t="shared" si="0"/>
         <v>(:Specialty {name: 'Pulmonologist', inPortuguese: 'Pneumologista'}),</v>
       </c>
     </row>
@@ -1836,7 +3152,7 @@
         <v>30</v>
       </c>
       <c r="C10" t="str">
-        <f>"(:Specialty {name: '" &amp; B10 &amp;"', inPortuguese: '" &amp; A10 &amp;"'}),"</f>
+        <f t="shared" si="0"/>
         <v>(:Specialty {name: 'Cardiologist', inPortuguese: 'Cardiologista'}),</v>
       </c>
     </row>
@@ -1848,7 +3164,7 @@
         <v>31</v>
       </c>
       <c r="C11" t="str">
-        <f>"(:Specialty {name: '" &amp; B11 &amp;"', inPortuguese: '" &amp; A11 &amp;"'}),"</f>
+        <f t="shared" si="0"/>
         <v>(:Specialty {name: 'Nutritionist', inPortuguese: 'Nutrólogo'}),</v>
       </c>
     </row>
@@ -1860,7 +3176,7 @@
         <v>32</v>
       </c>
       <c r="C12" t="str">
-        <f>"(:Specialty {name: '" &amp; B12 &amp;"', inPortuguese: '" &amp; A12 &amp;"'}),"</f>
+        <f t="shared" si="0"/>
         <v>(:Specialty {name: 'Physiotherapist', inPortuguese: 'Fisioterapeuta'}),</v>
       </c>
     </row>
@@ -1872,7 +3188,7 @@
         <v>33</v>
       </c>
       <c r="C13" t="str">
-        <f>"(:Specialty {name: '" &amp; B13 &amp;"', inPortuguese: '" &amp; A13 &amp;"'}),"</f>
+        <f t="shared" si="0"/>
         <v>(:Specialty {name: 'Speech Therapist', inPortuguese: 'Fonoaudiólogo'}),</v>
       </c>
     </row>
@@ -1884,7 +3200,7 @@
         <v>34</v>
       </c>
       <c r="C14" t="str">
-        <f>"(:Specialty {name: '" &amp; B14 &amp;"', inPortuguese: '" &amp; A14 &amp;"'}),"</f>
+        <f t="shared" si="0"/>
         <v>(:Specialty {name: 'Psychologist', inPortuguese: 'Psicólogo'}),</v>
       </c>
     </row>
@@ -1896,7 +3212,7 @@
         <v>35</v>
       </c>
       <c r="C15" t="str">
-        <f>"(:Specialty {name: '" &amp; B15 &amp;"', inPortuguese: '" &amp; A15 &amp;"'}),"</f>
+        <f t="shared" si="0"/>
         <v>(:Specialty {name: 'Neurologist', inPortuguese: 'Neurologista'}),</v>
       </c>
     </row>
@@ -1908,7 +3224,7 @@
         <v>36</v>
       </c>
       <c r="C16" t="str">
-        <f>"(:Specialty {name: '" &amp; B16 &amp;"', inPortuguese: '" &amp; A16 &amp;"'}),"</f>
+        <f t="shared" si="0"/>
         <v>(:Specialty {name: 'Oncologist', inPortuguese: 'Oncologista'}),</v>
       </c>
     </row>
@@ -1920,7 +3236,7 @@
         <v>37</v>
       </c>
       <c r="C17" t="str">
-        <f>"(:Specialty {name: '" &amp; B17 &amp;"', inPortuguese: '" &amp; A17 &amp;"'}),"</f>
+        <f t="shared" si="0"/>
         <v>(:Specialty {name: 'Psychiatrist', inPortuguese: 'Psiquiatra'}),</v>
       </c>
     </row>
@@ -1932,7 +3248,7 @@
         <v>38</v>
       </c>
       <c r="C18" t="str">
-        <f>"(:Specialty {name: '" &amp; B18 &amp;"', inPortuguese: '" &amp; A18 &amp;"'}),"</f>
+        <f t="shared" si="0"/>
         <v>(:Specialty {name: 'Hebrew', inPortuguese: 'Hebiatra'}),</v>
       </c>
     </row>
@@ -1944,7 +3260,7 @@
         <v>39</v>
       </c>
       <c r="C19" t="str">
-        <f>"(:Specialty {name: '" &amp; B19 &amp;"', inPortuguese: '" &amp; A19 &amp;"'}),"</f>
+        <f t="shared" si="0"/>
         <v>(:Specialty {name: 'Nephrologist', inPortuguese: 'Nefrologista'}),</v>
       </c>
     </row>
@@ -1956,7 +3272,7 @@
         <v>40</v>
       </c>
       <c r="C20" t="str">
-        <f>"(:Specialty {name: '" &amp; B20 &amp;"', inPortuguese: '" &amp; A20 &amp;"'}),"</f>
+        <f t="shared" si="0"/>
         <v>(:Specialty {name: 'Urologist ', inPortuguese: 'Urologista'}),</v>
       </c>
     </row>
@@ -1966,1007 +3282,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16822055-6D7C-4562-869B-B3AD28812FB9}">
-  <dimension ref="A1:D81"/>
-  <sheetViews>
-    <sheetView zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="2" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D2" t="str">
-        <f>"(:Disease {name: '" &amp; B2 &amp;"', inPortuguese: '" &amp; A2 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Headache', inPortuguese: 'Cefaleia'}),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D3" t="str">
-        <f>"(:Disease {name: '" &amp; B3 &amp;"', inPortuguese: '" &amp; A3 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Migraine', inPortuguese: 'Enxaqueca'}),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D4" t="str">
-        <f>"(:Disease {name: '" &amp; B4 &amp;"', inPortuguese: '" &amp; A4 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Rhinitis', inPortuguese: 'Rinite'}),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D5" t="str">
-        <f>"(:Disease {name: '" &amp; B5 &amp;"', inPortuguese: '" &amp; A5 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Sinusitis', inPortuguese: 'Sinusite'}),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" t="s">
-        <v>92</v>
-      </c>
-      <c r="D6" t="str">
-        <f>"(:Disease {name: '" &amp; B6 &amp;"', inPortuguese: '" &amp; A6 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Asthma', inPortuguese: 'Asma'}),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" t="str">
-        <f>"(:Disease {name: '" &amp; B7 &amp;"', inPortuguese: '" &amp; A7 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Diabetes', inPortuguese: 'Diabetes'}),</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D8" t="str">
-        <f>"(:Disease {name: '" &amp; B8 &amp;"', inPortuguese: '" &amp; A8 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Hepatitis', inPortuguese: 'Hepatite'}),</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D9" t="str">
-        <f>"(:Disease {name: '" &amp; B9 &amp;"', inPortuguese: '" &amp; A9 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Depression', inPortuguese: 'Depressão'}),</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" t="str">
-        <f>"(:Disease {name: '" &amp; B10 &amp;"', inPortuguese: '" &amp; A10 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Anemia', inPortuguese: 'Anemia'}),</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" t="s">
-        <v>95</v>
-      </c>
-      <c r="D11" t="str">
-        <f>"(:Disease {name: '" &amp; B11 &amp;"', inPortuguese: '" &amp; A11 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Obesity', inPortuguese: 'Obesidade'}),</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" t="s">
-        <v>96</v>
-      </c>
-      <c r="D12" t="str">
-        <f>"(:Disease {name: '" &amp; B12 &amp;"', inPortuguese: '" &amp; A12 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Hypertension', inPortuguese: 'Hipertensão Arterial'}),</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" t="s">
-        <v>97</v>
-      </c>
-      <c r="D13" t="str">
-        <f>"(:Disease {name: '" &amp; B13 &amp;"', inPortuguese: '" &amp; A13 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Astigmatism', inPortuguese: 'Astigmatismo'}),</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" t="s">
-        <v>98</v>
-      </c>
-      <c r="D14" t="str">
-        <f>"(:Disease {name: '" &amp; B14 &amp;"', inPortuguese: '" &amp; A14 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Myopia', inPortuguese: 'Miopia'}),</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" t="s">
-        <v>99</v>
-      </c>
-      <c r="D15" t="str">
-        <f>"(:Disease {name: '" &amp; B15 &amp;"', inPortuguese: '" &amp; A15 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Hyperopia', inPortuguese: 'Hipermetropia'}),</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>55</v>
-      </c>
-      <c r="B16" t="s">
-        <v>100</v>
-      </c>
-      <c r="D16" t="str">
-        <f>"(:Disease {name: '" &amp; B16 &amp;"', inPortuguese: '" &amp; A16 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Blindness', inPortuguese: 'Cegueira'}),</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17" t="s">
-        <v>101</v>
-      </c>
-      <c r="D17" t="str">
-        <f>"(:Disease {name: '" &amp; B17 &amp;"', inPortuguese: '" &amp; A17 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Presbyopia', inPortuguese: 'Presbiopia'}),</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>57</v>
-      </c>
-      <c r="B18" t="s">
-        <v>102</v>
-      </c>
-      <c r="D18" t="str">
-        <f>"(:Disease {name: '" &amp; B18 &amp;"', inPortuguese: '" &amp; A18 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Cataract', inPortuguese: 'Catarata'}),</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>58</v>
-      </c>
-      <c r="B19" t="s">
-        <v>58</v>
-      </c>
-      <c r="D19" t="str">
-        <f>"(:Disease {name: '" &amp; B19 &amp;"', inPortuguese: '" &amp; A19 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Glaucoma', inPortuguese: 'Glaucoma'}),</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>59</v>
-      </c>
-      <c r="B20" t="s">
-        <v>103</v>
-      </c>
-      <c r="D20" t="str">
-        <f>"(:Disease {name: '" &amp; B20 &amp;"', inPortuguese: '" &amp; A20 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Conjunctivitis', inPortuguese: 'Conjuntivite'}),</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>142</v>
-      </c>
-      <c r="B21" t="s">
-        <v>149</v>
-      </c>
-      <c r="D21" t="str">
-        <f>"(:Disease {name: '" &amp; B21 &amp;"', inPortuguese: '" &amp; A21 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Diabetic Retinopathy', inPortuguese: 'Retinopatia Diabética'}),</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>60</v>
-      </c>
-      <c r="B22" t="s">
-        <v>104</v>
-      </c>
-      <c r="D22" t="str">
-        <f>"(:Disease {name: '" &amp; B22 &amp;"', inPortuguese: '" &amp; A22 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Deafness', inPortuguese: 'Surdez'}),</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23" t="s">
-        <v>105</v>
-      </c>
-      <c r="D23" t="str">
-        <f>"(:Disease {name: '" &amp; B23 &amp;"', inPortuguese: '" &amp; A23 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Otitis', inPortuguese: 'Otite'}),</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>62</v>
-      </c>
-      <c r="B24" t="s">
-        <v>106</v>
-      </c>
-      <c r="D24" t="str">
-        <f>"(:Disease {name: '" &amp; B24 &amp;"', inPortuguese: '" &amp; A24 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Labyrinthitis', inPortuguese: 'Labirintite'}),</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>63</v>
-      </c>
-      <c r="B25" t="s">
-        <v>63</v>
-      </c>
-      <c r="D25" t="str">
-        <f>"(:Disease {name: '" &amp; B25 &amp;"', inPortuguese: '" &amp; A25 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Tinnutus', inPortuguese: 'Tinnutus'}),</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>64</v>
-      </c>
-      <c r="B26" t="s">
-        <v>107</v>
-      </c>
-      <c r="D26" t="str">
-        <f>"(:Disease {name: '" &amp; B26 &amp;"', inPortuguese: '" &amp; A26 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Otosclerosis', inPortuguese: 'Otosclerose'}),</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>65</v>
-      </c>
-      <c r="B27" t="s">
-        <v>108</v>
-      </c>
-      <c r="D27" t="str">
-        <f>"(:Disease {name: '" &amp; B27 &amp;"', inPortuguese: '" &amp; A27 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Ototoxicity', inPortuguese: 'Ototoxicidade'}),</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>66</v>
-      </c>
-      <c r="B28" t="s">
-        <v>150</v>
-      </c>
-      <c r="D28" t="str">
-        <f>"(:Disease {name: '" &amp; B28 &amp;"', inPortuguese: '" &amp; A28 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Usher Syndrome', inPortuguese: 'Síndrome de Usher'}),</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>67</v>
-      </c>
-      <c r="B29" t="s">
-        <v>109</v>
-      </c>
-      <c r="D29" t="str">
-        <f>"(:Disease {name: '" &amp; B29 &amp;"', inPortuguese: '" &amp; A29 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Acoustic Neuroma', inPortuguese: 'Neuroma do Acústico'}),</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>68</v>
-      </c>
-      <c r="B30" t="s">
-        <v>151</v>
-      </c>
-      <c r="D30" t="str">
-        <f>"(:Disease {name: '" &amp; B30 &amp;"', inPortuguese: '" &amp; A30 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Meniere Disease', inPortuguese: 'Doença de Ménière'}),</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>69</v>
-      </c>
-      <c r="B31" t="s">
-        <v>110</v>
-      </c>
-      <c r="D31" t="str">
-        <f>"(:Disease {name: '" &amp; B31 &amp;"', inPortuguese: '" &amp; A31 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Stuttering', inPortuguese: 'Gagueira'}),</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>70</v>
-      </c>
-      <c r="B32" t="s">
-        <v>111</v>
-      </c>
-      <c r="D32" t="str">
-        <f>"(:Disease {name: '" &amp; B32 &amp;"', inPortuguese: '" &amp; A32 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Mute', inPortuguese: 'Mudez'}),</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>71</v>
-      </c>
-      <c r="B33" t="s">
-        <v>112</v>
-      </c>
-      <c r="D33" t="str">
-        <f>"(:Disease {name: '" &amp; B33 &amp;"', inPortuguese: '" &amp; A33 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Aphasia', inPortuguese: 'Afasia'}),</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>72</v>
-      </c>
-      <c r="B34" t="s">
-        <v>113</v>
-      </c>
-      <c r="D34" t="str">
-        <f>"(:Disease {name: '" &amp; B34 &amp;"', inPortuguese: '" &amp; A34 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Dysarthria', inPortuguese: 'Disartria'}),</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>73</v>
-      </c>
-      <c r="B35" t="s">
-        <v>114</v>
-      </c>
-      <c r="D35" t="str">
-        <f>"(:Disease {name: '" &amp; B35 &amp;"', inPortuguese: '" &amp; A35 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Dystonia', inPortuguese: 'Distonia'}),</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>74</v>
-      </c>
-      <c r="B36" t="s">
-        <v>115</v>
-      </c>
-      <c r="D36" t="str">
-        <f>"(:Disease {name: '" &amp; B36 &amp;"', inPortuguese: '" &amp; A36 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Cancer', inPortuguese: 'Câncer'}),</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>75</v>
-      </c>
-      <c r="B37" t="s">
-        <v>116</v>
-      </c>
-      <c r="D37" t="str">
-        <f>"(:Disease {name: '" &amp; B37 &amp;"', inPortuguese: '" &amp; A37 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Bipolarity', inPortuguese: 'Bipolaridade'}),</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>76</v>
-      </c>
-      <c r="B38" t="s">
-        <v>117</v>
-      </c>
-      <c r="D38" t="str">
-        <f>"(:Disease {name: '" &amp; B38 &amp;"', inPortuguese: '" &amp; A38 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Schizophrenia', inPortuguese: 'Esquizifrenia'}),</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>143</v>
-      </c>
-      <c r="B39" t="s">
-        <v>152</v>
-      </c>
-      <c r="D39" t="str">
-        <f>"(:Disease {name: '" &amp; B39 &amp;"', inPortuguese: '" &amp; A39 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Gastroesophageal Reflux', inPortuguese: 'Refluxo Gastroesofágico'}),</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>144</v>
-      </c>
-      <c r="B40" t="s">
-        <v>118</v>
-      </c>
-      <c r="D40" t="str">
-        <f>"(:Disease {name: '" &amp; B40 &amp;"', inPortuguese: '" &amp; A40 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Gallstone', inPortuguese: 'Cálculo Biliar'}),</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>77</v>
-      </c>
-      <c r="B41" t="s">
-        <v>119</v>
-      </c>
-      <c r="D41" t="str">
-        <f>"(:Disease {name: '" &amp; B41 &amp;"', inPortuguese: '" &amp; A41 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Pancreatitis', inPortuguese: 'Pancreatite'}),</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>145</v>
-      </c>
-      <c r="B42" t="s">
-        <v>153</v>
-      </c>
-      <c r="D42" t="str">
-        <f>"(:Disease {name: '" &amp; B42 &amp;"', inPortuguese: '" &amp; A42 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Abdominal Hernia', inPortuguese: 'Hérnia Abdominal'}),</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>146</v>
-      </c>
-      <c r="B43" t="s">
-        <v>154</v>
-      </c>
-      <c r="D43" t="str">
-        <f>"(:Disease {name: '" &amp; B43 &amp;"', inPortuguese: '" &amp; A43 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Hepatic Steatosis', inPortuguese: 'Esteatose Hepática'}),</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>78</v>
-      </c>
-      <c r="B44" t="s">
-        <v>120</v>
-      </c>
-      <c r="D44" t="str">
-        <f>"(:Disease {name: '" &amp; B44 &amp;"', inPortuguese: '" &amp; A44 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Gastritis', inPortuguese: 'Gastrite'}),</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>79</v>
-      </c>
-      <c r="B45" t="s">
-        <v>121</v>
-      </c>
-      <c r="D45" t="str">
-        <f>"(:Disease {name: '" &amp; B45 &amp;"', inPortuguese: '" &amp; A45 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Ulcer', inPortuguese: 'Úlcera'}),</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>147</v>
-      </c>
-      <c r="B46" t="s">
-        <v>122</v>
-      </c>
-      <c r="D46" t="str">
-        <f>"(:Disease {name: '" &amp; B46 &amp;"', inPortuguese: '" &amp; A46 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Constipation', inPortuguese: 'Prisão de Ventre'}),</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>80</v>
-      </c>
-      <c r="B47" t="s">
-        <v>123</v>
-      </c>
-      <c r="D47" t="str">
-        <f>"(:Disease {name: '" &amp; B47 &amp;"', inPortuguese: '" &amp; A47 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Appendicitis', inPortuguese: 'Apendicite'}),</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>81</v>
-      </c>
-      <c r="B48" t="s">
-        <v>124</v>
-      </c>
-      <c r="D48" t="str">
-        <f>"(:Disease {name: '" &amp; B48 &amp;"', inPortuguese: '" &amp; A48 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Diverticulitis', inPortuguese: 'Diverticulite'}),</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>82</v>
-      </c>
-      <c r="B49" t="s">
-        <v>125</v>
-      </c>
-      <c r="D49" t="str">
-        <f>"(:Disease {name: '" &amp; B49 &amp;"', inPortuguese: '" &amp; A49 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Heartburn', inPortuguese: 'Azia'}),</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>83</v>
-      </c>
-      <c r="B50" t="s">
-        <v>126</v>
-      </c>
-      <c r="D50" t="str">
-        <f>"(:Disease {name: '" &amp; B50 &amp;"', inPortuguese: '" &amp; A50 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Dyspepsia', inPortuguese: 'Dispepsia'}),</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>84</v>
-      </c>
-      <c r="B51" t="s">
-        <v>84</v>
-      </c>
-      <c r="D51" t="str">
-        <f>"(:Disease {name: '" &amp; B51 &amp;"', inPortuguese: '" &amp; A51 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Alzheimer', inPortuguese: 'Alzheimer'}),</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>148</v>
-      </c>
-      <c r="B52" t="s">
-        <v>148</v>
-      </c>
-      <c r="D52" t="str">
-        <f>"(:Disease {name: '" &amp; B52 &amp;"', inPortuguese: '" &amp; A52 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Aids', inPortuguese: 'Aids'}),</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>85</v>
-      </c>
-      <c r="B53" t="s">
-        <v>127</v>
-      </c>
-      <c r="D53" t="str">
-        <f>"(:Disease {name: '" &amp; B53 &amp;"', inPortuguese: '" &amp; A53 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Stroke', inPortuguese: 'Acidente Vascular Cerebral'}),</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>86</v>
-      </c>
-      <c r="B54" t="s">
-        <v>86</v>
-      </c>
-      <c r="D54" t="str">
-        <f>"(:Disease {name: '" &amp; B54 &amp;"', inPortuguese: '" &amp; A54 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Parkinson', inPortuguese: 'Parkinson'}),</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>87</v>
-      </c>
-      <c r="B55" t="s">
-        <v>155</v>
-      </c>
-      <c r="D55" t="str">
-        <f>"(:Disease {name: '" &amp; B55 &amp;"', inPortuguese: '" &amp; A55 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Polio', inPortuguese: 'Poliomielite'}),</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>128</v>
-      </c>
-      <c r="B56" t="s">
-        <v>134</v>
-      </c>
-      <c r="D56" t="str">
-        <f>"(:Disease {name: '" &amp; B56 &amp;"', inPortuguese: '" &amp; A56 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Dyslipidemia', inPortuguese: 'Dislipidemia'}),</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>172</v>
-      </c>
-      <c r="B57" t="s">
-        <v>135</v>
-      </c>
-      <c r="D57" t="str">
-        <f>"(:Disease {name: '" &amp; B57 &amp;"', inPortuguese: '" &amp; A57 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Ischemic Heart Disease', inPortuguese: 'Cardiopatia Isquêmica'}),</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>129</v>
-      </c>
-      <c r="B58" t="s">
-        <v>136</v>
-      </c>
-      <c r="D58" t="str">
-        <f>"(:Disease {name: '" &amp; B58 &amp;"', inPortuguese: '" &amp; A58 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Cardiac Insufficiency', inPortuguese: 'Insuficiência Cardíaca'}),</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>173</v>
-      </c>
-      <c r="B59" t="s">
-        <v>137</v>
-      </c>
-      <c r="D59" t="str">
-        <f>"(:Disease {name: '" &amp; B59 &amp;"', inPortuguese: '" &amp; A59 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Atrial Fibrillation', inPortuguese: 'Fibrilação Atrial'}),</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>130</v>
-      </c>
-      <c r="B60" t="s">
-        <v>138</v>
-      </c>
-      <c r="D60" t="str">
-        <f>"(:Disease {name: '" &amp; B60 &amp;"', inPortuguese: '" &amp; A60 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Stomatitis', inPortuguese: 'Estomatite'}),</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>131</v>
-      </c>
-      <c r="B61" t="s">
-        <v>139</v>
-      </c>
-      <c r="D61" t="str">
-        <f>"(:Disease {name: '" &amp; B61 &amp;"', inPortuguese: '" &amp; A61 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Crohn Disease', inPortuguese: 'Doença de Crohn'}),</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>132</v>
-      </c>
-      <c r="B62" t="s">
-        <v>140</v>
-      </c>
-      <c r="D62" t="str">
-        <f>"(:Disease {name: '" &amp; B62 &amp;"', inPortuguese: '" &amp; A62 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Irritable Bowel Syndrome', inPortuguese: 'Síndrome do Intestino Irritável'}),</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>174</v>
-      </c>
-      <c r="B63" t="s">
-        <v>141</v>
-      </c>
-      <c r="D63" t="str">
-        <f>"(:Disease {name: '" &amp; B63 &amp;"', inPortuguese: '" &amp; A63 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Ulcerative Colitis', inPortuguese: 'Retocolite Ulcerativa'}),</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>133</v>
-      </c>
-      <c r="B64" t="s">
-        <v>122</v>
-      </c>
-      <c r="D64" t="str">
-        <f>"(:Disease {name: '" &amp; B64 &amp;"', inPortuguese: '" &amp; A64 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Constipation', inPortuguese: 'Obstipação'}),</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>156</v>
-      </c>
-      <c r="B65" t="s">
-        <v>164</v>
-      </c>
-      <c r="D65" t="str">
-        <f>"(:Disease {name: '" &amp; B65 &amp;"', inPortuguese: '" &amp; A65 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Arthrosis', inPortuguese: 'Artrose'}),</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>157</v>
-      </c>
-      <c r="B66" t="s">
-        <v>165</v>
-      </c>
-      <c r="D66" t="str">
-        <f>"(:Disease {name: '" &amp; B66 &amp;"', inPortuguese: '" &amp; A66 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Flat Feet', inPortuguese: 'Pé Chato'}),</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>158</v>
-      </c>
-      <c r="B67" t="s">
-        <v>166</v>
-      </c>
-      <c r="D67" t="str">
-        <f>"(:Disease {name: '" &amp; B67 &amp;"', inPortuguese: '" &amp; A67 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Tendonitis', inPortuguese: 'Tendinite'}),</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>159</v>
-      </c>
-      <c r="B68" t="s">
-        <v>167</v>
-      </c>
-      <c r="D68" t="str">
-        <f>"(:Disease {name: '" &amp; B68 &amp;"', inPortuguese: '" &amp; A68 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Bursitis', inPortuguese: 'Bursite'}),</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>160</v>
-      </c>
-      <c r="B69" t="s">
-        <v>168</v>
-      </c>
-      <c r="D69" t="str">
-        <f>"(:Disease {name: '" &amp; B69 &amp;"', inPortuguese: '" &amp; A69 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Ligament Rupture', inPortuguese: 'Ruptura de Ligamento'}),</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>161</v>
-      </c>
-      <c r="B70" t="s">
-        <v>169</v>
-      </c>
-      <c r="D70" t="str">
-        <f>"(:Disease {name: '" &amp; B70 &amp;"', inPortuguese: '" &amp; A70 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Backache', inPortuguese: 'Lombalgia'}),</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>162</v>
-      </c>
-      <c r="B71" t="s">
-        <v>170</v>
-      </c>
-      <c r="D71" t="str">
-        <f>"(:Disease {name: '" &amp; B71 &amp;"', inPortuguese: '" &amp; A71 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Plantar Fasciitis', inPortuguese: 'Fascite Plantar'}),</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>163</v>
-      </c>
-      <c r="B72" t="s">
-        <v>171</v>
-      </c>
-      <c r="D72" t="str">
-        <f>"(:Disease {name: '" &amp; B72 &amp;"', inPortuguese: '" &amp; A72 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Osteoporosis', inPortuguese: 'Osteoporose'}),</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>175</v>
-      </c>
-      <c r="B73" t="s">
-        <v>180</v>
-      </c>
-      <c r="D73" t="str">
-        <f>"(:Disease {name: '" &amp; B73 &amp;"', inPortuguese: '" &amp; A73 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Pulmonary Emphysema', inPortuguese: 'Enfisema Pulmonar'}),</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>176</v>
-      </c>
-      <c r="B74" t="s">
-        <v>181</v>
-      </c>
-      <c r="D74" t="str">
-        <f>"(:Disease {name: '" &amp; B74 &amp;"', inPortuguese: '" &amp; A74 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Bronchitis', inPortuguese: 'Bronquite'}),</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>177</v>
-      </c>
-      <c r="B75" t="s">
-        <v>182</v>
-      </c>
-      <c r="D75" t="str">
-        <f>"(:Disease {name: '" &amp; B75 &amp;"', inPortuguese: '" &amp; A75 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Tuberculosis', inPortuguese: 'Tuberculose'}),</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>178</v>
-      </c>
-      <c r="B76" t="s">
-        <v>183</v>
-      </c>
-      <c r="D76" t="str">
-        <f>"(:Disease {name: '" &amp; B76 &amp;"', inPortuguese: '" &amp; A76 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Pharyngitis', inPortuguese: 'Faringite'}),</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>179</v>
-      </c>
-      <c r="B77" t="s">
-        <v>179</v>
-      </c>
-      <c r="D77" t="str">
-        <f>"(:Disease {name: '" &amp; B77 &amp;"', inPortuguese: '" &amp; A77 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Pneumonia', inPortuguese: 'Pneumonia'}),</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>185</v>
-      </c>
-      <c r="B78" t="s">
-        <v>189</v>
-      </c>
-      <c r="D78" t="str">
-        <f>"(:Disease {name: '" &amp; B78 &amp;"', inPortuguese: '" &amp; A78 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Allergic Urticaria', inPortuguese: 'Urticária Alérgica'}),</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>186</v>
-      </c>
-      <c r="B79" t="s">
-        <v>186</v>
-      </c>
-      <c r="D79" t="str">
-        <f>"(:Disease {name: '" &amp; B79 &amp;"', inPortuguese: '" &amp; A79 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Angioedema', inPortuguese: 'Angioedema'}),</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>187</v>
-      </c>
-      <c r="B80" t="s">
-        <v>190</v>
-      </c>
-      <c r="D80" t="str">
-        <f>"(:Disease {name: '" &amp; B80 &amp;"', inPortuguese: '" &amp; A80 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Contact Dermatitis', inPortuguese: 'Dermatite de Contato'}),</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>188</v>
-      </c>
-      <c r="B81" t="s">
-        <v>191</v>
-      </c>
-      <c r="D81" t="str">
-        <f>"(:Disease {name: '" &amp; B81 &amp;"', inPortuguese: '" &amp; A81 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Atopic Dermatitis', inPortuguese: 'Dermatite Atópica'}),</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:D74" xr:uid="{B2FAB676-2031-4EBE-8374-605422BD9A7E}"/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F94BB071-87F4-4604-9E70-F91A6E8FB04C}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48:D50"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3730,7 +4051,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FBDA324-BA52-4553-9EA4-1F1EB8000A70}">
   <dimension ref="A1:D50"/>
   <sheetViews>
@@ -4646,11 +4967,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A61B1D1-1498-4062-8FF1-43F1DDC4F5BE}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -5066,103 +5387,103 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F21" t="str">
-        <f>"MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '" &amp; A2 &amp; "' AND d.vaccine = '" &amp; A2 &amp; "' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);"</f>
+        <f t="shared" ref="F21:F37" si="2">"MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '" &amp; A2 &amp; "' AND d.vaccine = '" &amp; A2 &amp; "' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);"</f>
         <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'BCG ID' AND d.vaccine = 'BCG ID' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F22" t="str">
-        <f>"MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '" &amp; A3 &amp; "' AND d.vaccine = '" &amp; A3 &amp; "' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);"</f>
+        <f t="shared" si="2"/>
         <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Hepatite B' AND d.vaccine = 'Hepatite B' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F23" t="str">
-        <f>"MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '" &amp; A4 &amp; "' AND d.vaccine = '" &amp; A4 &amp; "' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);"</f>
+        <f t="shared" si="2"/>
         <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'DTPw' AND d.vaccine = 'DTPw' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F24" t="str">
-        <f>"MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '" &amp; A5 &amp; "' AND d.vaccine = '" &amp; A5 &amp; "' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);"</f>
+        <f t="shared" si="2"/>
         <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'H Influenzae' AND d.vaccine = 'H Influenzae' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F25" t="str">
-        <f>"MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '" &amp; A6 &amp; "' AND d.vaccine = '" &amp; A6 &amp; "' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);"</f>
+        <f t="shared" si="2"/>
         <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Pólio VIP' AND d.vaccine = 'Pólio VIP' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F26" t="str">
-        <f>"MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '" &amp; A7 &amp; "' AND d.vaccine = '" &amp; A7 &amp; "' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);"</f>
+        <f t="shared" si="2"/>
         <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Pólio VOP' AND d.vaccine = 'Pólio VOP' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F27" t="str">
-        <f>"MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '" &amp; A8 &amp; "' AND d.vaccine = '" &amp; A8 &amp; "' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);"</f>
+        <f t="shared" si="2"/>
         <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Rotavírus' AND d.vaccine = 'Rotavírus' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F28" t="str">
-        <f>"MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '" &amp; A9 &amp; "' AND d.vaccine = '" &amp; A9 &amp; "' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);"</f>
+        <f t="shared" si="2"/>
         <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'VPC10' AND d.vaccine = 'VPC10' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F29" t="str">
-        <f>"MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '" &amp; A10 &amp; "' AND d.vaccine = '" &amp; A10 &amp; "' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);"</f>
+        <f t="shared" si="2"/>
         <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'ACWY/C' AND d.vaccine = 'ACWY/C' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F30" t="str">
-        <f>"MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '" &amp; A11 &amp; "' AND d.vaccine = '" &amp; A11 &amp; "' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);"</f>
+        <f t="shared" si="2"/>
         <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Meningocócica B' AND d.vaccine = 'Meningocócica B' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F31" t="str">
-        <f>"MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '" &amp; A12 &amp; "' AND d.vaccine = '" &amp; A12 &amp; "' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);"</f>
+        <f t="shared" si="2"/>
         <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '3V' AND d.vaccine = '3V' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F32" t="str">
-        <f>"MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '" &amp; A13 &amp; "' AND d.vaccine = '" &amp; A13 &amp; "' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);"</f>
+        <f t="shared" si="2"/>
         <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Febre amarela' AND d.vaccine = 'Febre amarela' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
       </c>
     </row>
     <row r="33" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F33" t="str">
-        <f>"MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '" &amp; A14 &amp; "' AND d.vaccine = '" &amp; A14 &amp; "' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);"</f>
+        <f t="shared" si="2"/>
         <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Hepatite A' AND d.vaccine = 'Hepatite A' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
       </c>
     </row>
     <row r="34" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F34" t="str">
-        <f>"MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '" &amp; A15 &amp; "' AND d.vaccine = '" &amp; A15 &amp; "' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);"</f>
+        <f t="shared" si="2"/>
         <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'BCG' AND d.vaccine = 'BCG' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
       </c>
     </row>
     <row r="35" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F35" t="str">
-        <f>"MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '" &amp; A16 &amp; "' AND d.vaccine = '" &amp; A16 &amp; "' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);"</f>
+        <f t="shared" si="2"/>
         <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Varicela' AND d.vaccine = 'Varicela' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
       </c>
     </row>
     <row r="36" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F36" t="str">
-        <f>"MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '" &amp; A17 &amp; "' AND d.vaccine = '" &amp; A17 &amp; "' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);"</f>
+        <f t="shared" si="2"/>
         <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'HPV4' AND d.vaccine = 'HPV4' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
       </c>
     </row>
     <row r="37" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F37" t="str">
-        <f>"MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '" &amp; A18 &amp; "' AND d.vaccine = '" &amp; A18 &amp; "' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);"</f>
+        <f t="shared" si="2"/>
         <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'DTPa' AND d.vaccine = 'DTPa' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
       </c>
     </row>
@@ -5171,7 +5492,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{391AE3A0-7DB7-4C1A-B882-6DBA4383A0D7}">
   <dimension ref="A1:O55"/>
   <sheetViews>
@@ -6785,4 +7106,40 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF7AE525-CAA1-4E99-A7E7-A745DD507DF7}">
+  <sheetPr>
+    <tabColor rgb="FF002060"/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="3" max="3" width="88.88671875" customWidth="1"/>
+    <col min="4" max="4" width="53.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="C2" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>371</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
refactor: :recycle: refactoring EMR & Vaccination tasks
</commit_message>
<xml_diff>
--- a/poc.xlsx
+++ b/poc.xlsx
@@ -8,20 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\renatospaka\dev\heykid\draft\poc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC5408D-7F1A-4E6D-8C46-B722A4543D77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2FAF7DE-B35F-4274-A185-FDAA53B52F2D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="complication" sheetId="1" r:id="rId1"/>
     <sheet name="disease" sheetId="3" r:id="rId2"/>
-    <sheet name="measurement" sheetId="8" r:id="rId3"/>
-    <sheet name="specialty" sheetId="2" r:id="rId4"/>
-    <sheet name="allergy" sheetId="4" r:id="rId5"/>
-    <sheet name="intolerance" sheetId="5" r:id="rId6"/>
+    <sheet name="allergy" sheetId="4" r:id="rId3"/>
+    <sheet name="intolerance" sheetId="5" r:id="rId4"/>
+    <sheet name="measurement" sheetId="8" r:id="rId5"/>
+    <sheet name="specialty" sheetId="2" r:id="rId6"/>
     <sheet name="vaccine" sheetId="6" r:id="rId7"/>
     <sheet name="vaccine dose" sheetId="7" r:id="rId8"/>
-    <sheet name="Date Range" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">disease!$A$1:$D$74</definedName>
@@ -46,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="370">
   <si>
     <t>Tipos</t>
   </si>
@@ -1156,88 +1155,6 @@
   </si>
   <si>
     <t>Query Relationship</t>
-  </si>
-  <si>
-    <t>MERGE (r:TimeTreeRoot)
-WITH r, range(2010, 2020) AS years, range(1,12) as months
-FOREACH(year IN years |
-  MERGE (y:Year {value: year})
-  MERGE (r)-[:CHILD]-&gt;(y)
-  FOREACH(month IN months |
-    CREATE (m:Month {value: month})
-    MERGE (y)-[:CHILD]-&gt;(m)
-    FOREACH(day IN (CASE
-                      WHEN month IN [1,3,5,7,8,10,12] THEN range(1,31)
-                      WHEN month = 2 THEN
-                        CASE
-                          WHEN year % 4 &lt;&gt; 0 THEN range(1,28)
-                          WHEN year % 100 &lt;&gt; 0 THEN range(1,29)
-                          WHEN year % 400 &lt;&gt; 0 THEN range(1,29)
-                          ELSE range(1,28)
-                        END
-                      ELSE range(1,30)
-                    END) |
-      CREATE (d:Day {value: day})
-      MERGE (m)-[:CHILD]-&gt;(d))))
-WITH *
-//Create years linked list
-MATCH (root:TimeTreeRoot)--&gt;(year:Year)
-WITH root, year ORDER BY year.value
-WITH root, collect(year) as years
-WITH root, years, years[0] AS first, years[size(years)-1] AS last
-MERGE (root)-[:FIRST]-&gt;(first)
-MERGE (root)-[:LAST]-&gt;(last)
-FOREACH(i in RANGE(0, size(years)-2) |
-    FOREACH(year1 in [years[i]] |
-        FOREACH(year2 in [years[i+1]] |
-            MERGE (year1)-[:NEXT]-&gt;(year2))))
-WITH *
-//Create months linked list
-MATCH (year:Year)
-WITH collect(year) as years
-UNWIND years AS year
-	MATCH (year)--(first:Month {value: 1}), (year)--(last:Month {value: 12})
-	MERGE (year)-[:FIRST]-&gt;(first)
-	MERGE (year)-[:LAST]-&gt;(last)
-WITH *
-MATCH (year:Year)-[:CHILD]-&gt;(month:Month)
-WITH year, month
-ORDER BY year.value, month.value
-WITH collect(month) as months
-FOREACH(i in RANGE(0, size(months)-2) |
-    FOREACH(month1 in [months[i]] |
-        FOREACH(month2 in [months[i+1]] |
-            MERGE (month1)-[:NEXT]-&gt;(month2))))
-WITH *
-//Create days linked list
-MATCH (month:Month)
-WITH collect(month) as months
-UNWIND months AS month
-	MATCH (month)-[:CHILD]-&gt;(day:Day)
-	WITH month, collect(day) AS days
-	WITH month, days[0] AS first, days[size(days)-1] AS last
-	MERGE (month)-[:FIRST]-&gt;(first)
-	MERGE (month)-[:LAST]-&gt;(last)
-WITH *
-MATCH (year:Year)-[:CHILD]-&gt;(month:Month)-[:CHILD]-&gt;(day:Day)
-WITH year,month,day
-ORDER BY year.value, month.value, day.value
-WITH collect(day) as days
-FOREACH(i in RANGE(0, size(days)-2) |
-    FOREACH(day1 in [days[i]] |
-        FOREACH(day2 in [days[i+1]] |
-            MERGE (day1)-[:NEXT]-&gt;(day2))))
-;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MATCH (year:Year)-[:CHILD]-&gt;(month:Month)-[:CHILD]-&gt;(day:Day)
-WHERE year.value &gt;=2018
-RETURN year.value AS Year, month.value AS Month, day.value AS Day
-ORDER BY Year, Month, Day
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Creates a Date structure to allow connecting date nodes to other nodes instead of pure properties </t>
   </si>
 </sst>
 </file>
@@ -1273,14 +1190,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1565,7 +1479,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C2" sqref="C2:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1593,8 +1507,8 @@
         <v>308</v>
       </c>
       <c r="C2" t="str">
-        <f t="shared" ref="C2:C18" si="0">"(:Complication {name: '" &amp; B2 &amp;"', inPortuguese: '" &amp; A2 &amp;"'}),"</f>
-        <v>(:Complication {name: 'Cry', inPortuguese: 'Choro'}),</v>
+        <f>"(:Complication {uuid: apoc.create.uuid(), name: '" &amp; B2 &amp;"', inPortuguese: '" &amp; A2 &amp;"'}),"</f>
+        <v>(:Complication {uuid: apoc.create.uuid(), name: 'Cry', inPortuguese: 'Choro'}),</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1605,8 +1519,8 @@
         <v>309</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Complication {name: 'Fever', inPortuguese: 'Febre'}),</v>
+        <f t="shared" ref="C3:C18" si="0">"(:Complication {uuid: apoc.create.uuid(), name: '" &amp; B3 &amp;"', inPortuguese: '" &amp; A3 &amp;"'}),"</f>
+        <v>(:Complication {uuid: apoc.create.uuid(), name: 'Fever', inPortuguese: 'Febre'}),</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1618,7 +1532,7 @@
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
-        <v>(:Complication {name: 'Vomiting', inPortuguese: 'Vômito'}),</v>
+        <v>(:Complication {uuid: apoc.create.uuid(), name: 'Vomiting', inPortuguese: 'Vômito'}),</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1630,7 +1544,7 @@
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
-        <v>(:Complication {name: 'Diarrhea', inPortuguese: 'Diarreia'}),</v>
+        <v>(:Complication {uuid: apoc.create.uuid(), name: 'Diarrhea', inPortuguese: 'Diarreia'}),</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1642,7 +1556,7 @@
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
-        <v>(:Complication {name: 'Coryza', inPortuguese: 'Coriza'}),</v>
+        <v>(:Complication {uuid: apoc.create.uuid(), name: 'Coryza', inPortuguese: 'Coriza'}),</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1654,7 +1568,7 @@
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
-        <v>(:Complication {name: 'Stress', inPortuguese: 'Estresse'}),</v>
+        <v>(:Complication {uuid: apoc.create.uuid(), name: 'Stress', inPortuguese: 'Estresse'}),</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1666,7 +1580,7 @@
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
-        <v>(:Complication {name: 'Cough', inPortuguese: 'Tosse'}),</v>
+        <v>(:Complication {uuid: apoc.create.uuid(), name: 'Cough', inPortuguese: 'Tosse'}),</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1678,7 +1592,7 @@
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
-        <v>(:Complication {name: 'Sneeze', inPortuguese: 'Espirro'}),</v>
+        <v>(:Complication {uuid: apoc.create.uuid(), name: 'Sneeze', inPortuguese: 'Espirro'}),</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1690,7 +1604,7 @@
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
-        <v>(:Complication {name: 'Nausea', inPortuguese: 'Náusea'}),</v>
+        <v>(:Complication {uuid: apoc.create.uuid(), name: 'Nausea', inPortuguese: 'Náusea'}),</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1702,7 +1616,7 @@
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
-        <v>(:Complication {name: 'Fall', inPortuguese: 'Queda'}),</v>
+        <v>(:Complication {uuid: apoc.create.uuid(), name: 'Fall', inPortuguese: 'Queda'}),</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1714,7 +1628,7 @@
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
-        <v>(:Complication {name: 'Vertigo', inPortuguese: 'Vertigem'}),</v>
+        <v>(:Complication {uuid: apoc.create.uuid(), name: 'Vertigo', inPortuguese: 'Vertigem'}),</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1726,7 +1640,7 @@
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
-        <v>(:Complication {name: 'Twist', inPortuguese: 'Torção'}),</v>
+        <v>(:Complication {uuid: apoc.create.uuid(), name: 'Twist', inPortuguese: 'Torção'}),</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -1738,7 +1652,7 @@
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
-        <v>(:Complication {name: 'Cut', inPortuguese: 'Corte'}),</v>
+        <v>(:Complication {uuid: apoc.create.uuid(), name: 'Cut', inPortuguese: 'Corte'}),</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -1750,7 +1664,7 @@
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
-        <v>(:Complication {name: 'Shock', inPortuguese: 'Choque'}),</v>
+        <v>(:Complication {uuid: apoc.create.uuid(), name: 'Shock', inPortuguese: 'Choque'}),</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -1762,7 +1676,7 @@
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
-        <v>(:Complication {name: 'Weakness', inPortuguese: 'Fraqueza'}),</v>
+        <v>(:Complication {uuid: apoc.create.uuid(), name: 'Weakness', inPortuguese: 'Fraqueza'}),</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -1774,7 +1688,7 @@
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
-        <v>(:Complication {name: 'Ingestion', inPortuguese: 'Ingestão'}),</v>
+        <v>(:Complication {uuid: apoc.create.uuid(), name: 'Ingestion', inPortuguese: 'Ingestão'}),</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -1786,7 +1700,7 @@
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
-        <v>(:Complication {name: 'Ache', inPortuguese: 'Dor'}),</v>
+        <v>(:Complication {uuid: apoc.create.uuid(), name: 'Ache', inPortuguese: 'Dor'}),</v>
       </c>
     </row>
   </sheetData>
@@ -1798,8 +1712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16822055-6D7C-4562-869B-B3AD28812FB9}">
   <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1831,8 +1745,8 @@
         <v>88</v>
       </c>
       <c r="D2" t="str">
-        <f t="shared" ref="D2:D33" si="0">"(:Disease {name: '" &amp; B2 &amp;"', inPortuguese: '" &amp; A2 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Headache', inPortuguese: 'Cefaleia'}),</v>
+        <f>"(:Disease {uuid: apoc.create.uuid(), name: '" &amp; B2 &amp;"', inPortuguese: '" &amp; A2 &amp;"'}),"</f>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Headache', inPortuguese: 'Cefaleia'}),</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1843,8 +1757,8 @@
         <v>89</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Disease {name: 'Migraine', inPortuguese: 'Enxaqueca'}),</v>
+        <f t="shared" ref="D3:D66" si="0">"(:Disease {uuid: apoc.create.uuid(), name: '" &amp; B3 &amp;"', inPortuguese: '" &amp; A3 &amp;"'}),"</f>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Migraine', inPortuguese: 'Enxaqueca'}),</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1856,7 +1770,7 @@
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
-        <v>(:Disease {name: 'Rhinitis', inPortuguese: 'Rinite'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Rhinitis', inPortuguese: 'Rinite'}),</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1868,7 +1782,7 @@
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
-        <v>(:Disease {name: 'Sinusitis', inPortuguese: 'Sinusite'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Sinusitis', inPortuguese: 'Sinusite'}),</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1880,7 +1794,7 @@
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
-        <v>(:Disease {name: 'Asthma', inPortuguese: 'Asma'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Asthma', inPortuguese: 'Asma'}),</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1892,7 +1806,7 @@
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>(:Disease {name: 'Diabetes', inPortuguese: 'Diabetes'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Diabetes', inPortuguese: 'Diabetes'}),</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1904,7 +1818,7 @@
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>(:Disease {name: 'Hepatitis', inPortuguese: 'Hepatite'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Hepatitis', inPortuguese: 'Hepatite'}),</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1916,7 +1830,7 @@
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>(:Disease {name: 'Depression', inPortuguese: 'Depressão'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Depression', inPortuguese: 'Depressão'}),</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1928,7 +1842,7 @@
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>(:Disease {name: 'Anemia', inPortuguese: 'Anemia'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Anemia', inPortuguese: 'Anemia'}),</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1940,7 +1854,7 @@
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v>(:Disease {name: 'Obesity', inPortuguese: 'Obesidade'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Obesity', inPortuguese: 'Obesidade'}),</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1952,7 +1866,7 @@
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>(:Disease {name: 'Hypertension', inPortuguese: 'Hipertensão Arterial'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Hypertension', inPortuguese: 'Hipertensão Arterial'}),</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1964,7 +1878,7 @@
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>(:Disease {name: 'Astigmatism', inPortuguese: 'Astigmatismo'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Astigmatism', inPortuguese: 'Astigmatismo'}),</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1976,7 +1890,7 @@
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v>(:Disease {name: 'Myopia', inPortuguese: 'Miopia'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Myopia', inPortuguese: 'Miopia'}),</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -1988,7 +1902,7 @@
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v>(:Disease {name: 'Hyperopia', inPortuguese: 'Hipermetropia'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Hyperopia', inPortuguese: 'Hipermetropia'}),</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -2000,7 +1914,7 @@
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v>(:Disease {name: 'Blindness', inPortuguese: 'Cegueira'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Blindness', inPortuguese: 'Cegueira'}),</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -2012,7 +1926,7 @@
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
-        <v>(:Disease {name: 'Presbyopia', inPortuguese: 'Presbiopia'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Presbyopia', inPortuguese: 'Presbiopia'}),</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -2024,7 +1938,7 @@
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
-        <v>(:Disease {name: 'Cataract', inPortuguese: 'Catarata'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Cataract', inPortuguese: 'Catarata'}),</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -2036,7 +1950,7 @@
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
-        <v>(:Disease {name: 'Glaucoma', inPortuguese: 'Glaucoma'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Glaucoma', inPortuguese: 'Glaucoma'}),</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -2048,7 +1962,7 @@
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
-        <v>(:Disease {name: 'Conjunctivitis', inPortuguese: 'Conjuntivite'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Conjunctivitis', inPortuguese: 'Conjuntivite'}),</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -2060,7 +1974,7 @@
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
-        <v>(:Disease {name: 'Diabetic Retinopathy', inPortuguese: 'Retinopatia Diabética'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Diabetic Retinopathy', inPortuguese: 'Retinopatia Diabética'}),</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -2072,7 +1986,7 @@
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
-        <v>(:Disease {name: 'Deafness', inPortuguese: 'Surdez'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Deafness', inPortuguese: 'Surdez'}),</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -2084,7 +1998,7 @@
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
-        <v>(:Disease {name: 'Otitis', inPortuguese: 'Otite'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Otitis', inPortuguese: 'Otite'}),</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -2096,7 +2010,7 @@
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
-        <v>(:Disease {name: 'Labyrinthitis', inPortuguese: 'Labirintite'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Labyrinthitis', inPortuguese: 'Labirintite'}),</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -2108,7 +2022,7 @@
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
-        <v>(:Disease {name: 'Tinnutus', inPortuguese: 'Tinnutus'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Tinnutus', inPortuguese: 'Tinnutus'}),</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -2120,7 +2034,7 @@
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
-        <v>(:Disease {name: 'Otosclerosis', inPortuguese: 'Otosclerose'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Otosclerosis', inPortuguese: 'Otosclerose'}),</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -2132,7 +2046,7 @@
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
-        <v>(:Disease {name: 'Ototoxicity', inPortuguese: 'Ototoxicidade'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Ototoxicity', inPortuguese: 'Ototoxicidade'}),</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -2144,7 +2058,7 @@
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
-        <v>(:Disease {name: 'Usher Syndrome', inPortuguese: 'Síndrome de Usher'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Usher Syndrome', inPortuguese: 'Síndrome de Usher'}),</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -2156,7 +2070,7 @@
       </c>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
-        <v>(:Disease {name: 'Acoustic Neuroma', inPortuguese: 'Neuroma do Acústico'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Acoustic Neuroma', inPortuguese: 'Neuroma do Acústico'}),</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -2168,7 +2082,7 @@
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
-        <v>(:Disease {name: 'Meniere Disease', inPortuguese: 'Doença de Ménière'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Meniere Disease', inPortuguese: 'Doença de Ménière'}),</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -2180,7 +2094,7 @@
       </c>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
-        <v>(:Disease {name: 'Stuttering', inPortuguese: 'Gagueira'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Stuttering', inPortuguese: 'Gagueira'}),</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -2192,7 +2106,7 @@
       </c>
       <c r="D32" t="str">
         <f t="shared" si="0"/>
-        <v>(:Disease {name: 'Mute', inPortuguese: 'Mudez'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Mute', inPortuguese: 'Mudez'}),</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -2204,7 +2118,7 @@
       </c>
       <c r="D33" t="str">
         <f t="shared" si="0"/>
-        <v>(:Disease {name: 'Aphasia', inPortuguese: 'Afasia'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Aphasia', inPortuguese: 'Afasia'}),</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -2215,8 +2129,8 @@
         <v>113</v>
       </c>
       <c r="D34" t="str">
-        <f t="shared" ref="D34:D65" si="1">"(:Disease {name: '" &amp; B34 &amp;"', inPortuguese: '" &amp; A34 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Dysarthria', inPortuguese: 'Disartria'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Dysarthria', inPortuguese: 'Disartria'}),</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -2227,8 +2141,8 @@
         <v>114</v>
       </c>
       <c r="D35" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Disease {name: 'Dystonia', inPortuguese: 'Distonia'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Dystonia', inPortuguese: 'Distonia'}),</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -2239,8 +2153,8 @@
         <v>115</v>
       </c>
       <c r="D36" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Disease {name: 'Cancer', inPortuguese: 'Câncer'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Cancer', inPortuguese: 'Câncer'}),</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -2251,8 +2165,8 @@
         <v>116</v>
       </c>
       <c r="D37" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Disease {name: 'Bipolarity', inPortuguese: 'Bipolaridade'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Bipolarity', inPortuguese: 'Bipolaridade'}),</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -2263,8 +2177,8 @@
         <v>117</v>
       </c>
       <c r="D38" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Disease {name: 'Schizophrenia', inPortuguese: 'Esquizifrenia'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Schizophrenia', inPortuguese: 'Esquizifrenia'}),</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -2275,8 +2189,8 @@
         <v>152</v>
       </c>
       <c r="D39" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Disease {name: 'Gastroesophageal Reflux', inPortuguese: 'Refluxo Gastroesofágico'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Gastroesophageal Reflux', inPortuguese: 'Refluxo Gastroesofágico'}),</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -2287,8 +2201,8 @@
         <v>118</v>
       </c>
       <c r="D40" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Disease {name: 'Gallstone', inPortuguese: 'Cálculo Biliar'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Gallstone', inPortuguese: 'Cálculo Biliar'}),</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -2299,8 +2213,8 @@
         <v>119</v>
       </c>
       <c r="D41" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Disease {name: 'Pancreatitis', inPortuguese: 'Pancreatite'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Pancreatitis', inPortuguese: 'Pancreatite'}),</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -2311,8 +2225,8 @@
         <v>153</v>
       </c>
       <c r="D42" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Disease {name: 'Abdominal Hernia', inPortuguese: 'Hérnia Abdominal'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Abdominal Hernia', inPortuguese: 'Hérnia Abdominal'}),</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -2323,8 +2237,8 @@
         <v>154</v>
       </c>
       <c r="D43" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Disease {name: 'Hepatic Steatosis', inPortuguese: 'Esteatose Hepática'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Hepatic Steatosis', inPortuguese: 'Esteatose Hepática'}),</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -2335,8 +2249,8 @@
         <v>120</v>
       </c>
       <c r="D44" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Disease {name: 'Gastritis', inPortuguese: 'Gastrite'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Gastritis', inPortuguese: 'Gastrite'}),</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -2347,8 +2261,8 @@
         <v>121</v>
       </c>
       <c r="D45" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Disease {name: 'Ulcer', inPortuguese: 'Úlcera'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Ulcer', inPortuguese: 'Úlcera'}),</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -2359,8 +2273,8 @@
         <v>122</v>
       </c>
       <c r="D46" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Disease {name: 'Constipation', inPortuguese: 'Prisão de Ventre'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Constipation', inPortuguese: 'Prisão de Ventre'}),</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -2371,8 +2285,8 @@
         <v>123</v>
       </c>
       <c r="D47" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Disease {name: 'Appendicitis', inPortuguese: 'Apendicite'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Appendicitis', inPortuguese: 'Apendicite'}),</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -2383,8 +2297,8 @@
         <v>124</v>
       </c>
       <c r="D48" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Disease {name: 'Diverticulitis', inPortuguese: 'Diverticulite'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Diverticulitis', inPortuguese: 'Diverticulite'}),</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -2395,8 +2309,8 @@
         <v>125</v>
       </c>
       <c r="D49" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Disease {name: 'Heartburn', inPortuguese: 'Azia'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Heartburn', inPortuguese: 'Azia'}),</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -2407,8 +2321,8 @@
         <v>126</v>
       </c>
       <c r="D50" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Disease {name: 'Dyspepsia', inPortuguese: 'Dispepsia'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Dyspepsia', inPortuguese: 'Dispepsia'}),</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -2419,8 +2333,8 @@
         <v>84</v>
       </c>
       <c r="D51" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Disease {name: 'Alzheimer', inPortuguese: 'Alzheimer'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Alzheimer', inPortuguese: 'Alzheimer'}),</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -2431,8 +2345,8 @@
         <v>148</v>
       </c>
       <c r="D52" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Disease {name: 'Aids', inPortuguese: 'Aids'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Aids', inPortuguese: 'Aids'}),</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -2443,8 +2357,8 @@
         <v>127</v>
       </c>
       <c r="D53" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Disease {name: 'Stroke', inPortuguese: 'Acidente Vascular Cerebral'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Stroke', inPortuguese: 'Acidente Vascular Cerebral'}),</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -2455,8 +2369,8 @@
         <v>86</v>
       </c>
       <c r="D54" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Disease {name: 'Parkinson', inPortuguese: 'Parkinson'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Parkinson', inPortuguese: 'Parkinson'}),</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -2467,8 +2381,8 @@
         <v>155</v>
       </c>
       <c r="D55" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Disease {name: 'Polio', inPortuguese: 'Poliomielite'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Polio', inPortuguese: 'Poliomielite'}),</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -2479,8 +2393,8 @@
         <v>134</v>
       </c>
       <c r="D56" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Disease {name: 'Dyslipidemia', inPortuguese: 'Dislipidemia'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Dyslipidemia', inPortuguese: 'Dislipidemia'}),</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -2491,8 +2405,8 @@
         <v>135</v>
       </c>
       <c r="D57" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Disease {name: 'Ischemic Heart Disease', inPortuguese: 'Cardiopatia Isquêmica'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Ischemic Heart Disease', inPortuguese: 'Cardiopatia Isquêmica'}),</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -2503,8 +2417,8 @@
         <v>136</v>
       </c>
       <c r="D58" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Disease {name: 'Cardiac Insufficiency', inPortuguese: 'Insuficiência Cardíaca'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Cardiac Insufficiency', inPortuguese: 'Insuficiência Cardíaca'}),</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -2515,8 +2429,8 @@
         <v>137</v>
       </c>
       <c r="D59" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Disease {name: 'Atrial Fibrillation', inPortuguese: 'Fibrilação Atrial'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Atrial Fibrillation', inPortuguese: 'Fibrilação Atrial'}),</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -2527,8 +2441,8 @@
         <v>138</v>
       </c>
       <c r="D60" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Disease {name: 'Stomatitis', inPortuguese: 'Estomatite'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Stomatitis', inPortuguese: 'Estomatite'}),</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -2539,8 +2453,8 @@
         <v>139</v>
       </c>
       <c r="D61" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Disease {name: 'Crohn Disease', inPortuguese: 'Doença de Crohn'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Crohn Disease', inPortuguese: 'Doença de Crohn'}),</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -2551,8 +2465,8 @@
         <v>140</v>
       </c>
       <c r="D62" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Disease {name: 'Irritable Bowel Syndrome', inPortuguese: 'Síndrome do Intestino Irritável'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Irritable Bowel Syndrome', inPortuguese: 'Síndrome do Intestino Irritável'}),</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -2563,8 +2477,8 @@
         <v>141</v>
       </c>
       <c r="D63" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Disease {name: 'Ulcerative Colitis', inPortuguese: 'Retocolite Ulcerativa'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Ulcerative Colitis', inPortuguese: 'Retocolite Ulcerativa'}),</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -2575,8 +2489,8 @@
         <v>122</v>
       </c>
       <c r="D64" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Disease {name: 'Constipation', inPortuguese: 'Obstipação'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Constipation', inPortuguese: 'Obstipação'}),</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -2587,8 +2501,8 @@
         <v>164</v>
       </c>
       <c r="D65" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Disease {name: 'Arthrosis', inPortuguese: 'Artrose'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Arthrosis', inPortuguese: 'Artrose'}),</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -2599,8 +2513,8 @@
         <v>165</v>
       </c>
       <c r="D66" t="str">
-        <f t="shared" ref="D66:D81" si="2">"(:Disease {name: '" &amp; B66 &amp;"', inPortuguese: '" &amp; A66 &amp;"'}),"</f>
-        <v>(:Disease {name: 'Flat Feet', inPortuguese: 'Pé Chato'}),</v>
+        <f t="shared" si="0"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Flat Feet', inPortuguese: 'Pé Chato'}),</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -2611,8 +2525,8 @@
         <v>166</v>
       </c>
       <c r="D67" t="str">
-        <f t="shared" si="2"/>
-        <v>(:Disease {name: 'Tendonitis', inPortuguese: 'Tendinite'}),</v>
+        <f t="shared" ref="D67:D81" si="1">"(:Disease {uuid: apoc.create.uuid(), name: '" &amp; B67 &amp;"', inPortuguese: '" &amp; A67 &amp;"'}),"</f>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Tendonitis', inPortuguese: 'Tendinite'}),</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -2623,8 +2537,8 @@
         <v>167</v>
       </c>
       <c r="D68" t="str">
-        <f t="shared" si="2"/>
-        <v>(:Disease {name: 'Bursitis', inPortuguese: 'Bursite'}),</v>
+        <f t="shared" si="1"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Bursitis', inPortuguese: 'Bursite'}),</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -2635,8 +2549,8 @@
         <v>168</v>
       </c>
       <c r="D69" t="str">
-        <f t="shared" si="2"/>
-        <v>(:Disease {name: 'Ligament Rupture', inPortuguese: 'Ruptura de Ligamento'}),</v>
+        <f t="shared" si="1"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Ligament Rupture', inPortuguese: 'Ruptura de Ligamento'}),</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -2647,8 +2561,8 @@
         <v>169</v>
       </c>
       <c r="D70" t="str">
-        <f t="shared" si="2"/>
-        <v>(:Disease {name: 'Backache', inPortuguese: 'Lombalgia'}),</v>
+        <f t="shared" si="1"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Backache', inPortuguese: 'Lombalgia'}),</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -2659,8 +2573,8 @@
         <v>170</v>
       </c>
       <c r="D71" t="str">
-        <f t="shared" si="2"/>
-        <v>(:Disease {name: 'Plantar Fasciitis', inPortuguese: 'Fascite Plantar'}),</v>
+        <f t="shared" si="1"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Plantar Fasciitis', inPortuguese: 'Fascite Plantar'}),</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -2671,8 +2585,8 @@
         <v>171</v>
       </c>
       <c r="D72" t="str">
-        <f t="shared" si="2"/>
-        <v>(:Disease {name: 'Osteoporosis', inPortuguese: 'Osteoporose'}),</v>
+        <f t="shared" si="1"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Osteoporosis', inPortuguese: 'Osteoporose'}),</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -2683,8 +2597,8 @@
         <v>180</v>
       </c>
       <c r="D73" t="str">
-        <f t="shared" si="2"/>
-        <v>(:Disease {name: 'Pulmonary Emphysema', inPortuguese: 'Enfisema Pulmonar'}),</v>
+        <f t="shared" si="1"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Pulmonary Emphysema', inPortuguese: 'Enfisema Pulmonar'}),</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -2695,8 +2609,8 @@
         <v>181</v>
       </c>
       <c r="D74" t="str">
-        <f t="shared" si="2"/>
-        <v>(:Disease {name: 'Bronchitis', inPortuguese: 'Bronquite'}),</v>
+        <f t="shared" si="1"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Bronchitis', inPortuguese: 'Bronquite'}),</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -2707,8 +2621,8 @@
         <v>182</v>
       </c>
       <c r="D75" t="str">
-        <f t="shared" si="2"/>
-        <v>(:Disease {name: 'Tuberculosis', inPortuguese: 'Tuberculose'}),</v>
+        <f t="shared" si="1"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Tuberculosis', inPortuguese: 'Tuberculose'}),</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
@@ -2719,8 +2633,8 @@
         <v>183</v>
       </c>
       <c r="D76" t="str">
-        <f t="shared" si="2"/>
-        <v>(:Disease {name: 'Pharyngitis', inPortuguese: 'Faringite'}),</v>
+        <f t="shared" si="1"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Pharyngitis', inPortuguese: 'Faringite'}),</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
@@ -2731,8 +2645,8 @@
         <v>179</v>
       </c>
       <c r="D77" t="str">
-        <f t="shared" si="2"/>
-        <v>(:Disease {name: 'Pneumonia', inPortuguese: 'Pneumonia'}),</v>
+        <f t="shared" si="1"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Pneumonia', inPortuguese: 'Pneumonia'}),</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
@@ -2743,8 +2657,8 @@
         <v>189</v>
       </c>
       <c r="D78" t="str">
-        <f t="shared" si="2"/>
-        <v>(:Disease {name: 'Allergic Urticaria', inPortuguese: 'Urticária Alérgica'}),</v>
+        <f t="shared" si="1"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Allergic Urticaria', inPortuguese: 'Urticária Alérgica'}),</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
@@ -2755,8 +2669,8 @@
         <v>186</v>
       </c>
       <c r="D79" t="str">
-        <f t="shared" si="2"/>
-        <v>(:Disease {name: 'Angioedema', inPortuguese: 'Angioedema'}),</v>
+        <f t="shared" si="1"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Angioedema', inPortuguese: 'Angioedema'}),</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -2767,8 +2681,8 @@
         <v>190</v>
       </c>
       <c r="D80" t="str">
-        <f t="shared" si="2"/>
-        <v>(:Disease {name: 'Contact Dermatitis', inPortuguese: 'Dermatite de Contato'}),</v>
+        <f t="shared" si="1"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Contact Dermatitis', inPortuguese: 'Dermatite de Contato'}),</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
@@ -2779,8 +2693,8 @@
         <v>191</v>
       </c>
       <c r="D81" t="str">
-        <f t="shared" si="2"/>
-        <v>(:Disease {name: 'Atopic Dermatitis', inPortuguese: 'Dermatite Atópica'}),</v>
+        <f t="shared" si="1"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Atopic Dermatitis', inPortuguese: 'Dermatite Atópica'}),</v>
       </c>
     </row>
   </sheetData>
@@ -2790,6 +2704,1691 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F94BB071-87F4-4604-9E70-F91A6E8FB04C}">
+  <dimension ref="A1:D50"/>
+  <sheetViews>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1"/>
+    <col min="4" max="4" width="48.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D2" t="str">
+        <f>"(:Allergy {uuid: apoc.create.uuid(), name: '" &amp; B2 &amp;"', inPortuguese: '" &amp; A2 &amp;"', type: '" &amp; C2 &amp;"'}),"</f>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Cream', inPortuguese: 'Creme', type: 'Other'}),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C3" t="s">
+        <v>235</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D50" si="0">"(:Allergy {uuid: apoc.create.uuid(), name: '" &amp; B3 &amp;"', inPortuguese: '" &amp; A3 &amp;"', type: '" &amp; C3 &amp;"'}),"</f>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Soap', inPortuguese: 'Sabonete', type: 'Other'}),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>230</v>
+      </c>
+      <c r="B4" t="s">
+        <v>242</v>
+      </c>
+      <c r="C4" t="s">
+        <v>235</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Make up', inPortuguese: 'Maquiagem', type: 'Other'}),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B5" t="s">
+        <v>243</v>
+      </c>
+      <c r="C5" t="s">
+        <v>235</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'perfume', inPortuguese: 'Perfume', type: 'Other'}),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>232</v>
+      </c>
+      <c r="B6" t="s">
+        <v>244</v>
+      </c>
+      <c r="C6" t="s">
+        <v>235</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Latex Product', inPortuguese: 'Produto de Látex', type: 'Other'}),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B7" t="s">
+        <v>245</v>
+      </c>
+      <c r="C7" t="s">
+        <v>235</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Bijou', inPortuguese: 'Bijuteria', type: 'Other'}),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>192</v>
+      </c>
+      <c r="B8" t="s">
+        <v>246</v>
+      </c>
+      <c r="C8" t="s">
+        <v>235</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Ink', inPortuguese: 'Tinta', type: 'Other'}),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>193</v>
+      </c>
+      <c r="B9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C9" t="s">
+        <v>236</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Mosquito', inPortuguese: 'Mosquito', type: 'Insect'}),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>194</v>
+      </c>
+      <c r="B10" t="s">
+        <v>247</v>
+      </c>
+      <c r="C10" t="s">
+        <v>236</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Bee', inPortuguese: 'Abelha', type: 'Insect'}),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>195</v>
+      </c>
+      <c r="B11" t="s">
+        <v>248</v>
+      </c>
+      <c r="C11" t="s">
+        <v>236</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Flea', inPortuguese: 'Pulga', type: 'Insect'}),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>196</v>
+      </c>
+      <c r="B12" t="s">
+        <v>249</v>
+      </c>
+      <c r="C12" t="s">
+        <v>239</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Cat', inPortuguese: 'Gato', type: 'Animal'}),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>197</v>
+      </c>
+      <c r="B13" t="s">
+        <v>250</v>
+      </c>
+      <c r="C13" t="s">
+        <v>239</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Puppy', inPortuguese: 'Cachorro', type: 'Animal'}),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>198</v>
+      </c>
+      <c r="B14" t="s">
+        <v>277</v>
+      </c>
+      <c r="C14" t="s">
+        <v>236</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Ant', inPortuguese: 'Formiga', type: 'Insect'}),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>199</v>
+      </c>
+      <c r="B15" t="s">
+        <v>251</v>
+      </c>
+      <c r="C15" t="s">
+        <v>236</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Wasp', inPortuguese: 'Vespa', type: 'Insect'}),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>200</v>
+      </c>
+      <c r="B16" t="s">
+        <v>252</v>
+      </c>
+      <c r="C16" t="s">
+        <v>236</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Tick', inPortuguese: 'Carrapato', type: 'Insect'}),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>201</v>
+      </c>
+      <c r="B17" t="s">
+        <v>253</v>
+      </c>
+      <c r="C17" t="s">
+        <v>236</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Leggy', inPortuguese: 'Pernilongo', type: 'Insect'}),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>202</v>
+      </c>
+      <c r="B18" t="s">
+        <v>254</v>
+      </c>
+      <c r="C18" t="s">
+        <v>236</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Rubber', inPortuguese: 'Borrachudo', type: 'Insect'}),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>203</v>
+      </c>
+      <c r="B19" t="s">
+        <v>255</v>
+      </c>
+      <c r="C19" t="s">
+        <v>237</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Aspirin', inPortuguese: 'Aspirina', type: 'Drug'}),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>204</v>
+      </c>
+      <c r="B20" t="s">
+        <v>256</v>
+      </c>
+      <c r="C20" t="s">
+        <v>237</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Dipyrone', inPortuguese: 'Dipirona', type: 'Drug'}),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>205</v>
+      </c>
+      <c r="B21" t="s">
+        <v>205</v>
+      </c>
+      <c r="C21" t="s">
+        <v>237</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Paracetamol', inPortuguese: 'Paracetamol', type: 'Drug'}),</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>206</v>
+      </c>
+      <c r="B22" t="s">
+        <v>257</v>
+      </c>
+      <c r="C22" t="s">
+        <v>237</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Diclofenac', inPortuguese: 'Diclofenaco', type: 'Drug'}),</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>207</v>
+      </c>
+      <c r="B23" t="s">
+        <v>258</v>
+      </c>
+      <c r="C23" t="s">
+        <v>237</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Penicillin', inPortuguese: 'Penicilina', type: 'Drug'}),</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>208</v>
+      </c>
+      <c r="B24" t="s">
+        <v>208</v>
+      </c>
+      <c r="C24" t="s">
+        <v>237</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Sulfa', inPortuguese: 'Sulfa', type: 'Drug'}),</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>209</v>
+      </c>
+      <c r="B25" t="s">
+        <v>259</v>
+      </c>
+      <c r="C25" t="s">
+        <v>237</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Quinolone', inPortuguese: 'Quinolona', type: 'Drug'}),</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>210</v>
+      </c>
+      <c r="B26" t="s">
+        <v>260</v>
+      </c>
+      <c r="C26" t="s">
+        <v>237</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Erythromycin', inPortuguese: 'Eritromicina', type: 'Drug'}),</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>211</v>
+      </c>
+      <c r="B27" t="s">
+        <v>261</v>
+      </c>
+      <c r="C27" t="s">
+        <v>237</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Azithromycin', inPortuguese: 'Azitromicina', type: 'Drug'}),</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>212</v>
+      </c>
+      <c r="B28" t="s">
+        <v>262</v>
+      </c>
+      <c r="C28" t="s">
+        <v>237</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Iodinated Contrast', inPortuguese: 'Contraste Iodado', type: 'Drug'}),</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>213</v>
+      </c>
+      <c r="B29" t="s">
+        <v>263</v>
+      </c>
+      <c r="C29" t="s">
+        <v>236</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Mite', inPortuguese: 'Ácaro', type: 'Insect'}),</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>214</v>
+      </c>
+      <c r="B30" t="s">
+        <v>264</v>
+      </c>
+      <c r="C30" t="s">
+        <v>235</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Dust', inPortuguese: 'Poeira', type: 'Other'}),</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>215</v>
+      </c>
+      <c r="B31" t="s">
+        <v>265</v>
+      </c>
+      <c r="C31" t="s">
+        <v>235</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Mold', inPortuguese: 'Mofo', type: 'Other'}),</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>216</v>
+      </c>
+      <c r="B32" t="s">
+        <v>266</v>
+      </c>
+      <c r="C32" t="s">
+        <v>235</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Pollen', inPortuguese: 'Pólen', type: 'Other'}),</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>217</v>
+      </c>
+      <c r="B33" t="s">
+        <v>267</v>
+      </c>
+      <c r="C33" t="s">
+        <v>235</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Smoke', inPortuguese: 'Fumaça', type: 'Other'}),</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>218</v>
+      </c>
+      <c r="B34" t="s">
+        <v>268</v>
+      </c>
+      <c r="C34" t="s">
+        <v>235</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Pollution', inPortuguese: 'Poluição', type: 'Other'}),</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>219</v>
+      </c>
+      <c r="B35" t="s">
+        <v>269</v>
+      </c>
+      <c r="C35" t="s">
+        <v>238</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Milk', inPortuguese: 'Leite', type: 'Food'}),</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>220</v>
+      </c>
+      <c r="B36" t="s">
+        <v>270</v>
+      </c>
+      <c r="C36" t="s">
+        <v>238</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Egg', inPortuguese: 'Ovo', type: 'Food'}),</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>221</v>
+      </c>
+      <c r="B37" t="s">
+        <v>271</v>
+      </c>
+      <c r="C37" t="s">
+        <v>238</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Wheat', inPortuguese: 'Trigo', type: 'Food'}),</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>222</v>
+      </c>
+      <c r="B38" t="s">
+        <v>272</v>
+      </c>
+      <c r="C38" t="s">
+        <v>238</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Peanut', inPortuguese: 'Amendoim', type: 'Food'}),</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>223</v>
+      </c>
+      <c r="B39" t="s">
+        <v>273</v>
+      </c>
+      <c r="C39" t="s">
+        <v>238</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Seafood', inPortuguese: 'Frutos do Mar', type: 'Food'}),</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>224</v>
+      </c>
+      <c r="B40" t="s">
+        <v>278</v>
+      </c>
+      <c r="C40" t="s">
+        <v>238</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Dry Fruits', inPortuguese: 'Frutas Secas', type: 'Food'}),</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>225</v>
+      </c>
+      <c r="B41" t="s">
+        <v>274</v>
+      </c>
+      <c r="C41" t="s">
+        <v>238</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Soy', inPortuguese: 'Soja', type: 'Food'}),</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>226</v>
+      </c>
+      <c r="B42" t="s">
+        <v>275</v>
+      </c>
+      <c r="C42" t="s">
+        <v>238</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Fish', inPortuguese: 'Peixe', type: 'Food'}),</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>279</v>
+      </c>
+      <c r="B43" t="s">
+        <v>288</v>
+      </c>
+      <c r="C43" t="s">
+        <v>238</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Crustacean', inPortuguese: 'Crustáceo', type: 'Food'}),</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>280</v>
+      </c>
+      <c r="B44" t="s">
+        <v>287</v>
+      </c>
+      <c r="C44" t="s">
+        <v>238</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Mollusk', inPortuguese: 'Molusco', type: 'Food'}),</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>227</v>
+      </c>
+      <c r="B45" t="s">
+        <v>276</v>
+      </c>
+      <c r="C45" t="s">
+        <v>238</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Gluten', inPortuguese: 'Glúten', type: 'Food'}),</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>281</v>
+      </c>
+      <c r="B46" t="s">
+        <v>283</v>
+      </c>
+      <c r="C46" t="s">
+        <v>238</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Shrimp', inPortuguese: 'Camarão', type: 'Food'}),</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>282</v>
+      </c>
+      <c r="B47" t="s">
+        <v>284</v>
+      </c>
+      <c r="C47" t="s">
+        <v>238</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Squid', inPortuguese: 'Lula', type: 'Food'}),</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>285</v>
+      </c>
+      <c r="B48" t="s">
+        <v>286</v>
+      </c>
+      <c r="C48" t="s">
+        <v>238</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Pufferfish', inPortuguese: 'Baiacu', type: 'Food'}),</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>289</v>
+      </c>
+      <c r="B49" t="s">
+        <v>289</v>
+      </c>
+      <c r="C49" t="s">
+        <v>238</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Chocolate', inPortuguese: 'Chocolate', type: 'Food'}),</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>290</v>
+      </c>
+      <c r="B50" t="s">
+        <v>290</v>
+      </c>
+      <c r="C50" t="s">
+        <v>238</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Allergy {uuid: apoc.create.uuid(), name: 'Caviar', inPortuguese: 'Caviar', type: 'Food'}),</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FBDA324-BA52-4553-9EA4-1F1EB8000A70}">
+  <dimension ref="A1:D50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1"/>
+    <col min="4" max="4" width="48.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="str">
+        <f>allergy!A2</f>
+        <v>Creme</v>
+      </c>
+      <c r="B2" t="str">
+        <f>allergy!B2</f>
+        <v>Cream</v>
+      </c>
+      <c r="C2" t="str">
+        <f>allergy!C2</f>
+        <v>Other</v>
+      </c>
+      <c r="D2" t="str">
+        <f>"(:Intolerance {uuid: apoc.create.uuid(), name: '" &amp; B2 &amp;"', inPortuguese: '" &amp; A2 &amp;"', type: '" &amp; C2 &amp;"'}),"</f>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Cream', inPortuguese: 'Creme', type: 'Other'}),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="str">
+        <f>allergy!A3</f>
+        <v>Sabonete</v>
+      </c>
+      <c r="B3" t="str">
+        <f>allergy!B3</f>
+        <v>Soap</v>
+      </c>
+      <c r="C3" t="str">
+        <f>allergy!C3</f>
+        <v>Other</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D50" si="0">"(:Intolerance {uuid: apoc.create.uuid(), name: '" &amp; B3 &amp;"', inPortuguese: '" &amp; A3 &amp;"', type: '" &amp; C3 &amp;"'}),"</f>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Soap', inPortuguese: 'Sabonete', type: 'Other'}),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="str">
+        <f>allergy!A4</f>
+        <v>Maquiagem</v>
+      </c>
+      <c r="B4" t="str">
+        <f>allergy!B4</f>
+        <v>Make up</v>
+      </c>
+      <c r="C4" t="str">
+        <f>allergy!C4</f>
+        <v>Other</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Make up', inPortuguese: 'Maquiagem', type: 'Other'}),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="str">
+        <f>allergy!A5</f>
+        <v>Perfume</v>
+      </c>
+      <c r="B5" t="str">
+        <f>allergy!B5</f>
+        <v>perfume</v>
+      </c>
+      <c r="C5" t="str">
+        <f>allergy!C5</f>
+        <v>Other</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'perfume', inPortuguese: 'Perfume', type: 'Other'}),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="str">
+        <f>allergy!A6</f>
+        <v>Produto de Látex</v>
+      </c>
+      <c r="B6" t="str">
+        <f>allergy!B6</f>
+        <v>Latex Product</v>
+      </c>
+      <c r="C6" t="str">
+        <f>allergy!C6</f>
+        <v>Other</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Latex Product', inPortuguese: 'Produto de Látex', type: 'Other'}),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="str">
+        <f>allergy!A7</f>
+        <v>Bijuteria</v>
+      </c>
+      <c r="B7" t="str">
+        <f>allergy!B7</f>
+        <v>Bijou</v>
+      </c>
+      <c r="C7" t="str">
+        <f>allergy!C7</f>
+        <v>Other</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Bijou', inPortuguese: 'Bijuteria', type: 'Other'}),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="str">
+        <f>allergy!A8</f>
+        <v>Tinta</v>
+      </c>
+      <c r="B8" t="str">
+        <f>allergy!B8</f>
+        <v>Ink</v>
+      </c>
+      <c r="C8" t="str">
+        <f>allergy!C8</f>
+        <v>Other</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Ink', inPortuguese: 'Tinta', type: 'Other'}),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="str">
+        <f>allergy!A9</f>
+        <v>Mosquito</v>
+      </c>
+      <c r="B9" t="str">
+        <f>allergy!B9</f>
+        <v>Mosquito</v>
+      </c>
+      <c r="C9" t="str">
+        <f>allergy!C9</f>
+        <v>Insect</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Mosquito', inPortuguese: 'Mosquito', type: 'Insect'}),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="str">
+        <f>allergy!A10</f>
+        <v>Abelha</v>
+      </c>
+      <c r="B10" t="str">
+        <f>allergy!B10</f>
+        <v>Bee</v>
+      </c>
+      <c r="C10" t="str">
+        <f>allergy!C10</f>
+        <v>Insect</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Bee', inPortuguese: 'Abelha', type: 'Insect'}),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="str">
+        <f>allergy!A11</f>
+        <v>Pulga</v>
+      </c>
+      <c r="B11" t="str">
+        <f>allergy!B11</f>
+        <v>Flea</v>
+      </c>
+      <c r="C11" t="str">
+        <f>allergy!C11</f>
+        <v>Insect</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Flea', inPortuguese: 'Pulga', type: 'Insect'}),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="str">
+        <f>allergy!A12</f>
+        <v>Gato</v>
+      </c>
+      <c r="B12" t="str">
+        <f>allergy!B12</f>
+        <v>Cat</v>
+      </c>
+      <c r="C12" t="str">
+        <f>allergy!C12</f>
+        <v>Animal</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Cat', inPortuguese: 'Gato', type: 'Animal'}),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="str">
+        <f>allergy!A13</f>
+        <v>Cachorro</v>
+      </c>
+      <c r="B13" t="str">
+        <f>allergy!B13</f>
+        <v>Puppy</v>
+      </c>
+      <c r="C13" t="str">
+        <f>allergy!C13</f>
+        <v>Animal</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Puppy', inPortuguese: 'Cachorro', type: 'Animal'}),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="str">
+        <f>allergy!A14</f>
+        <v>Formiga</v>
+      </c>
+      <c r="B14" t="str">
+        <f>allergy!B14</f>
+        <v>Ant</v>
+      </c>
+      <c r="C14" t="str">
+        <f>allergy!C14</f>
+        <v>Insect</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Ant', inPortuguese: 'Formiga', type: 'Insect'}),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="str">
+        <f>allergy!A15</f>
+        <v>Vespa</v>
+      </c>
+      <c r="B15" t="str">
+        <f>allergy!B15</f>
+        <v>Wasp</v>
+      </c>
+      <c r="C15" t="str">
+        <f>allergy!C15</f>
+        <v>Insect</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Wasp', inPortuguese: 'Vespa', type: 'Insect'}),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="str">
+        <f>allergy!A16</f>
+        <v>Carrapato</v>
+      </c>
+      <c r="B16" t="str">
+        <f>allergy!B16</f>
+        <v>Tick</v>
+      </c>
+      <c r="C16" t="str">
+        <f>allergy!C16</f>
+        <v>Insect</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Tick', inPortuguese: 'Carrapato', type: 'Insect'}),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="str">
+        <f>allergy!A17</f>
+        <v>Pernilongo</v>
+      </c>
+      <c r="B17" t="str">
+        <f>allergy!B17</f>
+        <v>Leggy</v>
+      </c>
+      <c r="C17" t="str">
+        <f>allergy!C17</f>
+        <v>Insect</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Leggy', inPortuguese: 'Pernilongo', type: 'Insect'}),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="str">
+        <f>allergy!A18</f>
+        <v>Borrachudo</v>
+      </c>
+      <c r="B18" t="str">
+        <f>allergy!B18</f>
+        <v>Rubber</v>
+      </c>
+      <c r="C18" t="str">
+        <f>allergy!C18</f>
+        <v>Insect</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Rubber', inPortuguese: 'Borrachudo', type: 'Insect'}),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="str">
+        <f>allergy!A19</f>
+        <v>Aspirina</v>
+      </c>
+      <c r="B19" t="str">
+        <f>allergy!B19</f>
+        <v>Aspirin</v>
+      </c>
+      <c r="C19" t="str">
+        <f>allergy!C19</f>
+        <v>Drug</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Aspirin', inPortuguese: 'Aspirina', type: 'Drug'}),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="str">
+        <f>allergy!A20</f>
+        <v>Dipirona</v>
+      </c>
+      <c r="B20" t="str">
+        <f>allergy!B20</f>
+        <v>Dipyrone</v>
+      </c>
+      <c r="C20" t="str">
+        <f>allergy!C20</f>
+        <v>Drug</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Dipyrone', inPortuguese: 'Dipirona', type: 'Drug'}),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="str">
+        <f>allergy!A21</f>
+        <v>Paracetamol</v>
+      </c>
+      <c r="B21" t="str">
+        <f>allergy!B21</f>
+        <v>Paracetamol</v>
+      </c>
+      <c r="C21" t="str">
+        <f>allergy!C21</f>
+        <v>Drug</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Paracetamol', inPortuguese: 'Paracetamol', type: 'Drug'}),</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="str">
+        <f>allergy!A22</f>
+        <v>Diclofenaco</v>
+      </c>
+      <c r="B22" t="str">
+        <f>allergy!B22</f>
+        <v>Diclofenac</v>
+      </c>
+      <c r="C22" t="str">
+        <f>allergy!C22</f>
+        <v>Drug</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Diclofenac', inPortuguese: 'Diclofenaco', type: 'Drug'}),</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="str">
+        <f>allergy!A23</f>
+        <v>Penicilina</v>
+      </c>
+      <c r="B23" t="str">
+        <f>allergy!B23</f>
+        <v>Penicillin</v>
+      </c>
+      <c r="C23" t="str">
+        <f>allergy!C23</f>
+        <v>Drug</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Penicillin', inPortuguese: 'Penicilina', type: 'Drug'}),</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="str">
+        <f>allergy!A24</f>
+        <v>Sulfa</v>
+      </c>
+      <c r="B24" t="str">
+        <f>allergy!B24</f>
+        <v>Sulfa</v>
+      </c>
+      <c r="C24" t="str">
+        <f>allergy!C24</f>
+        <v>Drug</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Sulfa', inPortuguese: 'Sulfa', type: 'Drug'}),</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="str">
+        <f>allergy!A25</f>
+        <v>Quinolona</v>
+      </c>
+      <c r="B25" t="str">
+        <f>allergy!B25</f>
+        <v>Quinolone</v>
+      </c>
+      <c r="C25" t="str">
+        <f>allergy!C25</f>
+        <v>Drug</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Quinolone', inPortuguese: 'Quinolona', type: 'Drug'}),</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="str">
+        <f>allergy!A26</f>
+        <v>Eritromicina</v>
+      </c>
+      <c r="B26" t="str">
+        <f>allergy!B26</f>
+        <v>Erythromycin</v>
+      </c>
+      <c r="C26" t="str">
+        <f>allergy!C26</f>
+        <v>Drug</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Erythromycin', inPortuguese: 'Eritromicina', type: 'Drug'}),</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="str">
+        <f>allergy!A27</f>
+        <v>Azitromicina</v>
+      </c>
+      <c r="B27" t="str">
+        <f>allergy!B27</f>
+        <v>Azithromycin</v>
+      </c>
+      <c r="C27" t="str">
+        <f>allergy!C27</f>
+        <v>Drug</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Azithromycin', inPortuguese: 'Azitromicina', type: 'Drug'}),</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="str">
+        <f>allergy!A28</f>
+        <v>Contraste Iodado</v>
+      </c>
+      <c r="B28" t="str">
+        <f>allergy!B28</f>
+        <v>Iodinated Contrast</v>
+      </c>
+      <c r="C28" t="str">
+        <f>allergy!C28</f>
+        <v>Drug</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Iodinated Contrast', inPortuguese: 'Contraste Iodado', type: 'Drug'}),</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="str">
+        <f>allergy!A29</f>
+        <v>Ácaro</v>
+      </c>
+      <c r="B29" t="str">
+        <f>allergy!B29</f>
+        <v>Mite</v>
+      </c>
+      <c r="C29" t="str">
+        <f>allergy!C29</f>
+        <v>Insect</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Mite', inPortuguese: 'Ácaro', type: 'Insect'}),</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="str">
+        <f>allergy!A30</f>
+        <v>Poeira</v>
+      </c>
+      <c r="B30" t="str">
+        <f>allergy!B30</f>
+        <v>Dust</v>
+      </c>
+      <c r="C30" t="str">
+        <f>allergy!C30</f>
+        <v>Other</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Dust', inPortuguese: 'Poeira', type: 'Other'}),</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="str">
+        <f>allergy!A31</f>
+        <v>Mofo</v>
+      </c>
+      <c r="B31" t="str">
+        <f>allergy!B31</f>
+        <v>Mold</v>
+      </c>
+      <c r="C31" t="str">
+        <f>allergy!C31</f>
+        <v>Other</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Mold', inPortuguese: 'Mofo', type: 'Other'}),</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="str">
+        <f>allergy!A32</f>
+        <v>Pólen</v>
+      </c>
+      <c r="B32" t="str">
+        <f>allergy!B32</f>
+        <v>Pollen</v>
+      </c>
+      <c r="C32" t="str">
+        <f>allergy!C32</f>
+        <v>Other</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Pollen', inPortuguese: 'Pólen', type: 'Other'}),</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="str">
+        <f>allergy!A33</f>
+        <v>Fumaça</v>
+      </c>
+      <c r="B33" t="str">
+        <f>allergy!B33</f>
+        <v>Smoke</v>
+      </c>
+      <c r="C33" t="str">
+        <f>allergy!C33</f>
+        <v>Other</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Smoke', inPortuguese: 'Fumaça', type: 'Other'}),</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="str">
+        <f>allergy!A34</f>
+        <v>Poluição</v>
+      </c>
+      <c r="B34" t="str">
+        <f>allergy!B34</f>
+        <v>Pollution</v>
+      </c>
+      <c r="C34" t="str">
+        <f>allergy!C34</f>
+        <v>Other</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Pollution', inPortuguese: 'Poluição', type: 'Other'}),</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="str">
+        <f>allergy!A35</f>
+        <v>Leite</v>
+      </c>
+      <c r="B35" t="str">
+        <f>allergy!B35</f>
+        <v>Milk</v>
+      </c>
+      <c r="C35" t="str">
+        <f>allergy!C35</f>
+        <v>Food</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Milk', inPortuguese: 'Leite', type: 'Food'}),</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="str">
+        <f>allergy!A36</f>
+        <v>Ovo</v>
+      </c>
+      <c r="B36" t="str">
+        <f>allergy!B36</f>
+        <v>Egg</v>
+      </c>
+      <c r="C36" t="str">
+        <f>allergy!C36</f>
+        <v>Food</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Egg', inPortuguese: 'Ovo', type: 'Food'}),</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="str">
+        <f>allergy!A37</f>
+        <v>Trigo</v>
+      </c>
+      <c r="B37" t="str">
+        <f>allergy!B37</f>
+        <v>Wheat</v>
+      </c>
+      <c r="C37" t="str">
+        <f>allergy!C37</f>
+        <v>Food</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Wheat', inPortuguese: 'Trigo', type: 'Food'}),</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="str">
+        <f>allergy!A38</f>
+        <v>Amendoim</v>
+      </c>
+      <c r="B38" t="str">
+        <f>allergy!B38</f>
+        <v>Peanut</v>
+      </c>
+      <c r="C38" t="str">
+        <f>allergy!C38</f>
+        <v>Food</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Peanut', inPortuguese: 'Amendoim', type: 'Food'}),</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="str">
+        <f>allergy!A39</f>
+        <v>Frutos do Mar</v>
+      </c>
+      <c r="B39" t="str">
+        <f>allergy!B39</f>
+        <v>Seafood</v>
+      </c>
+      <c r="C39" t="str">
+        <f>allergy!C39</f>
+        <v>Food</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Seafood', inPortuguese: 'Frutos do Mar', type: 'Food'}),</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="str">
+        <f>allergy!A40</f>
+        <v>Frutas Secas</v>
+      </c>
+      <c r="B40" t="str">
+        <f>allergy!B40</f>
+        <v>Dry Fruits</v>
+      </c>
+      <c r="C40" t="str">
+        <f>allergy!C40</f>
+        <v>Food</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Dry Fruits', inPortuguese: 'Frutas Secas', type: 'Food'}),</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="str">
+        <f>allergy!A41</f>
+        <v>Soja</v>
+      </c>
+      <c r="B41" t="str">
+        <f>allergy!B41</f>
+        <v>Soy</v>
+      </c>
+      <c r="C41" t="str">
+        <f>allergy!C41</f>
+        <v>Food</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Soy', inPortuguese: 'Soja', type: 'Food'}),</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="str">
+        <f>allergy!A42</f>
+        <v>Peixe</v>
+      </c>
+      <c r="B42" t="str">
+        <f>allergy!B42</f>
+        <v>Fish</v>
+      </c>
+      <c r="C42" t="str">
+        <f>allergy!C42</f>
+        <v>Food</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Fish', inPortuguese: 'Peixe', type: 'Food'}),</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="str">
+        <f>allergy!A43</f>
+        <v>Crustáceo</v>
+      </c>
+      <c r="B43" t="str">
+        <f>allergy!B43</f>
+        <v>Crustacean</v>
+      </c>
+      <c r="C43" t="str">
+        <f>allergy!C43</f>
+        <v>Food</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Crustacean', inPortuguese: 'Crustáceo', type: 'Food'}),</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="str">
+        <f>allergy!A44</f>
+        <v>Molusco</v>
+      </c>
+      <c r="B44" t="str">
+        <f>allergy!B44</f>
+        <v>Mollusk</v>
+      </c>
+      <c r="C44" t="str">
+        <f>allergy!C44</f>
+        <v>Food</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Mollusk', inPortuguese: 'Molusco', type: 'Food'}),</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="str">
+        <f>allergy!A45</f>
+        <v>Glúten</v>
+      </c>
+      <c r="B45" t="str">
+        <f>allergy!B45</f>
+        <v>Gluten</v>
+      </c>
+      <c r="C45" t="str">
+        <f>allergy!C45</f>
+        <v>Food</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Gluten', inPortuguese: 'Glúten', type: 'Food'}),</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="str">
+        <f>allergy!A46</f>
+        <v>Camarão</v>
+      </c>
+      <c r="B46" t="str">
+        <f>allergy!B46</f>
+        <v>Shrimp</v>
+      </c>
+      <c r="C46" t="str">
+        <f>allergy!C46</f>
+        <v>Food</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Shrimp', inPortuguese: 'Camarão', type: 'Food'}),</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" t="str">
+        <f>allergy!A47</f>
+        <v>Lula</v>
+      </c>
+      <c r="B47" t="str">
+        <f>allergy!B47</f>
+        <v>Squid</v>
+      </c>
+      <c r="C47" t="str">
+        <f>allergy!C47</f>
+        <v>Food</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Squid', inPortuguese: 'Lula', type: 'Food'}),</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="str">
+        <f>allergy!A48</f>
+        <v>Baiacu</v>
+      </c>
+      <c r="B48" t="str">
+        <f>allergy!B48</f>
+        <v>Pufferfish</v>
+      </c>
+      <c r="C48" t="str">
+        <f>allergy!C48</f>
+        <v>Food</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Pufferfish', inPortuguese: 'Baiacu', type: 'Food'}),</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" t="str">
+        <f>allergy!A49</f>
+        <v>Chocolate</v>
+      </c>
+      <c r="B49" t="str">
+        <f>allergy!B49</f>
+        <v>Chocolate</v>
+      </c>
+      <c r="C49" t="str">
+        <f>allergy!C49</f>
+        <v>Food</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Chocolate', inPortuguese: 'Chocolate', type: 'Food'}),</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" t="str">
+        <f>allergy!A50</f>
+        <v>Caviar</v>
+      </c>
+      <c r="B50" t="str">
+        <f>allergy!B50</f>
+        <v>Caviar</v>
+      </c>
+      <c r="C50" t="str">
+        <f>allergy!C50</f>
+        <v>Food</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Caviar', inPortuguese: 'Caviar', type: 'Food'}),</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F5CDE23-EAB5-47A7-B33D-96F18BE56CCE}">
   <dimension ref="A1:C18"/>
   <sheetViews>
@@ -3023,12 +4622,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8BE5788-872A-43B9-9E25-E8C1A583BFB6}">
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
-      <selection activeCell="C20" sqref="C2:C20"/>
+      <selection activeCell="C2" sqref="C2:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3056,8 +4655,8 @@
         <v>22</v>
       </c>
       <c r="C2" t="str">
-        <f t="shared" ref="C2:C20" si="0">"(:Specialty {name: '" &amp; B2 &amp;"', inPortuguese: '" &amp; A2 &amp;"'}),"</f>
-        <v>(:Specialty {name: 'Pediatrician', inPortuguese: 'Pediatra'}),</v>
+        <f>"(:Specialty {uuid: apoc.create.uuid(), name: '" &amp; B2 &amp;"', inPortuguese: '" &amp; A2 &amp;"'}),"</f>
+        <v>(:Specialty {uuid: apoc.create.uuid(), name: 'Pediatrician', inPortuguese: 'Pediatra'}),</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -3068,8 +4667,8 @@
         <v>23</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Specialty {name: 'Otolaryngologist', inPortuguese: 'Otorrinolaringologista'}),</v>
+        <f t="shared" ref="C3:C20" si="0">"(:Specialty {uuid: apoc.create.uuid(), name: '" &amp; B3 &amp;"', inPortuguese: '" &amp; A3 &amp;"'}),"</f>
+        <v>(:Specialty {uuid: apoc.create.uuid(), name: 'Otolaryngologist', inPortuguese: 'Otorrinolaringologista'}),</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -3081,7 +4680,7 @@
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
-        <v>(:Specialty {name: 'Ophthalmologist', inPortuguese: 'Oftalmologista'}),</v>
+        <v>(:Specialty {uuid: apoc.create.uuid(), name: 'Ophthalmologist', inPortuguese: 'Oftalmologista'}),</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -3093,7 +4692,7 @@
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
-        <v>(:Specialty {name: 'Allergist', inPortuguese: 'Alergologista'}),</v>
+        <v>(:Specialty {uuid: apoc.create.uuid(), name: 'Allergist', inPortuguese: 'Alergologista'}),</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -3105,7 +4704,7 @@
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
-        <v>(:Specialty {name: 'Dentist', inPortuguese: 'Dentista'}),</v>
+        <v>(:Specialty {uuid: apoc.create.uuid(), name: 'Dentist', inPortuguese: 'Dentista'}),</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -3117,7 +4716,7 @@
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
-        <v>(:Specialty {name: 'Endocrinologist', inPortuguese: 'Endocrinologista'}),</v>
+        <v>(:Specialty {uuid: apoc.create.uuid(), name: 'Endocrinologist', inPortuguese: 'Endocrinologista'}),</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -3129,7 +4728,7 @@
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
-        <v>(:Specialty {name: 'Orthopedist', inPortuguese: 'Ortopedista'}),</v>
+        <v>(:Specialty {uuid: apoc.create.uuid(), name: 'Orthopedist', inPortuguese: 'Ortopedista'}),</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -3141,7 +4740,7 @@
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
-        <v>(:Specialty {name: 'Pulmonologist', inPortuguese: 'Pneumologista'}),</v>
+        <v>(:Specialty {uuid: apoc.create.uuid(), name: 'Pulmonologist', inPortuguese: 'Pneumologista'}),</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -3153,7 +4752,7 @@
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
-        <v>(:Specialty {name: 'Cardiologist', inPortuguese: 'Cardiologista'}),</v>
+        <v>(:Specialty {uuid: apoc.create.uuid(), name: 'Cardiologist', inPortuguese: 'Cardiologista'}),</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -3165,7 +4764,7 @@
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
-        <v>(:Specialty {name: 'Nutritionist', inPortuguese: 'Nutrólogo'}),</v>
+        <v>(:Specialty {uuid: apoc.create.uuid(), name: 'Nutritionist', inPortuguese: 'Nutrólogo'}),</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -3177,7 +4776,7 @@
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
-        <v>(:Specialty {name: 'Physiotherapist', inPortuguese: 'Fisioterapeuta'}),</v>
+        <v>(:Specialty {uuid: apoc.create.uuid(), name: 'Physiotherapist', inPortuguese: 'Fisioterapeuta'}),</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -3189,7 +4788,7 @@
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
-        <v>(:Specialty {name: 'Speech Therapist', inPortuguese: 'Fonoaudiólogo'}),</v>
+        <v>(:Specialty {uuid: apoc.create.uuid(), name: 'Speech Therapist', inPortuguese: 'Fonoaudiólogo'}),</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -3201,7 +4800,7 @@
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
-        <v>(:Specialty {name: 'Psychologist', inPortuguese: 'Psicólogo'}),</v>
+        <v>(:Specialty {uuid: apoc.create.uuid(), name: 'Psychologist', inPortuguese: 'Psicólogo'}),</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -3213,7 +4812,7 @@
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
-        <v>(:Specialty {name: 'Neurologist', inPortuguese: 'Neurologista'}),</v>
+        <v>(:Specialty {uuid: apoc.create.uuid(), name: 'Neurologist', inPortuguese: 'Neurologista'}),</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -3225,7 +4824,7 @@
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
-        <v>(:Specialty {name: 'Oncologist', inPortuguese: 'Oncologista'}),</v>
+        <v>(:Specialty {uuid: apoc.create.uuid(), name: 'Oncologist', inPortuguese: 'Oncologista'}),</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -3237,7 +4836,7 @@
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
-        <v>(:Specialty {name: 'Psychiatrist', inPortuguese: 'Psiquiatra'}),</v>
+        <v>(:Specialty {uuid: apoc.create.uuid(), name: 'Psychiatrist', inPortuguese: 'Psiquiatra'}),</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -3249,7 +4848,7 @@
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
-        <v>(:Specialty {name: 'Hebrew', inPortuguese: 'Hebiatra'}),</v>
+        <v>(:Specialty {uuid: apoc.create.uuid(), name: 'Hebrew', inPortuguese: 'Hebiatra'}),</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -3261,7 +4860,7 @@
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
-        <v>(:Specialty {name: 'Nephrologist', inPortuguese: 'Nefrologista'}),</v>
+        <v>(:Specialty {uuid: apoc.create.uuid(), name: 'Nephrologist', inPortuguese: 'Nefrologista'}),</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -3273,1697 +4872,12 @@
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
-        <v>(:Specialty {name: 'Urologist ', inPortuguese: 'Urologista'}),</v>
+        <v>(:Specialty {uuid: apoc.create.uuid(), name: 'Urologist ', inPortuguese: 'Urologista'}),</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F94BB071-87F4-4604-9E70-F91A6E8FB04C}">
-  <dimension ref="A1:D50"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="2" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" customWidth="1"/>
-    <col min="4" max="4" width="48.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>234</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>228</v>
-      </c>
-      <c r="B2" t="s">
-        <v>240</v>
-      </c>
-      <c r="C2" t="s">
-        <v>235</v>
-      </c>
-      <c r="D2" t="str">
-        <f>"(:Allergy {name: '" &amp; B2 &amp;"', inPortuguese: '" &amp; A2 &amp;"', type: '" &amp; C2 &amp;"'}),"</f>
-        <v>(:Allergy {name: 'Cream', inPortuguese: 'Creme', type: 'Other'}),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>229</v>
-      </c>
-      <c r="B3" t="s">
-        <v>241</v>
-      </c>
-      <c r="C3" t="s">
-        <v>235</v>
-      </c>
-      <c r="D3" t="str">
-        <f t="shared" ref="D3:D45" si="0">"(:Allergy {name: '" &amp; B3 &amp;"', inPortuguese: '" &amp; A3 &amp;"', type: '" &amp; C3 &amp;"'}),"</f>
-        <v>(:Allergy {name: 'Soap', inPortuguese: 'Sabonete', type: 'Other'}),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>230</v>
-      </c>
-      <c r="B4" t="s">
-        <v>242</v>
-      </c>
-      <c r="C4" t="s">
-        <v>235</v>
-      </c>
-      <c r="D4" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Make up', inPortuguese: 'Maquiagem', type: 'Other'}),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>233</v>
-      </c>
-      <c r="B5" t="s">
-        <v>243</v>
-      </c>
-      <c r="C5" t="s">
-        <v>235</v>
-      </c>
-      <c r="D5" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'perfume', inPortuguese: 'Perfume', type: 'Other'}),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B6" t="s">
-        <v>244</v>
-      </c>
-      <c r="C6" t="s">
-        <v>235</v>
-      </c>
-      <c r="D6" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Latex Product', inPortuguese: 'Produto de Látex', type: 'Other'}),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>231</v>
-      </c>
-      <c r="B7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C7" t="s">
-        <v>235</v>
-      </c>
-      <c r="D7" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Bijou', inPortuguese: 'Bijuteria', type: 'Other'}),</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>192</v>
-      </c>
-      <c r="B8" t="s">
-        <v>246</v>
-      </c>
-      <c r="C8" t="s">
-        <v>235</v>
-      </c>
-      <c r="D8" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Ink', inPortuguese: 'Tinta', type: 'Other'}),</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>193</v>
-      </c>
-      <c r="B9" t="s">
-        <v>193</v>
-      </c>
-      <c r="C9" t="s">
-        <v>236</v>
-      </c>
-      <c r="D9" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Mosquito', inPortuguese: 'Mosquito', type: 'Insect'}),</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>194</v>
-      </c>
-      <c r="B10" t="s">
-        <v>247</v>
-      </c>
-      <c r="C10" t="s">
-        <v>236</v>
-      </c>
-      <c r="D10" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Bee', inPortuguese: 'Abelha', type: 'Insect'}),</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>195</v>
-      </c>
-      <c r="B11" t="s">
-        <v>248</v>
-      </c>
-      <c r="C11" t="s">
-        <v>236</v>
-      </c>
-      <c r="D11" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Flea', inPortuguese: 'Pulga', type: 'Insect'}),</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>196</v>
-      </c>
-      <c r="B12" t="s">
-        <v>249</v>
-      </c>
-      <c r="C12" t="s">
-        <v>239</v>
-      </c>
-      <c r="D12" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Cat', inPortuguese: 'Gato', type: 'Animal'}),</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>197</v>
-      </c>
-      <c r="B13" t="s">
-        <v>250</v>
-      </c>
-      <c r="C13" t="s">
-        <v>239</v>
-      </c>
-      <c r="D13" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Puppy', inPortuguese: 'Cachorro', type: 'Animal'}),</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>198</v>
-      </c>
-      <c r="B14" t="s">
-        <v>277</v>
-      </c>
-      <c r="C14" t="s">
-        <v>236</v>
-      </c>
-      <c r="D14" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Ant', inPortuguese: 'Formiga', type: 'Insect'}),</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>199</v>
-      </c>
-      <c r="B15" t="s">
-        <v>251</v>
-      </c>
-      <c r="C15" t="s">
-        <v>236</v>
-      </c>
-      <c r="D15" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Wasp', inPortuguese: 'Vespa', type: 'Insect'}),</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>200</v>
-      </c>
-      <c r="B16" t="s">
-        <v>252</v>
-      </c>
-      <c r="C16" t="s">
-        <v>236</v>
-      </c>
-      <c r="D16" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Tick', inPortuguese: 'Carrapato', type: 'Insect'}),</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>201</v>
-      </c>
-      <c r="B17" t="s">
-        <v>253</v>
-      </c>
-      <c r="C17" t="s">
-        <v>236</v>
-      </c>
-      <c r="D17" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Leggy', inPortuguese: 'Pernilongo', type: 'Insect'}),</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>202</v>
-      </c>
-      <c r="B18" t="s">
-        <v>254</v>
-      </c>
-      <c r="C18" t="s">
-        <v>236</v>
-      </c>
-      <c r="D18" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Rubber', inPortuguese: 'Borrachudo', type: 'Insect'}),</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>203</v>
-      </c>
-      <c r="B19" t="s">
-        <v>255</v>
-      </c>
-      <c r="C19" t="s">
-        <v>237</v>
-      </c>
-      <c r="D19" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Aspirin', inPortuguese: 'Aspirina', type: 'Drug'}),</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>204</v>
-      </c>
-      <c r="B20" t="s">
-        <v>256</v>
-      </c>
-      <c r="C20" t="s">
-        <v>237</v>
-      </c>
-      <c r="D20" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Dipyrone', inPortuguese: 'Dipirona', type: 'Drug'}),</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>205</v>
-      </c>
-      <c r="B21" t="s">
-        <v>205</v>
-      </c>
-      <c r="C21" t="s">
-        <v>237</v>
-      </c>
-      <c r="D21" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Paracetamol', inPortuguese: 'Paracetamol', type: 'Drug'}),</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>206</v>
-      </c>
-      <c r="B22" t="s">
-        <v>257</v>
-      </c>
-      <c r="C22" t="s">
-        <v>237</v>
-      </c>
-      <c r="D22" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Diclofenac', inPortuguese: 'Diclofenaco', type: 'Drug'}),</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>207</v>
-      </c>
-      <c r="B23" t="s">
-        <v>258</v>
-      </c>
-      <c r="C23" t="s">
-        <v>237</v>
-      </c>
-      <c r="D23" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Penicillin', inPortuguese: 'Penicilina', type: 'Drug'}),</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>208</v>
-      </c>
-      <c r="B24" t="s">
-        <v>208</v>
-      </c>
-      <c r="C24" t="s">
-        <v>237</v>
-      </c>
-      <c r="D24" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Sulfa', inPortuguese: 'Sulfa', type: 'Drug'}),</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>209</v>
-      </c>
-      <c r="B25" t="s">
-        <v>259</v>
-      </c>
-      <c r="C25" t="s">
-        <v>237</v>
-      </c>
-      <c r="D25" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Quinolone', inPortuguese: 'Quinolona', type: 'Drug'}),</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>210</v>
-      </c>
-      <c r="B26" t="s">
-        <v>260</v>
-      </c>
-      <c r="C26" t="s">
-        <v>237</v>
-      </c>
-      <c r="D26" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Erythromycin', inPortuguese: 'Eritromicina', type: 'Drug'}),</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>211</v>
-      </c>
-      <c r="B27" t="s">
-        <v>261</v>
-      </c>
-      <c r="C27" t="s">
-        <v>237</v>
-      </c>
-      <c r="D27" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Azithromycin', inPortuguese: 'Azitromicina', type: 'Drug'}),</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>212</v>
-      </c>
-      <c r="B28" t="s">
-        <v>262</v>
-      </c>
-      <c r="C28" t="s">
-        <v>237</v>
-      </c>
-      <c r="D28" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Iodinated Contrast', inPortuguese: 'Contraste Iodado', type: 'Drug'}),</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>213</v>
-      </c>
-      <c r="B29" t="s">
-        <v>263</v>
-      </c>
-      <c r="C29" t="s">
-        <v>236</v>
-      </c>
-      <c r="D29" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Mite', inPortuguese: 'Ácaro', type: 'Insect'}),</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>214</v>
-      </c>
-      <c r="B30" t="s">
-        <v>264</v>
-      </c>
-      <c r="C30" t="s">
-        <v>235</v>
-      </c>
-      <c r="D30" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Dust', inPortuguese: 'Poeira', type: 'Other'}),</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>215</v>
-      </c>
-      <c r="B31" t="s">
-        <v>265</v>
-      </c>
-      <c r="C31" t="s">
-        <v>235</v>
-      </c>
-      <c r="D31" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Mold', inPortuguese: 'Mofo', type: 'Other'}),</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>216</v>
-      </c>
-      <c r="B32" t="s">
-        <v>266</v>
-      </c>
-      <c r="C32" t="s">
-        <v>235</v>
-      </c>
-      <c r="D32" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Pollen', inPortuguese: 'Pólen', type: 'Other'}),</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>217</v>
-      </c>
-      <c r="B33" t="s">
-        <v>267</v>
-      </c>
-      <c r="C33" t="s">
-        <v>235</v>
-      </c>
-      <c r="D33" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Smoke', inPortuguese: 'Fumaça', type: 'Other'}),</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>218</v>
-      </c>
-      <c r="B34" t="s">
-        <v>268</v>
-      </c>
-      <c r="C34" t="s">
-        <v>235</v>
-      </c>
-      <c r="D34" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Pollution', inPortuguese: 'Poluição', type: 'Other'}),</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>219</v>
-      </c>
-      <c r="B35" t="s">
-        <v>269</v>
-      </c>
-      <c r="C35" t="s">
-        <v>238</v>
-      </c>
-      <c r="D35" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Milk', inPortuguese: 'Leite', type: 'Food'}),</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>220</v>
-      </c>
-      <c r="B36" t="s">
-        <v>270</v>
-      </c>
-      <c r="C36" t="s">
-        <v>238</v>
-      </c>
-      <c r="D36" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Egg', inPortuguese: 'Ovo', type: 'Food'}),</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>221</v>
-      </c>
-      <c r="B37" t="s">
-        <v>271</v>
-      </c>
-      <c r="C37" t="s">
-        <v>238</v>
-      </c>
-      <c r="D37" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Wheat', inPortuguese: 'Trigo', type: 'Food'}),</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>222</v>
-      </c>
-      <c r="B38" t="s">
-        <v>272</v>
-      </c>
-      <c r="C38" t="s">
-        <v>238</v>
-      </c>
-      <c r="D38" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Peanut', inPortuguese: 'Amendoim', type: 'Food'}),</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>223</v>
-      </c>
-      <c r="B39" t="s">
-        <v>273</v>
-      </c>
-      <c r="C39" t="s">
-        <v>238</v>
-      </c>
-      <c r="D39" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Seafood', inPortuguese: 'Frutos do Mar', type: 'Food'}),</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>224</v>
-      </c>
-      <c r="B40" t="s">
-        <v>278</v>
-      </c>
-      <c r="C40" t="s">
-        <v>238</v>
-      </c>
-      <c r="D40" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Dry Fruits', inPortuguese: 'Frutas Secas', type: 'Food'}),</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>225</v>
-      </c>
-      <c r="B41" t="s">
-        <v>274</v>
-      </c>
-      <c r="C41" t="s">
-        <v>238</v>
-      </c>
-      <c r="D41" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Soy', inPortuguese: 'Soja', type: 'Food'}),</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>226</v>
-      </c>
-      <c r="B42" t="s">
-        <v>275</v>
-      </c>
-      <c r="C42" t="s">
-        <v>238</v>
-      </c>
-      <c r="D42" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Fish', inPortuguese: 'Peixe', type: 'Food'}),</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>279</v>
-      </c>
-      <c r="B43" t="s">
-        <v>288</v>
-      </c>
-      <c r="C43" t="s">
-        <v>238</v>
-      </c>
-      <c r="D43" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Crustacean', inPortuguese: 'Crustáceo', type: 'Food'}),</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>280</v>
-      </c>
-      <c r="B44" t="s">
-        <v>287</v>
-      </c>
-      <c r="C44" t="s">
-        <v>238</v>
-      </c>
-      <c r="D44" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Mollusk', inPortuguese: 'Molusco', type: 'Food'}),</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>227</v>
-      </c>
-      <c r="B45" t="s">
-        <v>276</v>
-      </c>
-      <c r="C45" t="s">
-        <v>238</v>
-      </c>
-      <c r="D45" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Allergy {name: 'Gluten', inPortuguese: 'Glúten', type: 'Food'}),</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>281</v>
-      </c>
-      <c r="B46" t="s">
-        <v>283</v>
-      </c>
-      <c r="C46" t="s">
-        <v>238</v>
-      </c>
-      <c r="D46" t="str">
-        <f t="shared" ref="D46:D48" si="1">"(:Allergy {name: '" &amp; B46 &amp;"', inPortuguese: '" &amp; A46 &amp;"', type: '" &amp; C46 &amp;"'}),"</f>
-        <v>(:Allergy {name: 'Shrimp', inPortuguese: 'Camarão', type: 'Food'}),</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>282</v>
-      </c>
-      <c r="B47" t="s">
-        <v>284</v>
-      </c>
-      <c r="C47" t="s">
-        <v>238</v>
-      </c>
-      <c r="D47" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Allergy {name: 'Squid', inPortuguese: 'Lula', type: 'Food'}),</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>285</v>
-      </c>
-      <c r="B48" t="s">
-        <v>286</v>
-      </c>
-      <c r="C48" t="s">
-        <v>238</v>
-      </c>
-      <c r="D48" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Allergy {name: 'Pufferfish', inPortuguese: 'Baiacu', type: 'Food'}),</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>289</v>
-      </c>
-      <c r="B49" t="s">
-        <v>289</v>
-      </c>
-      <c r="C49" t="s">
-        <v>238</v>
-      </c>
-      <c r="D49" t="str">
-        <f t="shared" ref="D49:D50" si="2">"(:Allergy {name: '" &amp; B49 &amp;"', inPortuguese: '" &amp; A49 &amp;"', type: '" &amp; C49 &amp;"'}),"</f>
-        <v>(:Allergy {name: 'Chocolate', inPortuguese: 'Chocolate', type: 'Food'}),</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>290</v>
-      </c>
-      <c r="B50" t="s">
-        <v>290</v>
-      </c>
-      <c r="C50" t="s">
-        <v>238</v>
-      </c>
-      <c r="D50" t="str">
-        <f t="shared" si="2"/>
-        <v>(:Allergy {name: 'Caviar', inPortuguese: 'Caviar', type: 'Food'}),</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FBDA324-BA52-4553-9EA4-1F1EB8000A70}">
-  <dimension ref="A1:D50"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="2" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" customWidth="1"/>
-    <col min="4" max="4" width="48.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>234</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="str">
-        <f>allergy!A2</f>
-        <v>Creme</v>
-      </c>
-      <c r="B2" t="str">
-        <f>allergy!B2</f>
-        <v>Cream</v>
-      </c>
-      <c r="C2" t="str">
-        <f>allergy!C2</f>
-        <v>Other</v>
-      </c>
-      <c r="D2" t="str">
-        <f>"(:Intolerance {name: '" &amp; B2 &amp;"', inPortuguese: '" &amp; A2 &amp;"', type: '" &amp; C2 &amp;"'}),"</f>
-        <v>(:Intolerance {name: 'Cream', inPortuguese: 'Creme', type: 'Other'}),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="str">
-        <f>allergy!A3</f>
-        <v>Sabonete</v>
-      </c>
-      <c r="B3" t="str">
-        <f>allergy!B3</f>
-        <v>Soap</v>
-      </c>
-      <c r="C3" t="str">
-        <f>allergy!C3</f>
-        <v>Other</v>
-      </c>
-      <c r="D3" t="str">
-        <f t="shared" ref="D3:D45" si="0">"(:Intolerance {name: '" &amp; B3 &amp;"', inPortuguese: '" &amp; A3 &amp;"', type: '" &amp; C3 &amp;"'}),"</f>
-        <v>(:Intolerance {name: 'Soap', inPortuguese: 'Sabonete', type: 'Other'}),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="str">
-        <f>allergy!A4</f>
-        <v>Maquiagem</v>
-      </c>
-      <c r="B4" t="str">
-        <f>allergy!B4</f>
-        <v>Make up</v>
-      </c>
-      <c r="C4" t="str">
-        <f>allergy!C4</f>
-        <v>Other</v>
-      </c>
-      <c r="D4" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Make up', inPortuguese: 'Maquiagem', type: 'Other'}),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="str">
-        <f>allergy!A5</f>
-        <v>Perfume</v>
-      </c>
-      <c r="B5" t="str">
-        <f>allergy!B5</f>
-        <v>perfume</v>
-      </c>
-      <c r="C5" t="str">
-        <f>allergy!C5</f>
-        <v>Other</v>
-      </c>
-      <c r="D5" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'perfume', inPortuguese: 'Perfume', type: 'Other'}),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="str">
-        <f>allergy!A6</f>
-        <v>Produto de Látex</v>
-      </c>
-      <c r="B6" t="str">
-        <f>allergy!B6</f>
-        <v>Latex Product</v>
-      </c>
-      <c r="C6" t="str">
-        <f>allergy!C6</f>
-        <v>Other</v>
-      </c>
-      <c r="D6" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Latex Product', inPortuguese: 'Produto de Látex', type: 'Other'}),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="str">
-        <f>allergy!A7</f>
-        <v>Bijuteria</v>
-      </c>
-      <c r="B7" t="str">
-        <f>allergy!B7</f>
-        <v>Bijou</v>
-      </c>
-      <c r="C7" t="str">
-        <f>allergy!C7</f>
-        <v>Other</v>
-      </c>
-      <c r="D7" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Bijou', inPortuguese: 'Bijuteria', type: 'Other'}),</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="str">
-        <f>allergy!A8</f>
-        <v>Tinta</v>
-      </c>
-      <c r="B8" t="str">
-        <f>allergy!B8</f>
-        <v>Ink</v>
-      </c>
-      <c r="C8" t="str">
-        <f>allergy!C8</f>
-        <v>Other</v>
-      </c>
-      <c r="D8" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Ink', inPortuguese: 'Tinta', type: 'Other'}),</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="str">
-        <f>allergy!A9</f>
-        <v>Mosquito</v>
-      </c>
-      <c r="B9" t="str">
-        <f>allergy!B9</f>
-        <v>Mosquito</v>
-      </c>
-      <c r="C9" t="str">
-        <f>allergy!C9</f>
-        <v>Insect</v>
-      </c>
-      <c r="D9" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Mosquito', inPortuguese: 'Mosquito', type: 'Insect'}),</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="str">
-        <f>allergy!A10</f>
-        <v>Abelha</v>
-      </c>
-      <c r="B10" t="str">
-        <f>allergy!B10</f>
-        <v>Bee</v>
-      </c>
-      <c r="C10" t="str">
-        <f>allergy!C10</f>
-        <v>Insect</v>
-      </c>
-      <c r="D10" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Bee', inPortuguese: 'Abelha', type: 'Insect'}),</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="str">
-        <f>allergy!A11</f>
-        <v>Pulga</v>
-      </c>
-      <c r="B11" t="str">
-        <f>allergy!B11</f>
-        <v>Flea</v>
-      </c>
-      <c r="C11" t="str">
-        <f>allergy!C11</f>
-        <v>Insect</v>
-      </c>
-      <c r="D11" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Flea', inPortuguese: 'Pulga', type: 'Insect'}),</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="str">
-        <f>allergy!A12</f>
-        <v>Gato</v>
-      </c>
-      <c r="B12" t="str">
-        <f>allergy!B12</f>
-        <v>Cat</v>
-      </c>
-      <c r="C12" t="str">
-        <f>allergy!C12</f>
-        <v>Animal</v>
-      </c>
-      <c r="D12" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Cat', inPortuguese: 'Gato', type: 'Animal'}),</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="str">
-        <f>allergy!A13</f>
-        <v>Cachorro</v>
-      </c>
-      <c r="B13" t="str">
-        <f>allergy!B13</f>
-        <v>Puppy</v>
-      </c>
-      <c r="C13" t="str">
-        <f>allergy!C13</f>
-        <v>Animal</v>
-      </c>
-      <c r="D13" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Puppy', inPortuguese: 'Cachorro', type: 'Animal'}),</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="str">
-        <f>allergy!A14</f>
-        <v>Formiga</v>
-      </c>
-      <c r="B14" t="str">
-        <f>allergy!B14</f>
-        <v>Ant</v>
-      </c>
-      <c r="C14" t="str">
-        <f>allergy!C14</f>
-        <v>Insect</v>
-      </c>
-      <c r="D14" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Ant', inPortuguese: 'Formiga', type: 'Insect'}),</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="str">
-        <f>allergy!A15</f>
-        <v>Vespa</v>
-      </c>
-      <c r="B15" t="str">
-        <f>allergy!B15</f>
-        <v>Wasp</v>
-      </c>
-      <c r="C15" t="str">
-        <f>allergy!C15</f>
-        <v>Insect</v>
-      </c>
-      <c r="D15" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Wasp', inPortuguese: 'Vespa', type: 'Insect'}),</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="str">
-        <f>allergy!A16</f>
-        <v>Carrapato</v>
-      </c>
-      <c r="B16" t="str">
-        <f>allergy!B16</f>
-        <v>Tick</v>
-      </c>
-      <c r="C16" t="str">
-        <f>allergy!C16</f>
-        <v>Insect</v>
-      </c>
-      <c r="D16" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Tick', inPortuguese: 'Carrapato', type: 'Insect'}),</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="str">
-        <f>allergy!A17</f>
-        <v>Pernilongo</v>
-      </c>
-      <c r="B17" t="str">
-        <f>allergy!B17</f>
-        <v>Leggy</v>
-      </c>
-      <c r="C17" t="str">
-        <f>allergy!C17</f>
-        <v>Insect</v>
-      </c>
-      <c r="D17" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Leggy', inPortuguese: 'Pernilongo', type: 'Insect'}),</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="str">
-        <f>allergy!A18</f>
-        <v>Borrachudo</v>
-      </c>
-      <c r="B18" t="str">
-        <f>allergy!B18</f>
-        <v>Rubber</v>
-      </c>
-      <c r="C18" t="str">
-        <f>allergy!C18</f>
-        <v>Insect</v>
-      </c>
-      <c r="D18" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Rubber', inPortuguese: 'Borrachudo', type: 'Insect'}),</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="str">
-        <f>allergy!A19</f>
-        <v>Aspirina</v>
-      </c>
-      <c r="B19" t="str">
-        <f>allergy!B19</f>
-        <v>Aspirin</v>
-      </c>
-      <c r="C19" t="str">
-        <f>allergy!C19</f>
-        <v>Drug</v>
-      </c>
-      <c r="D19" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Aspirin', inPortuguese: 'Aspirina', type: 'Drug'}),</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="str">
-        <f>allergy!A20</f>
-        <v>Dipirona</v>
-      </c>
-      <c r="B20" t="str">
-        <f>allergy!B20</f>
-        <v>Dipyrone</v>
-      </c>
-      <c r="C20" t="str">
-        <f>allergy!C20</f>
-        <v>Drug</v>
-      </c>
-      <c r="D20" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Dipyrone', inPortuguese: 'Dipirona', type: 'Drug'}),</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="str">
-        <f>allergy!A21</f>
-        <v>Paracetamol</v>
-      </c>
-      <c r="B21" t="str">
-        <f>allergy!B21</f>
-        <v>Paracetamol</v>
-      </c>
-      <c r="C21" t="str">
-        <f>allergy!C21</f>
-        <v>Drug</v>
-      </c>
-      <c r="D21" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Paracetamol', inPortuguese: 'Paracetamol', type: 'Drug'}),</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="str">
-        <f>allergy!A22</f>
-        <v>Diclofenaco</v>
-      </c>
-      <c r="B22" t="str">
-        <f>allergy!B22</f>
-        <v>Diclofenac</v>
-      </c>
-      <c r="C22" t="str">
-        <f>allergy!C22</f>
-        <v>Drug</v>
-      </c>
-      <c r="D22" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Diclofenac', inPortuguese: 'Diclofenaco', type: 'Drug'}),</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" t="str">
-        <f>allergy!A23</f>
-        <v>Penicilina</v>
-      </c>
-      <c r="B23" t="str">
-        <f>allergy!B23</f>
-        <v>Penicillin</v>
-      </c>
-      <c r="C23" t="str">
-        <f>allergy!C23</f>
-        <v>Drug</v>
-      </c>
-      <c r="D23" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Penicillin', inPortuguese: 'Penicilina', type: 'Drug'}),</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="str">
-        <f>allergy!A24</f>
-        <v>Sulfa</v>
-      </c>
-      <c r="B24" t="str">
-        <f>allergy!B24</f>
-        <v>Sulfa</v>
-      </c>
-      <c r="C24" t="str">
-        <f>allergy!C24</f>
-        <v>Drug</v>
-      </c>
-      <c r="D24" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Sulfa', inPortuguese: 'Sulfa', type: 'Drug'}),</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="str">
-        <f>allergy!A25</f>
-        <v>Quinolona</v>
-      </c>
-      <c r="B25" t="str">
-        <f>allergy!B25</f>
-        <v>Quinolone</v>
-      </c>
-      <c r="C25" t="str">
-        <f>allergy!C25</f>
-        <v>Drug</v>
-      </c>
-      <c r="D25" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Quinolone', inPortuguese: 'Quinolona', type: 'Drug'}),</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" t="str">
-        <f>allergy!A26</f>
-        <v>Eritromicina</v>
-      </c>
-      <c r="B26" t="str">
-        <f>allergy!B26</f>
-        <v>Erythromycin</v>
-      </c>
-      <c r="C26" t="str">
-        <f>allergy!C26</f>
-        <v>Drug</v>
-      </c>
-      <c r="D26" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Erythromycin', inPortuguese: 'Eritromicina', type: 'Drug'}),</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" t="str">
-        <f>allergy!A27</f>
-        <v>Azitromicina</v>
-      </c>
-      <c r="B27" t="str">
-        <f>allergy!B27</f>
-        <v>Azithromycin</v>
-      </c>
-      <c r="C27" t="str">
-        <f>allergy!C27</f>
-        <v>Drug</v>
-      </c>
-      <c r="D27" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Azithromycin', inPortuguese: 'Azitromicina', type: 'Drug'}),</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" t="str">
-        <f>allergy!A28</f>
-        <v>Contraste Iodado</v>
-      </c>
-      <c r="B28" t="str">
-        <f>allergy!B28</f>
-        <v>Iodinated Contrast</v>
-      </c>
-      <c r="C28" t="str">
-        <f>allergy!C28</f>
-        <v>Drug</v>
-      </c>
-      <c r="D28" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Iodinated Contrast', inPortuguese: 'Contraste Iodado', type: 'Drug'}),</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" t="str">
-        <f>allergy!A29</f>
-        <v>Ácaro</v>
-      </c>
-      <c r="B29" t="str">
-        <f>allergy!B29</f>
-        <v>Mite</v>
-      </c>
-      <c r="C29" t="str">
-        <f>allergy!C29</f>
-        <v>Insect</v>
-      </c>
-      <c r="D29" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Mite', inPortuguese: 'Ácaro', type: 'Insect'}),</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" t="str">
-        <f>allergy!A30</f>
-        <v>Poeira</v>
-      </c>
-      <c r="B30" t="str">
-        <f>allergy!B30</f>
-        <v>Dust</v>
-      </c>
-      <c r="C30" t="str">
-        <f>allergy!C30</f>
-        <v>Other</v>
-      </c>
-      <c r="D30" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Dust', inPortuguese: 'Poeira', type: 'Other'}),</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" t="str">
-        <f>allergy!A31</f>
-        <v>Mofo</v>
-      </c>
-      <c r="B31" t="str">
-        <f>allergy!B31</f>
-        <v>Mold</v>
-      </c>
-      <c r="C31" t="str">
-        <f>allergy!C31</f>
-        <v>Other</v>
-      </c>
-      <c r="D31" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Mold', inPortuguese: 'Mofo', type: 'Other'}),</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" t="str">
-        <f>allergy!A32</f>
-        <v>Pólen</v>
-      </c>
-      <c r="B32" t="str">
-        <f>allergy!B32</f>
-        <v>Pollen</v>
-      </c>
-      <c r="C32" t="str">
-        <f>allergy!C32</f>
-        <v>Other</v>
-      </c>
-      <c r="D32" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Pollen', inPortuguese: 'Pólen', type: 'Other'}),</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" t="str">
-        <f>allergy!A33</f>
-        <v>Fumaça</v>
-      </c>
-      <c r="B33" t="str">
-        <f>allergy!B33</f>
-        <v>Smoke</v>
-      </c>
-      <c r="C33" t="str">
-        <f>allergy!C33</f>
-        <v>Other</v>
-      </c>
-      <c r="D33" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Smoke', inPortuguese: 'Fumaça', type: 'Other'}),</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" t="str">
-        <f>allergy!A34</f>
-        <v>Poluição</v>
-      </c>
-      <c r="B34" t="str">
-        <f>allergy!B34</f>
-        <v>Pollution</v>
-      </c>
-      <c r="C34" t="str">
-        <f>allergy!C34</f>
-        <v>Other</v>
-      </c>
-      <c r="D34" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Pollution', inPortuguese: 'Poluição', type: 'Other'}),</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" t="str">
-        <f>allergy!A35</f>
-        <v>Leite</v>
-      </c>
-      <c r="B35" t="str">
-        <f>allergy!B35</f>
-        <v>Milk</v>
-      </c>
-      <c r="C35" t="str">
-        <f>allergy!C35</f>
-        <v>Food</v>
-      </c>
-      <c r="D35" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Milk', inPortuguese: 'Leite', type: 'Food'}),</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" t="str">
-        <f>allergy!A36</f>
-        <v>Ovo</v>
-      </c>
-      <c r="B36" t="str">
-        <f>allergy!B36</f>
-        <v>Egg</v>
-      </c>
-      <c r="C36" t="str">
-        <f>allergy!C36</f>
-        <v>Food</v>
-      </c>
-      <c r="D36" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Egg', inPortuguese: 'Ovo', type: 'Food'}),</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" t="str">
-        <f>allergy!A37</f>
-        <v>Trigo</v>
-      </c>
-      <c r="B37" t="str">
-        <f>allergy!B37</f>
-        <v>Wheat</v>
-      </c>
-      <c r="C37" t="str">
-        <f>allergy!C37</f>
-        <v>Food</v>
-      </c>
-      <c r="D37" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Wheat', inPortuguese: 'Trigo', type: 'Food'}),</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" t="str">
-        <f>allergy!A38</f>
-        <v>Amendoim</v>
-      </c>
-      <c r="B38" t="str">
-        <f>allergy!B38</f>
-        <v>Peanut</v>
-      </c>
-      <c r="C38" t="str">
-        <f>allergy!C38</f>
-        <v>Food</v>
-      </c>
-      <c r="D38" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Peanut', inPortuguese: 'Amendoim', type: 'Food'}),</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" t="str">
-        <f>allergy!A39</f>
-        <v>Frutos do Mar</v>
-      </c>
-      <c r="B39" t="str">
-        <f>allergy!B39</f>
-        <v>Seafood</v>
-      </c>
-      <c r="C39" t="str">
-        <f>allergy!C39</f>
-        <v>Food</v>
-      </c>
-      <c r="D39" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Seafood', inPortuguese: 'Frutos do Mar', type: 'Food'}),</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" t="str">
-        <f>allergy!A40</f>
-        <v>Frutas Secas</v>
-      </c>
-      <c r="B40" t="str">
-        <f>allergy!B40</f>
-        <v>Dry Fruits</v>
-      </c>
-      <c r="C40" t="str">
-        <f>allergy!C40</f>
-        <v>Food</v>
-      </c>
-      <c r="D40" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Dry Fruits', inPortuguese: 'Frutas Secas', type: 'Food'}),</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" t="str">
-        <f>allergy!A41</f>
-        <v>Soja</v>
-      </c>
-      <c r="B41" t="str">
-        <f>allergy!B41</f>
-        <v>Soy</v>
-      </c>
-      <c r="C41" t="str">
-        <f>allergy!C41</f>
-        <v>Food</v>
-      </c>
-      <c r="D41" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Soy', inPortuguese: 'Soja', type: 'Food'}),</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" t="str">
-        <f>allergy!A42</f>
-        <v>Peixe</v>
-      </c>
-      <c r="B42" t="str">
-        <f>allergy!B42</f>
-        <v>Fish</v>
-      </c>
-      <c r="C42" t="str">
-        <f>allergy!C42</f>
-        <v>Food</v>
-      </c>
-      <c r="D42" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Fish', inPortuguese: 'Peixe', type: 'Food'}),</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" t="str">
-        <f>allergy!A43</f>
-        <v>Crustáceo</v>
-      </c>
-      <c r="B43" t="str">
-        <f>allergy!B43</f>
-        <v>Crustacean</v>
-      </c>
-      <c r="C43" t="str">
-        <f>allergy!C43</f>
-        <v>Food</v>
-      </c>
-      <c r="D43" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Crustacean', inPortuguese: 'Crustáceo', type: 'Food'}),</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" t="str">
-        <f>allergy!A44</f>
-        <v>Molusco</v>
-      </c>
-      <c r="B44" t="str">
-        <f>allergy!B44</f>
-        <v>Mollusk</v>
-      </c>
-      <c r="C44" t="str">
-        <f>allergy!C44</f>
-        <v>Food</v>
-      </c>
-      <c r="D44" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Mollusk', inPortuguese: 'Molusco', type: 'Food'}),</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" t="str">
-        <f>allergy!A45</f>
-        <v>Glúten</v>
-      </c>
-      <c r="B45" t="str">
-        <f>allergy!B45</f>
-        <v>Gluten</v>
-      </c>
-      <c r="C45" t="str">
-        <f>allergy!C45</f>
-        <v>Food</v>
-      </c>
-      <c r="D45" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Intolerance {name: 'Gluten', inPortuguese: 'Glúten', type: 'Food'}),</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" t="str">
-        <f>allergy!A46</f>
-        <v>Camarão</v>
-      </c>
-      <c r="B46" t="str">
-        <f>allergy!B46</f>
-        <v>Shrimp</v>
-      </c>
-      <c r="C46" t="str">
-        <f>allergy!C46</f>
-        <v>Food</v>
-      </c>
-      <c r="D46" t="str">
-        <f t="shared" ref="D46:D48" si="1">"(:Intolerance {name: '" &amp; B46 &amp;"', inPortuguese: '" &amp; A46 &amp;"', type: '" &amp; C46 &amp;"'}),"</f>
-        <v>(:Intolerance {name: 'Shrimp', inPortuguese: 'Camarão', type: 'Food'}),</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" t="str">
-        <f>allergy!A47</f>
-        <v>Lula</v>
-      </c>
-      <c r="B47" t="str">
-        <f>allergy!B47</f>
-        <v>Squid</v>
-      </c>
-      <c r="C47" t="str">
-        <f>allergy!C47</f>
-        <v>Food</v>
-      </c>
-      <c r="D47" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Intolerance {name: 'Squid', inPortuguese: 'Lula', type: 'Food'}),</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" t="str">
-        <f>allergy!A48</f>
-        <v>Baiacu</v>
-      </c>
-      <c r="B48" t="str">
-        <f>allergy!B48</f>
-        <v>Pufferfish</v>
-      </c>
-      <c r="C48" t="str">
-        <f>allergy!C48</f>
-        <v>Food</v>
-      </c>
-      <c r="D48" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Intolerance {name: 'Pufferfish', inPortuguese: 'Baiacu', type: 'Food'}),</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" t="str">
-        <f>allergy!A49</f>
-        <v>Chocolate</v>
-      </c>
-      <c r="B49" t="str">
-        <f>allergy!B49</f>
-        <v>Chocolate</v>
-      </c>
-      <c r="C49" t="str">
-        <f>allergy!C49</f>
-        <v>Food</v>
-      </c>
-      <c r="D49" t="str">
-        <f t="shared" ref="D49:D50" si="2">"(:Intolerance {name: '" &amp; B49 &amp;"', inPortuguese: '" &amp; A49 &amp;"', type: '" &amp; C49 &amp;"'}),"</f>
-        <v>(:Intolerance {name: 'Chocolate', inPortuguese: 'Chocolate', type: 'Food'}),</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" t="str">
-        <f>allergy!A50</f>
-        <v>Caviar</v>
-      </c>
-      <c r="B50" t="str">
-        <f>allergy!B50</f>
-        <v>Caviar</v>
-      </c>
-      <c r="C50" t="str">
-        <f>allergy!C50</f>
-        <v>Food</v>
-      </c>
-      <c r="D50" t="str">
-        <f t="shared" si="2"/>
-        <v>(:Intolerance {name: 'Caviar', inPortuguese: 'Caviar', type: 'Food'}),</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
@@ -5496,7 +5410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{391AE3A0-7DB7-4C1A-B882-6DBA4383A0D7}">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="O1" sqref="O1:O2"/>
     </sheetView>
   </sheetViews>
@@ -7106,40 +7020,4 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF7AE525-CAA1-4E99-A7E7-A745DD507DF7}">
-  <sheetPr>
-    <tabColor rgb="FF002060"/>
-  </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="3" max="3" width="88.88671875" customWidth="1"/>
-    <col min="4" max="4" width="53.5546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="C2" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>371</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
refactor: :recycle: refactoring Disease diagnostic tasks
</commit_message>
<xml_diff>
--- a/poc.xlsx
+++ b/poc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\renatospaka\dev\heykid\draft\poc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2FAF7DE-B35F-4274-A185-FDAA53B52F2D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{954F8497-8AFA-43A5-BE7A-27382973D72D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="complication" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="vaccine dose" sheetId="7" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">disease!$A$1:$D$74</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">disease!$A$1:$D$80</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'vaccine dose'!$A$1:$F$55</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="369">
   <si>
     <t>Tipos</t>
   </si>
@@ -444,9 +444,6 @@
   </si>
   <si>
     <t>Síndrome do Intestino Irritável</t>
-  </si>
-  <si>
-    <t>Obstipação</t>
   </si>
   <si>
     <t>Dyslipidemia</t>
@@ -1501,10 +1498,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C2" t="str">
         <f>"(:Complication {uuid: apoc.create.uuid(), name: '" &amp; B2 &amp;"', inPortuguese: '" &amp; A2 &amp;"'}),"</f>
@@ -1513,10 +1510,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C18" si="0">"(:Complication {uuid: apoc.create.uuid(), name: '" &amp; B3 &amp;"', inPortuguese: '" &amp; A3 &amp;"'}),"</f>
@@ -1525,10 +1522,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
@@ -1537,10 +1534,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
@@ -1549,10 +1546,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -1561,10 +1558,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B7" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -1573,10 +1570,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -1585,10 +1582,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -1597,10 +1594,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B10" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -1609,10 +1606,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
@@ -1621,10 +1618,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B12" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
@@ -1633,10 +1630,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B13" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
@@ -1645,10 +1642,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B14" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
@@ -1657,10 +1654,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B15" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
@@ -1669,10 +1666,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B16" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
@@ -1681,10 +1678,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B17" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
@@ -1693,10 +1690,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B18" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
@@ -1710,10 +1707,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16822055-6D7C-4562-869B-B3AD28812FB9}">
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D81"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1731,7 +1728,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1757,7 +1754,7 @@
         <v>89</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D66" si="0">"(:Disease {uuid: apoc.create.uuid(), name: '" &amp; B3 &amp;"', inPortuguese: '" &amp; A3 &amp;"'}),"</f>
+        <f t="shared" ref="D3:D65" si="0">"(:Disease {uuid: apoc.create.uuid(), name: '" &amp; B3 &amp;"', inPortuguese: '" &amp; A3 &amp;"'}),"</f>
         <v>(:Disease {uuid: apoc.create.uuid(), name: 'Migraine', inPortuguese: 'Enxaqueca'}),</v>
       </c>
     </row>
@@ -1967,10 +1964,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
@@ -2054,7 +2051,7 @@
         <v>66</v>
       </c>
       <c r="B28" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
@@ -2078,7 +2075,7 @@
         <v>68</v>
       </c>
       <c r="B30" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
@@ -2183,10 +2180,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B39" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D39" t="str">
         <f t="shared" si="0"/>
@@ -2195,7 +2192,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B40" t="s">
         <v>118</v>
@@ -2219,10 +2216,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D42" t="str">
         <f t="shared" si="0"/>
@@ -2231,10 +2228,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B43" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D43" t="str">
         <f t="shared" si="0"/>
@@ -2267,7 +2264,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B46" t="s">
         <v>122</v>
@@ -2339,10 +2336,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B52" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D52" t="str">
         <f t="shared" si="0"/>
@@ -2378,7 +2375,7 @@
         <v>87</v>
       </c>
       <c r="B55" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D55" t="str">
         <f t="shared" si="0"/>
@@ -2390,7 +2387,7 @@
         <v>128</v>
       </c>
       <c r="B56" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D56" t="str">
         <f t="shared" si="0"/>
@@ -2399,10 +2396,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B57" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D57" t="str">
         <f t="shared" si="0"/>
@@ -2414,7 +2411,7 @@
         <v>129</v>
       </c>
       <c r="B58" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D58" t="str">
         <f t="shared" si="0"/>
@@ -2423,10 +2420,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B59" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D59" t="str">
         <f t="shared" si="0"/>
@@ -2438,7 +2435,7 @@
         <v>130</v>
       </c>
       <c r="B60" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D60" t="str">
         <f t="shared" si="0"/>
@@ -2450,7 +2447,7 @@
         <v>131</v>
       </c>
       <c r="B61" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D61" t="str">
         <f t="shared" si="0"/>
@@ -2462,7 +2459,7 @@
         <v>132</v>
       </c>
       <c r="B62" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D62" t="str">
         <f t="shared" si="0"/>
@@ -2471,10 +2468,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B63" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D63" t="str">
         <f t="shared" si="0"/>
@@ -2483,14 +2480,14 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>133</v>
+        <v>155</v>
       </c>
       <c r="B64" t="s">
-        <v>122</v>
+        <v>163</v>
       </c>
       <c r="D64" t="str">
         <f t="shared" si="0"/>
-        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Constipation', inPortuguese: 'Obstipação'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Arthrosis', inPortuguese: 'Artrose'}),</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -2502,7 +2499,7 @@
       </c>
       <c r="D65" t="str">
         <f t="shared" si="0"/>
-        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Arthrosis', inPortuguese: 'Artrose'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Flat Feet', inPortuguese: 'Pé Chato'}),</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -2513,8 +2510,8 @@
         <v>165</v>
       </c>
       <c r="D66" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Flat Feet', inPortuguese: 'Pé Chato'}),</v>
+        <f t="shared" ref="D66:D80" si="1">"(:Disease {uuid: apoc.create.uuid(), name: '" &amp; B66 &amp;"', inPortuguese: '" &amp; A66 &amp;"'}),"</f>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Tendonitis', inPortuguese: 'Tendinite'}),</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -2525,8 +2522,8 @@
         <v>166</v>
       </c>
       <c r="D67" t="str">
-        <f t="shared" ref="D67:D81" si="1">"(:Disease {uuid: apoc.create.uuid(), name: '" &amp; B67 &amp;"', inPortuguese: '" &amp; A67 &amp;"'}),"</f>
-        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Tendonitis', inPortuguese: 'Tendinite'}),</v>
+        <f t="shared" si="1"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Bursitis', inPortuguese: 'Bursite'}),</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -2538,7 +2535,7 @@
       </c>
       <c r="D68" t="str">
         <f t="shared" si="1"/>
-        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Bursitis', inPortuguese: 'Bursite'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Ligament Rupture', inPortuguese: 'Ruptura de Ligamento'}),</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -2550,7 +2547,7 @@
       </c>
       <c r="D69" t="str">
         <f t="shared" si="1"/>
-        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Ligament Rupture', inPortuguese: 'Ruptura de Ligamento'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Backache', inPortuguese: 'Lombalgia'}),</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -2562,7 +2559,7 @@
       </c>
       <c r="D70" t="str">
         <f t="shared" si="1"/>
-        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Backache', inPortuguese: 'Lombalgia'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Plantar Fasciitis', inPortuguese: 'Fascite Plantar'}),</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -2574,19 +2571,19 @@
       </c>
       <c r="D71" t="str">
         <f t="shared" si="1"/>
-        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Plantar Fasciitis', inPortuguese: 'Fascite Plantar'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Osteoporosis', inPortuguese: 'Osteoporose'}),</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="B72" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="D72" t="str">
         <f t="shared" si="1"/>
-        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Osteoporosis', inPortuguese: 'Osteoporose'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Pulmonary Emphysema', inPortuguese: 'Enfisema Pulmonar'}),</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -2598,7 +2595,7 @@
       </c>
       <c r="D73" t="str">
         <f t="shared" si="1"/>
-        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Pulmonary Emphysema', inPortuguese: 'Enfisema Pulmonar'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Bronchitis', inPortuguese: 'Bronquite'}),</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -2610,7 +2607,7 @@
       </c>
       <c r="D74" t="str">
         <f t="shared" si="1"/>
-        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Bronchitis', inPortuguese: 'Bronquite'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Tuberculosis', inPortuguese: 'Tuberculose'}),</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -2622,7 +2619,7 @@
       </c>
       <c r="D75" t="str">
         <f t="shared" si="1"/>
-        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Tuberculosis', inPortuguese: 'Tuberculose'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Pharyngitis', inPortuguese: 'Faringite'}),</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
@@ -2630,23 +2627,23 @@
         <v>178</v>
       </c>
       <c r="B76" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D76" t="str">
         <f t="shared" si="1"/>
-        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Pharyngitis', inPortuguese: 'Faringite'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Pneumonia', inPortuguese: 'Pneumonia'}),</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="B77" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="D77" t="str">
         <f t="shared" si="1"/>
-        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Pneumonia', inPortuguese: 'Pneumonia'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Allergic Urticaria', inPortuguese: 'Urticária Alérgica'}),</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
@@ -2654,11 +2651,11 @@
         <v>185</v>
       </c>
       <c r="B78" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D78" t="str">
         <f t="shared" si="1"/>
-        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Allergic Urticaria', inPortuguese: 'Urticária Alérgica'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Angioedema', inPortuguese: 'Angioedema'}),</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
@@ -2666,11 +2663,11 @@
         <v>186</v>
       </c>
       <c r="B79" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="D79" t="str">
         <f t="shared" si="1"/>
-        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Angioedema', inPortuguese: 'Angioedema'}),</v>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Contact Dermatitis', inPortuguese: 'Dermatite de Contato'}),</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -2682,23 +2679,11 @@
       </c>
       <c r="D80" t="str">
         <f t="shared" si="1"/>
-        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Contact Dermatitis', inPortuguese: 'Dermatite de Contato'}),</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>188</v>
-      </c>
-      <c r="B81" t="s">
-        <v>191</v>
-      </c>
-      <c r="D81" t="str">
-        <f t="shared" si="1"/>
         <v>(:Disease {uuid: apoc.create.uuid(), name: 'Atopic Dermatitis', inPortuguese: 'Dermatite Atópica'}),</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D74" xr:uid="{B2FAB676-2031-4EBE-8374-605422BD9A7E}"/>
+  <autoFilter ref="A1:D80" xr:uid="{B2FAB676-2031-4EBE-8374-605422BD9A7E}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
@@ -2726,7 +2711,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -2734,13 +2719,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D2" t="str">
         <f>"(:Allergy {uuid: apoc.create.uuid(), name: '" &amp; B2 &amp;"', inPortuguese: '" &amp; A2 &amp;"', type: '" &amp; C2 &amp;"'}),"</f>
@@ -2749,13 +2734,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D50" si="0">"(:Allergy {uuid: apoc.create.uuid(), name: '" &amp; B3 &amp;"', inPortuguese: '" &amp; A3 &amp;"', type: '" &amp; C3 &amp;"'}),"</f>
@@ -2764,13 +2749,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
@@ -2779,13 +2764,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
@@ -2794,13 +2779,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
@@ -2809,13 +2794,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
@@ -2824,13 +2809,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
@@ -2839,13 +2824,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
@@ -2854,13 +2839,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
@@ -2869,13 +2854,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
@@ -2884,13 +2869,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B12" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C12" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
@@ -2899,13 +2884,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B13" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
@@ -2914,13 +2899,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
@@ -2929,13 +2914,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B15" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C15" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
@@ -2944,13 +2929,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B16" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
@@ -2959,13 +2944,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B17" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
@@ -2974,13 +2959,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B18" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C18" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
@@ -2989,13 +2974,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B19" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
@@ -3004,13 +2989,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B20" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C20" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
@@ -3019,13 +3004,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C21" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
@@ -3034,13 +3019,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B22" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C22" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
@@ -3049,13 +3034,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C23" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
@@ -3064,13 +3049,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B24" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C24" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
@@ -3079,13 +3064,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B25" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C25" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
@@ -3094,13 +3079,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B26" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C26" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
@@ -3109,13 +3094,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B27" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C27" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
@@ -3124,13 +3109,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B28" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C28" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
@@ -3139,13 +3124,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B29" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C29" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
@@ -3154,13 +3139,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C30" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
@@ -3169,13 +3154,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B31" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C31" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
@@ -3184,13 +3169,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B32" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D32" t="str">
         <f t="shared" si="0"/>
@@ -3199,13 +3184,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B33" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C33" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D33" t="str">
         <f t="shared" si="0"/>
@@ -3214,13 +3199,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B34" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C34" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D34" t="str">
         <f t="shared" si="0"/>
@@ -3229,13 +3214,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B35" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C35" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D35" t="str">
         <f t="shared" si="0"/>
@@ -3244,13 +3229,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B36" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C36" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D36" t="str">
         <f t="shared" si="0"/>
@@ -3259,13 +3244,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B37" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C37" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D37" t="str">
         <f t="shared" si="0"/>
@@ -3274,13 +3259,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B38" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C38" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D38" t="str">
         <f t="shared" si="0"/>
@@ -3289,13 +3274,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B39" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C39" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D39" t="str">
         <f t="shared" si="0"/>
@@ -3304,13 +3289,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B40" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C40" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D40" t="str">
         <f t="shared" si="0"/>
@@ -3319,13 +3304,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B41" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D41" t="str">
         <f t="shared" si="0"/>
@@ -3334,13 +3319,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B42" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C42" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D42" t="str">
         <f t="shared" si="0"/>
@@ -3349,13 +3334,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B43" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C43" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D43" t="str">
         <f t="shared" si="0"/>
@@ -3364,13 +3349,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B44" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C44" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D44" t="str">
         <f t="shared" si="0"/>
@@ -3379,13 +3364,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B45" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C45" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D45" t="str">
         <f t="shared" si="0"/>
@@ -3394,13 +3379,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B46" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C46" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D46" t="str">
         <f t="shared" si="0"/>
@@ -3409,13 +3394,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B47" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C47" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D47" t="str">
         <f t="shared" si="0"/>
@@ -3424,13 +3409,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>284</v>
+      </c>
+      <c r="B48" t="s">
         <v>285</v>
       </c>
-      <c r="B48" t="s">
-        <v>286</v>
-      </c>
       <c r="C48" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D48" t="str">
         <f t="shared" si="0"/>
@@ -3439,13 +3424,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B49" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C49" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D49" t="str">
         <f t="shared" si="0"/>
@@ -3454,13 +3439,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B50" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C50" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D50" t="str">
         <f t="shared" si="0"/>
@@ -3495,7 +3480,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -4415,10 +4400,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C2" t="str">
         <f>"(:Measurement {name: '" &amp; B2 &amp;"', inPortuguese: '" &amp; A2 &amp;"'}),"</f>
@@ -4427,10 +4412,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C18" si="0">"(:Measurement {name: '" &amp; B3 &amp;"', inPortuguese: '" &amp; A3 &amp;"'}),"</f>
@@ -4439,10 +4424,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
@@ -4451,10 +4436,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
@@ -4463,10 +4448,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -4475,10 +4460,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B7" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -4487,10 +4472,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -4499,10 +4484,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -4511,10 +4496,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B10" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -4523,10 +4508,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
@@ -4535,10 +4520,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B12" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
@@ -4547,10 +4532,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B13" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
@@ -4559,10 +4544,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B14" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
@@ -4571,10 +4556,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B15" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
@@ -4583,10 +4568,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B16" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
@@ -4595,10 +4580,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B17" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
@@ -4607,10 +4592,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B18" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
@@ -4902,19 +4887,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>363</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>364</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -4922,20 +4907,20 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B2" t="str">
         <f>SUBSTITUTE(UPPER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(A2," ","_"),"ó","o"),"í","i")),"/","_")</f>
         <v>BCG_ID</v>
       </c>
       <c r="C2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F2" t="str">
         <f>"(:Vaccine {name: '" &amp; A2 &amp;"', description: '" &amp; C2 &amp;"', dosage: '" &amp; D2 &amp;"', classification: '" &amp; E2 &amp;"'}),"</f>
@@ -4944,20 +4929,20 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B3" t="str">
         <f t="shared" ref="B3:B18" si="0">SUBSTITUTE(UPPER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(A3," ","_"),"ó","o"),"í","i")),"/","_")</f>
         <v>HEPATITE_B</v>
       </c>
       <c r="C3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:F18" si="1">"(:Vaccine {name: '" &amp; A3 &amp;"', description: '" &amp; C3 &amp;"', dosage: '" &amp; D3 &amp;"', classification: '" &amp; E3 &amp;"'}),"</f>
@@ -4966,20 +4951,20 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" si="0"/>
         <v>DTPW</v>
       </c>
       <c r="C4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="1"/>
@@ -4988,20 +4973,20 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="0"/>
         <v>H_INFLUENZAE</v>
       </c>
       <c r="C5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="1"/>
@@ -5010,20 +4995,20 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="0"/>
         <v>POLIO_VIP</v>
       </c>
       <c r="C6" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="1"/>
@@ -5032,20 +5017,20 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
         <v>POLIO_VOP</v>
       </c>
       <c r="C7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D7" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E7" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="1"/>
@@ -5054,20 +5039,20 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
         <v>ROTAVIRUS</v>
       </c>
       <c r="C8" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D8" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="1"/>
@@ -5076,20 +5061,20 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
         <v>VPC10</v>
       </c>
       <c r="C9" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E9" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="1"/>
@@ -5098,20 +5083,20 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
         <v>ACWY_C</v>
       </c>
       <c r="C10" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D10" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E10" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="1"/>
@@ -5120,20 +5105,20 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
         <v>MENINGOCOCICA_B</v>
       </c>
       <c r="C11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D11" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E11" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="1"/>
@@ -5142,20 +5127,20 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B12" t="str">
         <f>"_" &amp;A12</f>
         <v>_3V</v>
       </c>
       <c r="C12" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D12" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E12" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="1"/>
@@ -5164,20 +5149,20 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B13" t="str">
         <f t="shared" si="0"/>
         <v>FEBRE_AMARELA</v>
       </c>
       <c r="C13" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D13" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E13" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="1"/>
@@ -5186,20 +5171,20 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
         <v>HEPATITE_A</v>
       </c>
       <c r="C14" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D14" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E14" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="1"/>
@@ -5208,20 +5193,20 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
         <v>BCG</v>
       </c>
       <c r="C15" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D15" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E15" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="1"/>
@@ -5230,20 +5215,20 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
         <v>VARICELA</v>
       </c>
       <c r="C16" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D16" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E16" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="1"/>
@@ -5252,20 +5237,20 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B17" t="str">
         <f t="shared" si="0"/>
         <v>HPV4</v>
       </c>
       <c r="C17" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D17" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E17" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="1"/>
@@ -5274,20 +5259,20 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
         <v>DTPA</v>
       </c>
       <c r="C18" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D18" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E18" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="1"/>
@@ -5296,7 +5281,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F20" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -5410,7 +5395,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{391AE3A0-7DB7-4C1A-B882-6DBA4383A0D7}">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="O1" sqref="O1:O2"/>
     </sheetView>
   </sheetViews>
@@ -5427,33 +5412,33 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1" t="s">
+        <v>366</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="B1" t="s">
-        <v>367</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>363</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>364</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="O1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B2" t="str">
         <f>SUBSTITUTE(UPPER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(A2," ","_"),"ó","o"),"í","i")),"/","_")</f>
@@ -5466,10 +5451,10 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G2" t="str">
         <f>"(:VaccineDose {name: '" &amp; E2 &amp;"', vaccine: '" &amp; A2 &amp;"', fromAgeInMonths: toInteger(" &amp; C2 &amp;"), toAgeInMonths:toInteger(" &amp; D2 &amp;"), classification: '" &amp; F2 &amp;"'}),"</f>
@@ -5482,7 +5467,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B3" t="str">
         <f t="shared" ref="B3:B55" si="0">SUBSTITUTE(UPPER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(A3," ","_"),"ó","o"),"í","i")),"/","_")</f>
@@ -5495,10 +5480,10 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" ref="G3:G55" si="1">"(:VaccineDose {name: '" &amp; E3 &amp;"', vaccine: '" &amp; A3 &amp;"', fromAgeInMonths: toInteger(" &amp; C3 &amp;"), toAgeInMonths:toInteger(" &amp; D3 &amp;"), classification: '" &amp; F3 &amp;"'}),"</f>
@@ -5511,7 +5496,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" si="0"/>
@@ -5524,10 +5509,10 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="1"/>
@@ -5540,7 +5525,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="0"/>
@@ -5553,10 +5538,10 @@
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="1"/>
@@ -5569,7 +5554,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="0"/>
@@ -5582,10 +5567,10 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="1"/>
@@ -5598,7 +5583,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
@@ -5611,10 +5596,10 @@
         <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F7" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="1"/>
@@ -5627,7 +5612,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
@@ -5640,10 +5625,10 @@
         <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="1"/>
@@ -5656,7 +5641,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
@@ -5669,10 +5654,10 @@
         <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F9" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="1"/>
@@ -5685,7 +5670,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
@@ -5698,10 +5683,10 @@
         <v>60</v>
       </c>
       <c r="E10" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F10" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="1"/>
@@ -5714,7 +5699,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
@@ -5727,10 +5712,10 @@
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F11" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="1"/>
@@ -5743,7 +5728,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B12" t="str">
         <f t="shared" si="0"/>
@@ -5756,10 +5741,10 @@
         <v>4</v>
       </c>
       <c r="E12" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F12" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="1"/>
@@ -5772,7 +5757,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B13" t="str">
         <f t="shared" si="0"/>
@@ -5785,10 +5770,10 @@
         <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F13" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="1"/>
@@ -5801,7 +5786,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
@@ -5814,10 +5799,10 @@
         <v>18</v>
       </c>
       <c r="E14" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F14" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="1"/>
@@ -5830,7 +5815,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
@@ -5843,10 +5828,10 @@
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F15" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="1"/>
@@ -5859,7 +5844,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
@@ -5872,10 +5857,10 @@
         <v>4</v>
       </c>
       <c r="E16" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F16" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="1"/>
@@ -5888,7 +5873,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B17" t="str">
         <f t="shared" si="0"/>
@@ -5901,10 +5886,10 @@
         <v>6</v>
       </c>
       <c r="E17" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F17" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="1"/>
@@ -5917,7 +5902,7 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
@@ -5930,10 +5915,10 @@
         <v>18</v>
       </c>
       <c r="E18" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F18" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="1"/>
@@ -5946,7 +5931,7 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B19" t="str">
         <f t="shared" si="0"/>
@@ -5959,10 +5944,10 @@
         <v>60</v>
       </c>
       <c r="E19" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F19" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="1"/>
@@ -5975,7 +5960,7 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B20" t="str">
         <f t="shared" si="0"/>
@@ -5988,10 +5973,10 @@
         <v>4</v>
       </c>
       <c r="E20" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F20" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="1"/>
@@ -6004,7 +5989,7 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B21" t="str">
         <f t="shared" si="0"/>
@@ -6017,10 +6002,10 @@
         <v>8</v>
       </c>
       <c r="E21" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F21" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="1"/>
@@ -6033,7 +6018,7 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B22" t="str">
         <f t="shared" si="0"/>
@@ -6046,10 +6031,10 @@
         <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F22" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="1"/>
@@ -6062,7 +6047,7 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B23" t="str">
         <f t="shared" si="0"/>
@@ -6075,10 +6060,10 @@
         <v>6</v>
       </c>
       <c r="E23" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F23" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="1"/>
@@ -6091,7 +6076,7 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B24" t="str">
         <f t="shared" si="0"/>
@@ -6104,10 +6089,10 @@
         <v>15</v>
       </c>
       <c r="E24" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F24" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="1"/>
@@ -6120,7 +6105,7 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B25" t="str">
         <f t="shared" si="0"/>
@@ -6133,10 +6118,10 @@
         <v>5</v>
       </c>
       <c r="E25" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F25" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="1"/>
@@ -6149,7 +6134,7 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B26" t="str">
         <f t="shared" si="0"/>
@@ -6162,10 +6147,10 @@
         <v>8</v>
       </c>
       <c r="E26" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F26" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="1"/>
@@ -6178,7 +6163,7 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B27" t="str">
         <f t="shared" si="0"/>
@@ -6191,10 +6176,10 @@
         <v>15</v>
       </c>
       <c r="E27" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F27" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="1"/>
@@ -6207,7 +6192,7 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B28" t="str">
         <f t="shared" si="0"/>
@@ -6220,10 +6205,10 @@
         <v>72</v>
       </c>
       <c r="E28" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F28" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="1"/>
@@ -6236,7 +6221,7 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B29" t="str">
         <f t="shared" si="0"/>
@@ -6249,10 +6234,10 @@
         <v>3</v>
       </c>
       <c r="E29" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F29" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="1"/>
@@ -6265,7 +6250,7 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B30" t="str">
         <f t="shared" si="0"/>
@@ -6278,10 +6263,10 @@
         <v>5</v>
       </c>
       <c r="E30" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F30" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="1"/>
@@ -6294,7 +6279,7 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B31" t="str">
         <f t="shared" si="0"/>
@@ -6307,10 +6292,10 @@
         <v>15</v>
       </c>
       <c r="E31" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F31" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" si="1"/>
@@ -6323,7 +6308,7 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B32" t="str">
         <f t="shared" si="0"/>
@@ -6336,10 +6321,10 @@
         <v>12</v>
       </c>
       <c r="E32" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F32" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G32" t="str">
         <f t="shared" si="1"/>
@@ -6352,7 +6337,7 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B33" t="str">
         <f t="shared" si="0"/>
@@ -6365,10 +6350,10 @@
         <v>24</v>
       </c>
       <c r="E33" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F33" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G33" t="str">
         <f t="shared" si="1"/>
@@ -6381,7 +6366,7 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B34" t="str">
         <f>SUBSTITUTE(UPPER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(A34," ","_"),"ó","o"),"í","i")),"/","_")</f>
@@ -6394,10 +6379,10 @@
         <v>36</v>
       </c>
       <c r="E34" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F34" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" si="1"/>
@@ -6410,7 +6395,7 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="0"/>
@@ -6423,10 +6408,10 @@
         <v>48</v>
       </c>
       <c r="E35" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F35" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="1"/>
@@ -6439,7 +6424,7 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="0"/>
@@ -6452,10 +6437,10 @@
         <v>60</v>
       </c>
       <c r="E36" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F36" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" si="1"/>
@@ -6468,7 +6453,7 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B37" t="str">
         <f t="shared" si="0"/>
@@ -6481,10 +6466,10 @@
         <v>72</v>
       </c>
       <c r="E37" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F37" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G37" t="str">
         <f t="shared" si="1"/>
@@ -6497,7 +6482,7 @@
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" si="0"/>
@@ -6510,10 +6495,10 @@
         <v>84</v>
       </c>
       <c r="E38" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F38" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G38" t="str">
         <f t="shared" si="1"/>
@@ -6526,7 +6511,7 @@
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B39" t="str">
         <f t="shared" si="0"/>
@@ -6539,10 +6524,10 @@
         <v>96</v>
       </c>
       <c r="E39" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F39" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G39" t="str">
         <f t="shared" si="1"/>
@@ -6555,7 +6540,7 @@
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B40" t="str">
         <f t="shared" si="0"/>
@@ -6568,10 +6553,10 @@
         <v>108</v>
       </c>
       <c r="E40" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F40" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G40" t="str">
         <f t="shared" si="1"/>
@@ -6584,7 +6569,7 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B41" t="str">
         <f t="shared" si="0"/>
@@ -6597,10 +6582,10 @@
         <v>120</v>
       </c>
       <c r="E41" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F41" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G41" t="str">
         <f t="shared" si="1"/>
@@ -6613,7 +6598,7 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B42" t="str">
         <f t="shared" si="0"/>
@@ -6626,10 +6611,10 @@
         <v>9</v>
       </c>
       <c r="E42" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F42" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G42" t="str">
         <f t="shared" si="1"/>
@@ -6642,7 +6627,7 @@
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B43" t="str">
         <f t="shared" si="0"/>
@@ -6655,10 +6640,10 @@
         <v>12</v>
       </c>
       <c r="E43" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F43" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G43" t="str">
         <f t="shared" si="1"/>
@@ -6671,7 +6656,7 @@
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B44" t="str">
         <f t="shared" si="0"/>
@@ -6684,10 +6669,10 @@
         <v>18</v>
       </c>
       <c r="E44" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F44" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" si="1"/>
@@ -6700,7 +6685,7 @@
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="0"/>
@@ -6713,10 +6698,10 @@
         <v>12</v>
       </c>
       <c r="E45" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F45" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G45" t="str">
         <f t="shared" si="1"/>
@@ -6729,7 +6714,7 @@
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="0"/>
@@ -6742,10 +6727,10 @@
         <v>24</v>
       </c>
       <c r="E46" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F46" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G46" t="str">
         <f t="shared" si="1"/>
@@ -6758,7 +6743,7 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B47" t="str">
         <f t="shared" si="0"/>
@@ -6771,10 +6756,10 @@
         <v>12</v>
       </c>
       <c r="E47" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F47" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G47" t="str">
         <f t="shared" si="1"/>
@@ -6787,7 +6772,7 @@
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B48" t="str">
         <f t="shared" si="0"/>
@@ -6800,10 +6785,10 @@
         <v>24</v>
       </c>
       <c r="E48" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F48" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G48" t="str">
         <f t="shared" si="1"/>
@@ -6816,7 +6801,7 @@
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B49" t="str">
         <f t="shared" si="0"/>
@@ -6829,10 +6814,10 @@
         <v>119</v>
       </c>
       <c r="E49" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F49" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G49" t="str">
         <f t="shared" si="1"/>
@@ -6845,7 +6830,7 @@
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B50" t="str">
         <f t="shared" si="0"/>
@@ -6858,10 +6843,10 @@
         <v>132</v>
       </c>
       <c r="E50" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F50" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G50" t="str">
         <f t="shared" si="1"/>
@@ -6874,7 +6859,7 @@
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B51" t="str">
         <f t="shared" si="0"/>
@@ -6887,10 +6872,10 @@
         <v>2</v>
       </c>
       <c r="E51" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F51" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G51" t="str">
         <f t="shared" si="1"/>
@@ -6903,7 +6888,7 @@
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B52" t="str">
         <f t="shared" si="0"/>
@@ -6916,10 +6901,10 @@
         <v>4</v>
       </c>
       <c r="E52" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F52" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="1"/>
@@ -6932,7 +6917,7 @@
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B53" t="str">
         <f t="shared" si="0"/>
@@ -6945,10 +6930,10 @@
         <v>6</v>
       </c>
       <c r="E53" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F53" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G53" t="str">
         <f t="shared" si="1"/>
@@ -6961,7 +6946,7 @@
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B54" t="str">
         <f t="shared" si="0"/>
@@ -6974,10 +6959,10 @@
         <v>18</v>
       </c>
       <c r="E54" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F54" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G54" t="str">
         <f t="shared" si="1"/>
@@ -6990,7 +6975,7 @@
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B55" t="str">
         <f t="shared" si="0"/>
@@ -7003,10 +6988,10 @@
         <v>60</v>
       </c>
       <c r="E55" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F55" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G55" t="str">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
refactor: :recycle: refactoring Intolerance tasks
</commit_message>
<xml_diff>
--- a/poc.xlsx
+++ b/poc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\renatospaka\dev\heykid\draft\poc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{954F8497-8AFA-43A5-BE7A-27382973D72D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F43E771-DDB5-4087-8442-58294D6E035E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="complication" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">disease!$A$1:$D$80</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">intolerance!$A$1:$D$50</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'vaccine dose'!$A$1:$F$55</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="370">
   <si>
     <t>Tipos</t>
   </si>
@@ -1152,6 +1153,9 @@
   </si>
   <si>
     <t>Query Relationship</t>
+  </si>
+  <si>
+    <t>Lactose</t>
   </si>
 </sst>
 </file>
@@ -1709,7 +1713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16822055-6D7C-4562-869B-B3AD28812FB9}">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
+    <sheetView topLeftCell="A56" zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
       <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
@@ -3461,7 +3465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FBDA324-BA52-4553-9EA4-1F1EB8000A70}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D50"/>
     </sheetView>
   </sheetViews>
@@ -4081,13 +4085,11 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" t="str">
-        <f>allergy!A35</f>
-        <v>Leite</v>
-      </c>
-      <c r="B35" t="str">
-        <f>allergy!B35</f>
-        <v>Milk</v>
+      <c r="A35" t="s">
+        <v>369</v>
+      </c>
+      <c r="B35" t="s">
+        <v>369</v>
       </c>
       <c r="C35" t="str">
         <f>allergy!C35</f>
@@ -4095,7 +4097,7 @@
       </c>
       <c r="D35" t="str">
         <f t="shared" si="0"/>
-        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Milk', inPortuguese: 'Leite', type: 'Food'}),</v>
+        <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Lactose', inPortuguese: 'Lactose', type: 'Food'}),</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -4369,6 +4371,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D50" xr:uid="{031B7EB9-4D4C-4A51-A283-0BEC9FAF1399}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
fix: :bug: Disease & Complication bugs
</commit_message>
<xml_diff>
--- a/poc.xlsx
+++ b/poc.xlsx
@@ -8,24 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\renatospaka\dev\heykid\draft\poc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F43E771-DDB5-4087-8442-58294D6E035E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD474712-6EBF-4959-8131-6EA2BA4AC84E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="complication" sheetId="1" r:id="rId1"/>
     <sheet name="disease" sheetId="3" r:id="rId2"/>
     <sheet name="allergy" sheetId="4" r:id="rId3"/>
     <sheet name="intolerance" sheetId="5" r:id="rId4"/>
-    <sheet name="measurement" sheetId="8" r:id="rId5"/>
-    <sheet name="specialty" sheetId="2" r:id="rId6"/>
-    <sheet name="vaccine" sheetId="6" r:id="rId7"/>
-    <sheet name="vaccine dose" sheetId="7" r:id="rId8"/>
+    <sheet name="symtom" sheetId="9" r:id="rId5"/>
+    <sheet name="measurement" sheetId="8" r:id="rId6"/>
+    <sheet name="specialty" sheetId="2" r:id="rId7"/>
+    <sheet name="vaccine" sheetId="6" r:id="rId8"/>
+    <sheet name="vaccine dose" sheetId="7" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">disease!$A$1:$D$80</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">disease!$A$1:$D$86</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">intolerance!$A$1:$D$50</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'vaccine dose'!$A$1:$F$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'vaccine dose'!$A$1:$F$55</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="432">
   <si>
     <t>Tipos</t>
   </si>
@@ -1156,6 +1157,192 @@
   </si>
   <si>
     <t>Lactose</t>
+  </si>
+  <si>
+    <t>Resfriado</t>
+  </si>
+  <si>
+    <t>Gripe</t>
+  </si>
+  <si>
+    <t>Caxumba</t>
+  </si>
+  <si>
+    <t>Sarampo</t>
+  </si>
+  <si>
+    <t>Rubéola</t>
+  </si>
+  <si>
+    <t>Meningite</t>
+  </si>
+  <si>
+    <t>Catapora</t>
+  </si>
+  <si>
+    <t>Cold</t>
+  </si>
+  <si>
+    <t>Mumps</t>
+  </si>
+  <si>
+    <t>Measles</t>
+  </si>
+  <si>
+    <t>Rubella</t>
+  </si>
+  <si>
+    <t>Meningitis</t>
+  </si>
+  <si>
+    <t>Chickenpox</t>
+  </si>
+  <si>
+    <t>Croup</t>
+  </si>
+  <si>
+    <t>Virose</t>
+  </si>
+  <si>
+    <t>Influenza</t>
+  </si>
+  <si>
+    <t>Strep Throat</t>
+  </si>
+  <si>
+    <t>Stomach Flu</t>
+  </si>
+  <si>
+    <t>Inflamação Garganta</t>
+  </si>
+  <si>
+    <t>Febre Estomacal</t>
+  </si>
+  <si>
+    <t>Sore Throat</t>
+  </si>
+  <si>
+    <t>Dor de Garganta</t>
+  </si>
+  <si>
+    <t>Chagas Disease</t>
+  </si>
+  <si>
+    <t>Dengue Fever</t>
+  </si>
+  <si>
+    <t>Zika Fever</t>
+  </si>
+  <si>
+    <t>Leptospirosis</t>
+  </si>
+  <si>
+    <t>Yellow Fever</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chikungunya </t>
+  </si>
+  <si>
+    <t>Doença de Chagas</t>
+  </si>
+  <si>
+    <t>Dengue</t>
+  </si>
+  <si>
+    <t>Zika</t>
+  </si>
+  <si>
+    <t>Leptospirose</t>
+  </si>
+  <si>
+    <t>Febre Amarela</t>
+  </si>
+  <si>
+    <t>Vomit</t>
+  </si>
+  <si>
+    <t>Choke</t>
+  </si>
+  <si>
+    <t>Pain</t>
+  </si>
+  <si>
+    <t>Diarréia</t>
+  </si>
+  <si>
+    <t>Engasgo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dor </t>
+  </si>
+  <si>
+    <t>Short of Breath</t>
+  </si>
+  <si>
+    <t>Falta de Ar</t>
+  </si>
+  <si>
+    <t>Sudorese</t>
+  </si>
+  <si>
+    <t>Sweating</t>
+  </si>
+  <si>
+    <t>Insônia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insomnia </t>
+  </si>
+  <si>
+    <t>Dry Mouth</t>
+  </si>
+  <si>
+    <t>Hoarseness</t>
+  </si>
+  <si>
+    <t>Sense of Taste</t>
+  </si>
+  <si>
+    <t>Bad Breath</t>
+  </si>
+  <si>
+    <t>Sense of Smell</t>
+  </si>
+  <si>
+    <t>Perda do Paladar</t>
+  </si>
+  <si>
+    <t>Perda do Olfato</t>
+  </si>
+  <si>
+    <t>Mau Hálito</t>
+  </si>
+  <si>
+    <t>Boca Seca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rouquidão </t>
+  </si>
+  <si>
+    <t>Apenéia</t>
+  </si>
+  <si>
+    <t>Apenea</t>
+  </si>
+  <si>
+    <t>Tremor</t>
+  </si>
+  <si>
+    <t>Dizziness</t>
+  </si>
+  <si>
+    <t>Tontura</t>
+  </si>
+  <si>
+    <t>Lack of Appetite</t>
+  </si>
+  <si>
+    <t>Falta de Apetite</t>
   </si>
 </sst>
 </file>
@@ -1711,10 +1898,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16822055-6D7C-4562-869B-B3AD28812FB9}">
-  <dimension ref="A1:D80"/>
+  <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView topLeftCell="A79" zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
+      <selection activeCell="D92" sqref="D92:D97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2514,7 +2701,7 @@
         <v>165</v>
       </c>
       <c r="D66" t="str">
-        <f t="shared" ref="D66:D80" si="1">"(:Disease {uuid: apoc.create.uuid(), name: '" &amp; B66 &amp;"', inPortuguese: '" &amp; A66 &amp;"'}),"</f>
+        <f t="shared" ref="D66:D97" si="1">"(:Disease {uuid: apoc.create.uuid(), name: '" &amp; B66 &amp;"', inPortuguese: '" &amp; A66 &amp;"'}),"</f>
         <v>(:Disease {uuid: apoc.create.uuid(), name: 'Tendonitis', inPortuguese: 'Tendinite'}),</v>
       </c>
     </row>
@@ -2686,9 +2873,214 @@
         <v>(:Disease {uuid: apoc.create.uuid(), name: 'Atopic Dermatitis', inPortuguese: 'Dermatite Atópica'}),</v>
       </c>
     </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>370</v>
+      </c>
+      <c r="B81" t="s">
+        <v>377</v>
+      </c>
+      <c r="D81" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Cold', inPortuguese: 'Resfriado'}),</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>371</v>
+      </c>
+      <c r="B82" t="s">
+        <v>385</v>
+      </c>
+      <c r="D82" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Influenza', inPortuguese: 'Gripe'}),</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>372</v>
+      </c>
+      <c r="B83" t="s">
+        <v>378</v>
+      </c>
+      <c r="D83" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Mumps', inPortuguese: 'Caxumba'}),</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>373</v>
+      </c>
+      <c r="B84" t="s">
+        <v>379</v>
+      </c>
+      <c r="D84" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Measles', inPortuguese: 'Sarampo'}),</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>374</v>
+      </c>
+      <c r="B85" t="s">
+        <v>380</v>
+      </c>
+      <c r="D85" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Rubella', inPortuguese: 'Rubéola'}),</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>375</v>
+      </c>
+      <c r="B86" t="s">
+        <v>381</v>
+      </c>
+      <c r="D86" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Meningitis', inPortuguese: 'Meningite'}),</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>376</v>
+      </c>
+      <c r="B87" t="s">
+        <v>382</v>
+      </c>
+      <c r="D87" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Chickenpox', inPortuguese: 'Catapora'}),</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>384</v>
+      </c>
+      <c r="B88" t="s">
+        <v>383</v>
+      </c>
+      <c r="D88" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Croup', inPortuguese: 'Virose'}),</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>388</v>
+      </c>
+      <c r="B89" t="s">
+        <v>386</v>
+      </c>
+      <c r="D89" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Strep Throat', inPortuguese: 'Inflamação Garganta'}),</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>389</v>
+      </c>
+      <c r="B90" t="s">
+        <v>387</v>
+      </c>
+      <c r="D90" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Stomach Flu', inPortuguese: 'Febre Estomacal'}),</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>391</v>
+      </c>
+      <c r="B91" t="s">
+        <v>390</v>
+      </c>
+      <c r="D91" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Sore Throat', inPortuguese: 'Dor de Garganta'}),</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>398</v>
+      </c>
+      <c r="B92" t="s">
+        <v>392</v>
+      </c>
+      <c r="D92" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Chagas Disease', inPortuguese: 'Doença de Chagas'}),</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>399</v>
+      </c>
+      <c r="B93" t="s">
+        <v>393</v>
+      </c>
+      <c r="D93" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Dengue Fever', inPortuguese: 'Dengue'}),</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>400</v>
+      </c>
+      <c r="B94" t="s">
+        <v>394</v>
+      </c>
+      <c r="D94" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Zika Fever', inPortuguese: 'Zika'}),</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>401</v>
+      </c>
+      <c r="B95" t="s">
+        <v>395</v>
+      </c>
+      <c r="D95" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Leptospirosis', inPortuguese: 'Leptospirose'}),</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>402</v>
+      </c>
+      <c r="B96" t="s">
+        <v>396</v>
+      </c>
+      <c r="D96" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Yellow Fever', inPortuguese: 'Febre Amarela'}),</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>397</v>
+      </c>
+      <c r="B97" t="s">
+        <v>397</v>
+      </c>
+      <c r="D97" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Chikungunya ', inPortuguese: 'Chikungunya '}),</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D80" xr:uid="{B2FAB676-2031-4EBE-8374-605422BD9A7E}"/>
+  <autoFilter ref="A1:D86" xr:uid="{4BA12A2B-C6F7-499D-BED0-9D0EF84A0FCD}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3465,8 +3857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FBDA324-BA52-4553-9EA4-1F1EB8000A70}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D50"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3954,7 +4346,7 @@
         <v>Drug</v>
       </c>
       <c r="D27" t="str">
-        <f t="shared" si="0"/>
+        <f>"(:Intolerance {uuid: apoc.create.uuid(), name: '" &amp; B27 &amp;"', inPortuguese: '" &amp; A27 &amp;"', type: '" &amp; C27 &amp;"'}),"</f>
         <v>(:Intolerance {uuid: apoc.create.uuid(), name: 'Azithromycin', inPortuguese: 'Azitromicina', type: 'Drug'}),</v>
       </c>
     </row>
@@ -4377,11 +4769,342 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7A3E379-11D0-4971-86BE-FD970275DE12}">
+  <dimension ref="A1:C26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.77734375" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
+    <col min="3" max="3" width="30.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C2" t="str">
+        <f>"(:Symptom {uuid: apoc.create.uuid(), name: '" &amp; B2 &amp;"', inPortuguese: '" &amp; A2 &amp;"'}),"</f>
+        <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Cry', inPortuguese: 'Choro'}),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>291</v>
+      </c>
+      <c r="B3" t="s">
+        <v>308</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C26" si="0">"(:Symptom {uuid: apoc.create.uuid(), name: '" &amp; B3 &amp;"', inPortuguese: '" &amp; A3 &amp;"'}),"</f>
+        <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Fever', inPortuguese: 'Febre'}),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>292</v>
+      </c>
+      <c r="B4" t="s">
+        <v>403</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Vomit', inPortuguese: 'Vômito'}),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>406</v>
+      </c>
+      <c r="B5" t="s">
+        <v>310</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Diarrhea', inPortuguese: 'Diarréia'}),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>294</v>
+      </c>
+      <c r="B6" t="s">
+        <v>311</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Coryza', inPortuguese: 'Coriza'}),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>295</v>
+      </c>
+      <c r="B7" t="s">
+        <v>312</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Stress', inPortuguese: 'Estresse'}),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>296</v>
+      </c>
+      <c r="B8" t="s">
+        <v>313</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Cough', inPortuguese: 'Tosse'}),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>297</v>
+      </c>
+      <c r="B9" t="s">
+        <v>314</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Sneeze', inPortuguese: 'Espirro'}),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>298</v>
+      </c>
+      <c r="B10" t="s">
+        <v>315</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Nausea', inPortuguese: 'Náusea'}),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>300</v>
+      </c>
+      <c r="B11" t="s">
+        <v>317</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Vertigo', inPortuguese: 'Vertigem'}),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>407</v>
+      </c>
+      <c r="B12" t="s">
+        <v>404</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Choke', inPortuguese: 'Engasgo'}),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>304</v>
+      </c>
+      <c r="B13" t="s">
+        <v>321</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Weakness', inPortuguese: 'Fraqueza'}),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>408</v>
+      </c>
+      <c r="B14" t="s">
+        <v>405</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Pain', inPortuguese: 'Dor '}),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>410</v>
+      </c>
+      <c r="B15" t="s">
+        <v>409</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Short of Breath', inPortuguese: 'Falta de Ar'}),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>411</v>
+      </c>
+      <c r="B16" t="s">
+        <v>412</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Sweating', inPortuguese: 'Sudorese'}),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>413</v>
+      </c>
+      <c r="B17" t="s">
+        <v>414</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Insomnia ', inPortuguese: 'Insônia'}),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>423</v>
+      </c>
+      <c r="B18" t="s">
+        <v>415</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Dry Mouth', inPortuguese: 'Boca Seca'}),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>424</v>
+      </c>
+      <c r="B19" t="s">
+        <v>416</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Hoarseness', inPortuguese: 'Rouquidão '}),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>420</v>
+      </c>
+      <c r="B20" t="s">
+        <v>417</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Sense of Taste', inPortuguese: 'Perda do Paladar'}),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>422</v>
+      </c>
+      <c r="B21" t="s">
+        <v>418</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Bad Breath', inPortuguese: 'Mau Hálito'}),</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>421</v>
+      </c>
+      <c r="B22" t="s">
+        <v>419</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Sense of Smell', inPortuguese: 'Perda do Olfato'}),</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>425</v>
+      </c>
+      <c r="B23" t="s">
+        <v>426</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Apenea', inPortuguese: 'Apenéia'}),</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>427</v>
+      </c>
+      <c r="B24" t="s">
+        <v>427</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Tremor', inPortuguese: 'Tremor'}),</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>429</v>
+      </c>
+      <c r="B25" t="s">
+        <v>428</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Dizziness', inPortuguese: 'Tontura'}),</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>431</v>
+      </c>
+      <c r="B26" t="s">
+        <v>430</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Lack of Appetite', inPortuguese: 'Falta de Apetite'}),</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F5CDE23-EAB5-47A7-B33D-96F18BE56CCE}">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C18"/>
+      <selection activeCell="A3" sqref="A3:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4414,195 +5137,99 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>291</v>
-      </c>
-      <c r="B3" t="s">
-        <v>308</v>
-      </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C18" si="0">"(:Measurement {name: '" &amp; B3 &amp;"', inPortuguese: '" &amp; A3 &amp;"'}),"</f>
-        <v>(:Measurement {name: 'Fever', inPortuguese: 'Febre'}),</v>
+        <v>(:Measurement {name: '', inPortuguese: ''}),</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>292</v>
-      </c>
-      <c r="B4" t="s">
-        <v>309</v>
-      </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
-        <v>(:Measurement {name: 'Vomiting', inPortuguese: 'Vômito'}),</v>
+        <v>(:Measurement {name: '', inPortuguese: ''}),</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>293</v>
-      </c>
-      <c r="B5" t="s">
-        <v>310</v>
-      </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
-        <v>(:Measurement {name: 'Diarrhea', inPortuguese: 'Diarreia'}),</v>
+        <v>(:Measurement {name: '', inPortuguese: ''}),</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>294</v>
-      </c>
-      <c r="B6" t="s">
-        <v>311</v>
-      </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
-        <v>(:Measurement {name: 'Coryza', inPortuguese: 'Coriza'}),</v>
+        <v>(:Measurement {name: '', inPortuguese: ''}),</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>295</v>
-      </c>
-      <c r="B7" t="s">
-        <v>312</v>
-      </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
-        <v>(:Measurement {name: 'Stress', inPortuguese: 'Estresse'}),</v>
+        <v>(:Measurement {name: '', inPortuguese: ''}),</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>296</v>
-      </c>
-      <c r="B8" t="s">
-        <v>313</v>
-      </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
-        <v>(:Measurement {name: 'Cough', inPortuguese: 'Tosse'}),</v>
+        <v>(:Measurement {name: '', inPortuguese: ''}),</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>297</v>
-      </c>
-      <c r="B9" t="s">
-        <v>314</v>
-      </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
-        <v>(:Measurement {name: 'Sneeze', inPortuguese: 'Espirro'}),</v>
+        <v>(:Measurement {name: '', inPortuguese: ''}),</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>298</v>
-      </c>
-      <c r="B10" t="s">
-        <v>315</v>
-      </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
-        <v>(:Measurement {name: 'Nausea', inPortuguese: 'Náusea'}),</v>
+        <v>(:Measurement {name: '', inPortuguese: ''}),</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>299</v>
-      </c>
-      <c r="B11" t="s">
-        <v>316</v>
-      </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
-        <v>(:Measurement {name: 'Fall', inPortuguese: 'Queda'}),</v>
+        <v>(:Measurement {name: '', inPortuguese: ''}),</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>300</v>
-      </c>
-      <c r="B12" t="s">
-        <v>317</v>
-      </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
-        <v>(:Measurement {name: 'Vertigo', inPortuguese: 'Vertigem'}),</v>
+        <v>(:Measurement {name: '', inPortuguese: ''}),</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>301</v>
-      </c>
-      <c r="B13" t="s">
-        <v>318</v>
-      </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
-        <v>(:Measurement {name: 'Twist', inPortuguese: 'Torção'}),</v>
+        <v>(:Measurement {name: '', inPortuguese: ''}),</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>302</v>
-      </c>
-      <c r="B14" t="s">
-        <v>319</v>
-      </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
-        <v>(:Measurement {name: 'Cut', inPortuguese: 'Corte'}),</v>
+        <v>(:Measurement {name: '', inPortuguese: ''}),</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>303</v>
-      </c>
-      <c r="B15" t="s">
-        <v>320</v>
-      </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
-        <v>(:Measurement {name: 'Shock', inPortuguese: 'Choque'}),</v>
+        <v>(:Measurement {name: '', inPortuguese: ''}),</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>304</v>
-      </c>
-      <c r="B16" t="s">
-        <v>321</v>
-      </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
-        <v>(:Measurement {name: 'Weakness', inPortuguese: 'Fraqueza'}),</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>305</v>
-      </c>
-      <c r="B17" t="s">
-        <v>322</v>
-      </c>
+        <v>(:Measurement {name: '', inPortuguese: ''}),</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C17" t="str">
         <f t="shared" si="0"/>
-        <v>(:Measurement {name: 'Ingestion', inPortuguese: 'Ingestão'}),</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>306</v>
-      </c>
-      <c r="B18" t="s">
-        <v>323</v>
-      </c>
+        <v>(:Measurement {name: '', inPortuguese: ''}),</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C18" t="str">
         <f t="shared" si="0"/>
-        <v>(:Measurement {name: 'Ache', inPortuguese: 'Dor'}),</v>
+        <v>(:Measurement {name: '', inPortuguese: ''}),</v>
       </c>
     </row>
   </sheetData>
@@ -4610,7 +5237,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8BE5788-872A-43B9-9E25-E8C1A583BFB6}">
   <dimension ref="A1:C20"/>
   <sheetViews>
@@ -4869,7 +5496,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A61B1D1-1498-4062-8FF1-43F1DDC4F5BE}">
   <dimension ref="A1:F37"/>
   <sheetViews>
@@ -5394,7 +6021,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{391AE3A0-7DB7-4C1A-B882-6DBA4383A0D7}">
   <dimension ref="A1:O55"/>
   <sheetViews>

</xml_diff>

<commit_message>
remove auxiliar file of the spreadsheet
</commit_message>
<xml_diff>
--- a/poc.xlsx
+++ b/poc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\renatospaka\dev\heykid\draft\poc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD474712-6EBF-4959-8131-6EA2BA4AC84E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5591167E-114D-444D-8BB9-A8F7544EACB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4773,7 +4773,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
feat: :sparkles: add measurement features.
</commit_message>
<xml_diff>
--- a/poc.xlsx
+++ b/poc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\renatospaka\dev\heykid\draft\poc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5591167E-114D-444D-8BB9-A8F7544EACB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E48F501F-462A-4090-992F-A48BC65D0A4A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="complication" sheetId="1" r:id="rId1"/>
@@ -19,14 +19,15 @@
     <sheet name="intolerance" sheetId="5" r:id="rId4"/>
     <sheet name="symtom" sheetId="9" r:id="rId5"/>
     <sheet name="measurement" sheetId="8" r:id="rId6"/>
-    <sheet name="specialty" sheetId="2" r:id="rId7"/>
-    <sheet name="vaccine" sheetId="6" r:id="rId8"/>
-    <sheet name="vaccine dose" sheetId="7" r:id="rId9"/>
+    <sheet name="measurement unit" sheetId="10" r:id="rId7"/>
+    <sheet name="specialty" sheetId="2" r:id="rId8"/>
+    <sheet name="vaccine" sheetId="6" r:id="rId9"/>
+    <sheet name="vaccine dose" sheetId="7" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">disease!$A$1:$D$86</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">intolerance!$A$1:$D$50</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'vaccine dose'!$A$1:$F$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'vaccine dose'!$A$1:$F$55</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="554">
   <si>
     <t>Tipos</t>
   </si>
@@ -1343,6 +1344,372 @@
   </si>
   <si>
     <t>Falta de Apetite</t>
+  </si>
+  <si>
+    <t>Sintomas</t>
+  </si>
+  <si>
+    <t>Em Português</t>
+  </si>
+  <si>
+    <t>Em Portugues</t>
+  </si>
+  <si>
+    <t>Chest</t>
+  </si>
+  <si>
+    <t>Head</t>
+  </si>
+  <si>
+    <t>Back</t>
+  </si>
+  <si>
+    <t>Toothache</t>
+  </si>
+  <si>
+    <t>Earache</t>
+  </si>
+  <si>
+    <t>Genital</t>
+  </si>
+  <si>
+    <t>Joint</t>
+  </si>
+  <si>
+    <t>Peito</t>
+  </si>
+  <si>
+    <t>Cabeça</t>
+  </si>
+  <si>
+    <t>Dor de Dente</t>
+  </si>
+  <si>
+    <t>Dor de Ouvido</t>
+  </si>
+  <si>
+    <t>Articulação</t>
+  </si>
+  <si>
+    <t>Tipo Dor</t>
+  </si>
+  <si>
+    <t>Localização Dor</t>
+  </si>
+  <si>
+    <t>Costas</t>
+  </si>
+  <si>
+    <t>Joelho</t>
+  </si>
+  <si>
+    <t>Pé</t>
+  </si>
+  <si>
+    <t>Calcanhar</t>
+  </si>
+  <si>
+    <t>Tornozelo</t>
+  </si>
+  <si>
+    <t>Knee</t>
+  </si>
+  <si>
+    <t>Foot</t>
+  </si>
+  <si>
+    <t>Heel</t>
+  </si>
+  <si>
+    <t>Ankle</t>
+  </si>
+  <si>
+    <t>Ombro</t>
+  </si>
+  <si>
+    <t>Shoulder</t>
+  </si>
+  <si>
+    <t>Pulsatile</t>
+  </si>
+  <si>
+    <t>Acute</t>
+  </si>
+  <si>
+    <t>Tightening</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Colic</t>
+  </si>
+  <si>
+    <t>Burning</t>
+  </si>
+  <si>
+    <t>Persistent</t>
+  </si>
+  <si>
+    <t>Pulsátil</t>
+  </si>
+  <si>
+    <t>Agudo</t>
+  </si>
+  <si>
+    <t>Aperto</t>
+  </si>
+  <si>
+    <t>Pesa</t>
+  </si>
+  <si>
+    <t>Cólica</t>
+  </si>
+  <si>
+    <t>Queima</t>
+  </si>
+  <si>
+    <t>Persistente</t>
+  </si>
+  <si>
+    <t>Numbness</t>
+  </si>
+  <si>
+    <t>Dormência</t>
+  </si>
+  <si>
+    <t>Pescoço</t>
+  </si>
+  <si>
+    <t>Neck</t>
+  </si>
+  <si>
+    <t>Abdomen</t>
+  </si>
+  <si>
+    <t>Abdômen</t>
+  </si>
+  <si>
+    <t>Quadril</t>
+  </si>
+  <si>
+    <t>Hip</t>
+  </si>
+  <si>
+    <t>Pélvis</t>
+  </si>
+  <si>
+    <t>Pelvis</t>
+  </si>
+  <si>
+    <t>Crônica</t>
+  </si>
+  <si>
+    <t>Chronic</t>
+  </si>
+  <si>
+    <t>Fibromyalgia</t>
+  </si>
+  <si>
+    <t>Fibromialgia</t>
+  </si>
+  <si>
+    <t>Em português</t>
+  </si>
+  <si>
+    <t>Medições</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Systolic Blood Pressure</t>
+  </si>
+  <si>
+    <t>Diastolic Blood Pressure</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>Sleep</t>
+  </si>
+  <si>
+    <t>Glucose</t>
+  </si>
+  <si>
+    <t>Altura</t>
+  </si>
+  <si>
+    <t>Peso</t>
+  </si>
+  <si>
+    <t>Pressão Arterial Sistólica</t>
+  </si>
+  <si>
+    <t>Pressão Sanguínea Diastólica</t>
+  </si>
+  <si>
+    <t>Temperatura</t>
+  </si>
+  <si>
+    <t>Glicose</t>
+  </si>
+  <si>
+    <t>Circunferência Torácica</t>
+  </si>
+  <si>
+    <t>Circunferência Craniana</t>
+  </si>
+  <si>
+    <t>Circunferência Abdominal</t>
+  </si>
+  <si>
+    <t>Número de Apgar</t>
+  </si>
+  <si>
+    <t>Sono</t>
+  </si>
+  <si>
+    <t>Thoracic Circumference</t>
+  </si>
+  <si>
+    <t>Head Circumference</t>
+  </si>
+  <si>
+    <t>Abdominal Circumference</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Auto</t>
+  </si>
+  <si>
+    <t>Clinical</t>
+  </si>
+  <si>
+    <t>Medic</t>
+  </si>
+  <si>
+    <t>Celsius</t>
+  </si>
+  <si>
+    <t>Meter</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>Centimeter</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>Liter</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>Milliliter</t>
+  </si>
+  <si>
+    <t>ml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kilogram </t>
+  </si>
+  <si>
+    <t>Degree</t>
+  </si>
+  <si>
+    <t>mmHg</t>
+  </si>
+  <si>
+    <t>Millimeters of Mercury</t>
+  </si>
+  <si>
+    <t>Apgar Score</t>
+  </si>
+  <si>
+    <t>Birth Weight</t>
+  </si>
+  <si>
+    <t>Peso ao Nascer</t>
+  </si>
+  <si>
+    <t>Birth Height</t>
+  </si>
+  <si>
+    <t>Comprimento ao Nascer</t>
+  </si>
+  <si>
+    <t>Metro</t>
+  </si>
+  <si>
+    <t>Quilograma</t>
+  </si>
+  <si>
+    <t>Centímetro</t>
+  </si>
+  <si>
+    <t>Litro</t>
+  </si>
+  <si>
+    <t>Mililitro</t>
+  </si>
+  <si>
+    <t>Grau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Milímetros de Mercúrio </t>
+  </si>
+  <si>
+    <t>Sigla</t>
+  </si>
+  <si>
+    <t>Unidade</t>
+  </si>
+  <si>
+    <t>mmol/L</t>
+  </si>
+  <si>
+    <t>Millimoles per Litre</t>
+  </si>
+  <si>
+    <t>Milligrams per 100 Millilitres</t>
+  </si>
+  <si>
+    <t>mg/dL</t>
+  </si>
+  <si>
+    <t>Milimoles por Litro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miligramas por 100 Mililitros </t>
+  </si>
+  <si>
+    <t>Grama</t>
+  </si>
+  <si>
+    <t>Gram</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>Nenhuma</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -1358,12 +1725,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1378,12 +1751,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1896,12 +2270,1628 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{391AE3A0-7DB7-4C1A-B882-6DBA4383A0D7}">
+  <dimension ref="A1:O55"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:O2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="3" max="4" width="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46.44140625" customWidth="1"/>
+    <col min="15" max="15" width="27.21875" customWidth="1"/>
+    <col min="16" max="16" width="9.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1" t="s">
+        <v>366</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>325</v>
+      </c>
+      <c r="B2" t="str">
+        <f>SUBSTITUTE(UPPER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(A2," ","_"),"ó","o"),"í","i")),"/","_")</f>
+        <v>BCG_ID</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>353</v>
+      </c>
+      <c r="F2" t="s">
+        <v>352</v>
+      </c>
+      <c r="G2" t="str">
+        <f>"(:VaccineDose {name: '" &amp; E2 &amp;"', vaccine: '" &amp; A2 &amp;"', fromAgeInMonths: toInteger(" &amp; C2 &amp;"), toAgeInMonths:toInteger(" &amp; D2 &amp;"), classification: '" &amp; F2 &amp;"'}),"</f>
+        <v>(:VaccineDose {name: 'Unique', vaccine: 'BCG ID', fromAgeInMonths: toInteger(1), toAgeInMonths:toInteger(1), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O2" t="str">
+        <f>"MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '" &amp; A2 &amp; "' AND d.vaccine = '" &amp; A2 &amp; "' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);"</f>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'BCG ID' AND d.vaccine = 'BCG ID' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>326</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B55" si="0">SUBSTITUTE(UPPER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(A3," ","_"),"ó","o"),"í","i")),"/","_")</f>
+        <v>HEPATITE_B</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>354</v>
+      </c>
+      <c r="F3" t="s">
+        <v>352</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G55" si="1">"(:VaccineDose {name: '" &amp; E3 &amp;"', vaccine: '" &amp; A3 &amp;"', fromAgeInMonths: toInteger(" &amp; C3 &amp;"), toAgeInMonths:toInteger(" &amp; D3 &amp;"), classification: '" &amp; F3 &amp;"'}),"</f>
+        <v>(:VaccineDose {name: '1st dose', vaccine: 'Hepatite B', fromAgeInMonths: toInteger(1), toAgeInMonths:toInteger(1), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O3" t="str">
+        <f t="shared" ref="O3:O55" si="2">"MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '" &amp; A3 &amp; "' AND d.vaccine = '" &amp; A3 &amp; "' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);"</f>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Hepatite B' AND d.vaccine = 'Hepatite B' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>326</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>HEPATITE_B</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>355</v>
+      </c>
+      <c r="F4" t="s">
+        <v>352</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: '2nd dose', vaccine: 'Hepatite B', fromAgeInMonths: toInteger(2), toAgeInMonths:toInteger(2), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O4" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Hepatite B' AND d.vaccine = 'Hepatite B' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>326</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>HEPATITE_B</v>
+      </c>
+      <c r="C5" s="1">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>357</v>
+      </c>
+      <c r="F5" t="s">
+        <v>352</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: '3rd dose', vaccine: 'Hepatite B', fromAgeInMonths: toInteger(6), toAgeInMonths:toInteger(6), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O5" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Hepatite B' AND d.vaccine = 'Hepatite B' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>364</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>DTPW</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>354</v>
+      </c>
+      <c r="F6" t="s">
+        <v>352</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: '1st dose', vaccine: 'DTPw', fromAgeInMonths: toInteger(2), toAgeInMonths:toInteger(2), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O6" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'DTPw' AND d.vaccine = 'DTPw' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>364</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>DTPW</v>
+      </c>
+      <c r="C7" s="1">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>355</v>
+      </c>
+      <c r="F7" t="s">
+        <v>352</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: '2nd dose', vaccine: 'DTPw', fromAgeInMonths: toInteger(4), toAgeInMonths:toInteger(4), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'DTPw' AND d.vaccine = 'DTPw' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>364</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>DTPW</v>
+      </c>
+      <c r="C8" s="1">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>357</v>
+      </c>
+      <c r="F8" t="s">
+        <v>352</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: '3rd dose', vaccine: 'DTPw', fromAgeInMonths: toInteger(6), toAgeInMonths:toInteger(6), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O8" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'DTPw' AND d.vaccine = 'DTPw' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>364</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>DTPW</v>
+      </c>
+      <c r="C9" s="1">
+        <v>15</v>
+      </c>
+      <c r="D9" s="1">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
+        <v>356</v>
+      </c>
+      <c r="F9" t="s">
+        <v>352</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: 'Booster', vaccine: 'DTPw', fromAgeInMonths: toInteger(15), toAgeInMonths:toInteger(18), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O9" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'DTPw' AND d.vaccine = 'DTPw' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>364</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>DTPW</v>
+      </c>
+      <c r="C10" s="1">
+        <v>48</v>
+      </c>
+      <c r="D10" s="1">
+        <v>60</v>
+      </c>
+      <c r="E10" t="s">
+        <v>356</v>
+      </c>
+      <c r="F10" t="s">
+        <v>352</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: 'Booster', vaccine: 'DTPw', fromAgeInMonths: toInteger(48), toAgeInMonths:toInteger(60), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O10" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'DTPw' AND d.vaccine = 'DTPw' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>367</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>H_INFLUENZAE</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>354</v>
+      </c>
+      <c r="F11" t="s">
+        <v>352</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: '1st dose', vaccine: 'H Influenzae', fromAgeInMonths: toInteger(2), toAgeInMonths:toInteger(2), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O11" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'H Influenzae' AND d.vaccine = 'H Influenzae' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>367</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>H_INFLUENZAE</v>
+      </c>
+      <c r="C12" s="1">
+        <v>4</v>
+      </c>
+      <c r="D12" s="1">
+        <v>4</v>
+      </c>
+      <c r="E12" t="s">
+        <v>355</v>
+      </c>
+      <c r="F12" t="s">
+        <v>352</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: '2nd dose', vaccine: 'H Influenzae', fromAgeInMonths: toInteger(4), toAgeInMonths:toInteger(4), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O12" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'H Influenzae' AND d.vaccine = 'H Influenzae' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>367</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>H_INFLUENZAE</v>
+      </c>
+      <c r="C13" s="1">
+        <v>6</v>
+      </c>
+      <c r="D13" s="1">
+        <v>6</v>
+      </c>
+      <c r="E13" t="s">
+        <v>357</v>
+      </c>
+      <c r="F13" t="s">
+        <v>352</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: '3rd dose', vaccine: 'H Influenzae', fromAgeInMonths: toInteger(6), toAgeInMonths:toInteger(6), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O13" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'H Influenzae' AND d.vaccine = 'H Influenzae' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>367</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>H_INFLUENZAE</v>
+      </c>
+      <c r="C14" s="1">
+        <v>15</v>
+      </c>
+      <c r="D14" s="1">
+        <v>18</v>
+      </c>
+      <c r="E14" t="s">
+        <v>356</v>
+      </c>
+      <c r="F14" t="s">
+        <v>352</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: 'Booster', vaccine: 'H Influenzae', fromAgeInMonths: toInteger(15), toAgeInMonths:toInteger(18), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O14" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'H Influenzae' AND d.vaccine = 'H Influenzae' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>327</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>POLIO_VIP</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>354</v>
+      </c>
+      <c r="F15" t="s">
+        <v>352</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: '1st dose', vaccine: 'Pólio VIP', fromAgeInMonths: toInteger(2), toAgeInMonths:toInteger(2), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O15" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Pólio VIP' AND d.vaccine = 'Pólio VIP' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>327</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>POLIO_VIP</v>
+      </c>
+      <c r="C16" s="1">
+        <v>4</v>
+      </c>
+      <c r="D16" s="1">
+        <v>4</v>
+      </c>
+      <c r="E16" t="s">
+        <v>355</v>
+      </c>
+      <c r="F16" t="s">
+        <v>352</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: '2nd dose', vaccine: 'Pólio VIP', fromAgeInMonths: toInteger(4), toAgeInMonths:toInteger(4), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O16" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Pólio VIP' AND d.vaccine = 'Pólio VIP' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>327</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>POLIO_VIP</v>
+      </c>
+      <c r="C17" s="1">
+        <v>6</v>
+      </c>
+      <c r="D17" s="1">
+        <v>6</v>
+      </c>
+      <c r="E17" t="s">
+        <v>357</v>
+      </c>
+      <c r="F17" t="s">
+        <v>352</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: '3rd dose', vaccine: 'Pólio VIP', fromAgeInMonths: toInteger(6), toAgeInMonths:toInteger(6), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O17" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Pólio VIP' AND d.vaccine = 'Pólio VIP' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>328</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>POLIO_VOP</v>
+      </c>
+      <c r="C18" s="1">
+        <v>15</v>
+      </c>
+      <c r="D18" s="1">
+        <v>18</v>
+      </c>
+      <c r="E18" t="s">
+        <v>356</v>
+      </c>
+      <c r="F18" t="s">
+        <v>352</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: 'Booster', vaccine: 'Pólio VOP', fromAgeInMonths: toInteger(15), toAgeInMonths:toInteger(18), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O18" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Pólio VOP' AND d.vaccine = 'Pólio VOP' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>328</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>POLIO_VOP</v>
+      </c>
+      <c r="C19" s="1">
+        <v>48</v>
+      </c>
+      <c r="D19" s="1">
+        <v>60</v>
+      </c>
+      <c r="E19" t="s">
+        <v>356</v>
+      </c>
+      <c r="F19" t="s">
+        <v>352</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: 'Booster', vaccine: 'Pólio VOP', fromAgeInMonths: toInteger(48), toAgeInMonths:toInteger(60), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O19" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Pólio VOP' AND d.vaccine = 'Pólio VOP' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>329</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>ROTAVIRUS</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1">
+        <v>4</v>
+      </c>
+      <c r="E20" t="s">
+        <v>354</v>
+      </c>
+      <c r="F20" t="s">
+        <v>352</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: '1st dose', vaccine: 'Rotavírus', fromAgeInMonths: toInteger(2), toAgeInMonths:toInteger(4), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O20" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Rotavírus' AND d.vaccine = 'Rotavírus' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>329</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>ROTAVIRUS</v>
+      </c>
+      <c r="C21" s="1">
+        <v>5</v>
+      </c>
+      <c r="D21" s="1">
+        <v>8</v>
+      </c>
+      <c r="E21" t="s">
+        <v>355</v>
+      </c>
+      <c r="F21" t="s">
+        <v>352</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: '2nd dose', vaccine: 'Rotavírus', fromAgeInMonths: toInteger(5), toAgeInMonths:toInteger(8), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O21" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Rotavírus' AND d.vaccine = 'Rotavírus' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>330</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>VPC10</v>
+      </c>
+      <c r="C22" s="1">
+        <v>2</v>
+      </c>
+      <c r="D22" s="1">
+        <v>3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>354</v>
+      </c>
+      <c r="F22" t="s">
+        <v>352</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: '1st dose', vaccine: 'VPC10', fromAgeInMonths: toInteger(2), toAgeInMonths:toInteger(3), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O22" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'VPC10' AND d.vaccine = 'VPC10' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>330</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>VPC10</v>
+      </c>
+      <c r="C23" s="1">
+        <v>4</v>
+      </c>
+      <c r="D23" s="1">
+        <v>6</v>
+      </c>
+      <c r="E23" t="s">
+        <v>355</v>
+      </c>
+      <c r="F23" t="s">
+        <v>352</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: '2nd dose', vaccine: 'VPC10', fromAgeInMonths: toInteger(4), toAgeInMonths:toInteger(6), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O23" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'VPC10' AND d.vaccine = 'VPC10' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>330</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>VPC10</v>
+      </c>
+      <c r="C24" s="1">
+        <v>12</v>
+      </c>
+      <c r="D24" s="1">
+        <v>15</v>
+      </c>
+      <c r="E24" t="s">
+        <v>356</v>
+      </c>
+      <c r="F24" t="s">
+        <v>352</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: 'Booster', vaccine: 'VPC10', fromAgeInMonths: toInteger(12), toAgeInMonths:toInteger(15), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O24" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'VPC10' AND d.vaccine = 'VPC10' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>331</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>ACWY_C</v>
+      </c>
+      <c r="C25" s="1">
+        <v>3</v>
+      </c>
+      <c r="D25" s="1">
+        <v>5</v>
+      </c>
+      <c r="E25" t="s">
+        <v>354</v>
+      </c>
+      <c r="F25" t="s">
+        <v>352</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: '1st dose', vaccine: 'ACWY/C', fromAgeInMonths: toInteger(3), toAgeInMonths:toInteger(5), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O25" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'ACWY/C' AND d.vaccine = 'ACWY/C' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>331</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>ACWY_C</v>
+      </c>
+      <c r="C26" s="1">
+        <v>6</v>
+      </c>
+      <c r="D26" s="1">
+        <v>8</v>
+      </c>
+      <c r="E26" t="s">
+        <v>355</v>
+      </c>
+      <c r="F26" t="s">
+        <v>352</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: '2nd dose', vaccine: 'ACWY/C', fromAgeInMonths: toInteger(6), toAgeInMonths:toInteger(8), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O26" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'ACWY/C' AND d.vaccine = 'ACWY/C' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>331</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>ACWY_C</v>
+      </c>
+      <c r="C27" s="1">
+        <v>12</v>
+      </c>
+      <c r="D27" s="1">
+        <v>15</v>
+      </c>
+      <c r="E27" t="s">
+        <v>356</v>
+      </c>
+      <c r="F27" t="s">
+        <v>352</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: 'Booster', vaccine: 'ACWY/C', fromAgeInMonths: toInteger(12), toAgeInMonths:toInteger(15), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O27" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'ACWY/C' AND d.vaccine = 'ACWY/C' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>331</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>ACWY_C</v>
+      </c>
+      <c r="C28" s="1">
+        <v>60</v>
+      </c>
+      <c r="D28" s="1">
+        <v>72</v>
+      </c>
+      <c r="E28" t="s">
+        <v>356</v>
+      </c>
+      <c r="F28" t="s">
+        <v>359</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: 'Booster', vaccine: 'ACWY/C', fromAgeInMonths: toInteger(60), toAgeInMonths:toInteger(72), classification: 'Optional'}),</v>
+      </c>
+      <c r="O28" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'ACWY/C' AND d.vaccine = 'ACWY/C' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>332</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>MENINGOCOCICA_B</v>
+      </c>
+      <c r="C29" s="1">
+        <v>3</v>
+      </c>
+      <c r="D29" s="1">
+        <v>3</v>
+      </c>
+      <c r="E29" t="s">
+        <v>354</v>
+      </c>
+      <c r="F29" t="s">
+        <v>352</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: '1st dose', vaccine: 'Meningocócica B', fromAgeInMonths: toInteger(3), toAgeInMonths:toInteger(3), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O29" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Meningocócica B' AND d.vaccine = 'Meningocócica B' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>332</v>
+      </c>
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>MENINGOCOCICA_B</v>
+      </c>
+      <c r="C30" s="1">
+        <v>5</v>
+      </c>
+      <c r="D30" s="1">
+        <v>5</v>
+      </c>
+      <c r="E30" t="s">
+        <v>355</v>
+      </c>
+      <c r="F30" t="s">
+        <v>352</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: '2nd dose', vaccine: 'Meningocócica B', fromAgeInMonths: toInteger(5), toAgeInMonths:toInteger(5), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O30" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Meningocócica B' AND d.vaccine = 'Meningocócica B' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>332</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>MENINGOCOCICA_B</v>
+      </c>
+      <c r="C31" s="1">
+        <v>12</v>
+      </c>
+      <c r="D31" s="1">
+        <v>15</v>
+      </c>
+      <c r="E31" t="s">
+        <v>356</v>
+      </c>
+      <c r="F31" t="s">
+        <v>352</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: 'Booster', vaccine: 'Meningocócica B', fromAgeInMonths: toInteger(12), toAgeInMonths:toInteger(15), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O31" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Meningocócica B' AND d.vaccine = 'Meningocócica B' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>333</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>3V</v>
+      </c>
+      <c r="C32" s="1">
+        <v>6</v>
+      </c>
+      <c r="D32" s="1">
+        <v>12</v>
+      </c>
+      <c r="E32" t="s">
+        <v>358</v>
+      </c>
+      <c r="F32" t="s">
+        <v>352</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: 'Annual', vaccine: '3V', fromAgeInMonths: toInteger(6), toAgeInMonths:toInteger(12), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O32" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '3V' AND d.vaccine = '3V' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>333</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>3V</v>
+      </c>
+      <c r="C33" s="1">
+        <v>13</v>
+      </c>
+      <c r="D33" s="1">
+        <v>24</v>
+      </c>
+      <c r="E33" t="s">
+        <v>358</v>
+      </c>
+      <c r="F33" t="s">
+        <v>352</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: 'Annual', vaccine: '3V', fromAgeInMonths: toInteger(13), toAgeInMonths:toInteger(24), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O33" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '3V' AND d.vaccine = '3V' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>333</v>
+      </c>
+      <c r="B34" t="str">
+        <f>SUBSTITUTE(UPPER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(A34," ","_"),"ó","o"),"í","i")),"/","_")</f>
+        <v>3V</v>
+      </c>
+      <c r="C34" s="1">
+        <v>25</v>
+      </c>
+      <c r="D34" s="1">
+        <v>36</v>
+      </c>
+      <c r="E34" t="s">
+        <v>358</v>
+      </c>
+      <c r="F34" t="s">
+        <v>352</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: 'Annual', vaccine: '3V', fromAgeInMonths: toInteger(25), toAgeInMonths:toInteger(36), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O34" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '3V' AND d.vaccine = '3V' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>333</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>3V</v>
+      </c>
+      <c r="C35" s="1">
+        <v>37</v>
+      </c>
+      <c r="D35" s="1">
+        <v>48</v>
+      </c>
+      <c r="E35" t="s">
+        <v>358</v>
+      </c>
+      <c r="F35" t="s">
+        <v>352</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: 'Annual', vaccine: '3V', fromAgeInMonths: toInteger(37), toAgeInMonths:toInteger(48), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O35" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '3V' AND d.vaccine = '3V' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>333</v>
+      </c>
+      <c r="B36" t="str">
+        <f t="shared" si="0"/>
+        <v>3V</v>
+      </c>
+      <c r="C36" s="1">
+        <v>49</v>
+      </c>
+      <c r="D36" s="1">
+        <v>60</v>
+      </c>
+      <c r="E36" t="s">
+        <v>358</v>
+      </c>
+      <c r="F36" t="s">
+        <v>352</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: 'Annual', vaccine: '3V', fromAgeInMonths: toInteger(49), toAgeInMonths:toInteger(60), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O36" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '3V' AND d.vaccine = '3V' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>333</v>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v>3V</v>
+      </c>
+      <c r="C37" s="1">
+        <v>61</v>
+      </c>
+      <c r="D37" s="1">
+        <v>72</v>
+      </c>
+      <c r="E37" t="s">
+        <v>358</v>
+      </c>
+      <c r="F37" t="s">
+        <v>352</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: 'Annual', vaccine: '3V', fromAgeInMonths: toInteger(61), toAgeInMonths:toInteger(72), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O37" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '3V' AND d.vaccine = '3V' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>333</v>
+      </c>
+      <c r="B38" t="str">
+        <f t="shared" si="0"/>
+        <v>3V</v>
+      </c>
+      <c r="C38" s="1">
+        <v>73</v>
+      </c>
+      <c r="D38" s="1">
+        <v>84</v>
+      </c>
+      <c r="E38" t="s">
+        <v>358</v>
+      </c>
+      <c r="F38" t="s">
+        <v>352</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: 'Annual', vaccine: '3V', fromAgeInMonths: toInteger(73), toAgeInMonths:toInteger(84), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O38" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '3V' AND d.vaccine = '3V' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>333</v>
+      </c>
+      <c r="B39" t="str">
+        <f t="shared" si="0"/>
+        <v>3V</v>
+      </c>
+      <c r="C39" s="1">
+        <v>85</v>
+      </c>
+      <c r="D39" s="1">
+        <v>96</v>
+      </c>
+      <c r="E39" t="s">
+        <v>358</v>
+      </c>
+      <c r="F39" t="s">
+        <v>352</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: 'Annual', vaccine: '3V', fromAgeInMonths: toInteger(85), toAgeInMonths:toInteger(96), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O39" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '3V' AND d.vaccine = '3V' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>333</v>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" si="0"/>
+        <v>3V</v>
+      </c>
+      <c r="C40" s="1">
+        <v>97</v>
+      </c>
+      <c r="D40" s="1">
+        <v>108</v>
+      </c>
+      <c r="E40" t="s">
+        <v>358</v>
+      </c>
+      <c r="F40" t="s">
+        <v>352</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: 'Annual', vaccine: '3V', fromAgeInMonths: toInteger(97), toAgeInMonths:toInteger(108), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O40" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '3V' AND d.vaccine = '3V' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>333</v>
+      </c>
+      <c r="B41" t="str">
+        <f t="shared" si="0"/>
+        <v>3V</v>
+      </c>
+      <c r="C41" s="1">
+        <v>109</v>
+      </c>
+      <c r="D41" s="1">
+        <v>120</v>
+      </c>
+      <c r="E41" t="s">
+        <v>358</v>
+      </c>
+      <c r="F41" t="s">
+        <v>352</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: 'Annual', vaccine: '3V', fromAgeInMonths: toInteger(109), toAgeInMonths:toInteger(120), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O41" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '3V' AND d.vaccine = '3V' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>334</v>
+      </c>
+      <c r="B42" t="str">
+        <f t="shared" si="0"/>
+        <v>FEBRE_AMARELA</v>
+      </c>
+      <c r="C42" s="1">
+        <v>9</v>
+      </c>
+      <c r="D42" s="1">
+        <v>9</v>
+      </c>
+      <c r="E42" t="s">
+        <v>353</v>
+      </c>
+      <c r="F42" t="s">
+        <v>352</v>
+      </c>
+      <c r="G42" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: 'Unique', vaccine: 'Febre amarela', fromAgeInMonths: toInteger(9), toAgeInMonths:toInteger(9), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O42" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Febre amarela' AND d.vaccine = 'Febre amarela' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>335</v>
+      </c>
+      <c r="B43" t="str">
+        <f t="shared" si="0"/>
+        <v>HEPATITE_A</v>
+      </c>
+      <c r="C43" s="1">
+        <v>12</v>
+      </c>
+      <c r="D43" s="1">
+        <v>12</v>
+      </c>
+      <c r="E43" t="s">
+        <v>354</v>
+      </c>
+      <c r="F43" t="s">
+        <v>352</v>
+      </c>
+      <c r="G43" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: '1st dose', vaccine: 'Hepatite A', fromAgeInMonths: toInteger(12), toAgeInMonths:toInteger(12), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O43" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Hepatite A' AND d.vaccine = 'Hepatite A' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>335</v>
+      </c>
+      <c r="B44" t="str">
+        <f t="shared" si="0"/>
+        <v>HEPATITE_A</v>
+      </c>
+      <c r="C44" s="1">
+        <v>18</v>
+      </c>
+      <c r="D44" s="1">
+        <v>18</v>
+      </c>
+      <c r="E44" t="s">
+        <v>355</v>
+      </c>
+      <c r="F44" t="s">
+        <v>352</v>
+      </c>
+      <c r="G44" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: '2nd dose', vaccine: 'Hepatite A', fromAgeInMonths: toInteger(18), toAgeInMonths:toInteger(18), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O44" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Hepatite A' AND d.vaccine = 'Hepatite A' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>336</v>
+      </c>
+      <c r="B45" t="str">
+        <f t="shared" si="0"/>
+        <v>BCG</v>
+      </c>
+      <c r="C45" s="1">
+        <v>12</v>
+      </c>
+      <c r="D45" s="1">
+        <v>12</v>
+      </c>
+      <c r="E45" t="s">
+        <v>354</v>
+      </c>
+      <c r="F45" t="s">
+        <v>352</v>
+      </c>
+      <c r="G45" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: '1st dose', vaccine: 'BCG', fromAgeInMonths: toInteger(12), toAgeInMonths:toInteger(12), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O45" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'BCG' AND d.vaccine = 'BCG' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>336</v>
+      </c>
+      <c r="B46" t="str">
+        <f t="shared" si="0"/>
+        <v>BCG</v>
+      </c>
+      <c r="C46" s="1">
+        <v>15</v>
+      </c>
+      <c r="D46" s="1">
+        <v>24</v>
+      </c>
+      <c r="E46" t="s">
+        <v>355</v>
+      </c>
+      <c r="F46" t="s">
+        <v>352</v>
+      </c>
+      <c r="G46" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: '2nd dose', vaccine: 'BCG', fromAgeInMonths: toInteger(15), toAgeInMonths:toInteger(24), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O46" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'BCG' AND d.vaccine = 'BCG' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>337</v>
+      </c>
+      <c r="B47" t="str">
+        <f t="shared" si="0"/>
+        <v>VARICELA</v>
+      </c>
+      <c r="C47" s="1">
+        <v>12</v>
+      </c>
+      <c r="D47" s="1">
+        <v>12</v>
+      </c>
+      <c r="E47" t="s">
+        <v>354</v>
+      </c>
+      <c r="F47" t="s">
+        <v>352</v>
+      </c>
+      <c r="G47" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: '1st dose', vaccine: 'Varicela', fromAgeInMonths: toInteger(12), toAgeInMonths:toInteger(12), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O47" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Varicela' AND d.vaccine = 'Varicela' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>337</v>
+      </c>
+      <c r="B48" t="str">
+        <f t="shared" si="0"/>
+        <v>VARICELA</v>
+      </c>
+      <c r="C48" s="1">
+        <v>15</v>
+      </c>
+      <c r="D48" s="1">
+        <v>24</v>
+      </c>
+      <c r="E48" t="s">
+        <v>355</v>
+      </c>
+      <c r="F48" t="s">
+        <v>352</v>
+      </c>
+      <c r="G48" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: '2nd dose', vaccine: 'Varicela', fromAgeInMonths: toInteger(15), toAgeInMonths:toInteger(24), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O48" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Varicela' AND d.vaccine = 'Varicela' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>338</v>
+      </c>
+      <c r="B49" t="str">
+        <f t="shared" si="0"/>
+        <v>HPV4</v>
+      </c>
+      <c r="C49" s="1">
+        <v>108</v>
+      </c>
+      <c r="D49" s="1">
+        <v>119</v>
+      </c>
+      <c r="E49" t="s">
+        <v>354</v>
+      </c>
+      <c r="F49" t="s">
+        <v>352</v>
+      </c>
+      <c r="G49" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: '1st dose', vaccine: 'HPV4', fromAgeInMonths: toInteger(108), toAgeInMonths:toInteger(119), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O49" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'HPV4' AND d.vaccine = 'HPV4' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>338</v>
+      </c>
+      <c r="B50" t="str">
+        <f t="shared" si="0"/>
+        <v>HPV4</v>
+      </c>
+      <c r="C50" s="1">
+        <v>120</v>
+      </c>
+      <c r="D50" s="1">
+        <v>132</v>
+      </c>
+      <c r="E50" t="s">
+        <v>355</v>
+      </c>
+      <c r="F50" t="s">
+        <v>352</v>
+      </c>
+      <c r="G50" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: '2nd dose', vaccine: 'HPV4', fromAgeInMonths: toInteger(120), toAgeInMonths:toInteger(132), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O50" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'HPV4' AND d.vaccine = 'HPV4' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>365</v>
+      </c>
+      <c r="B51" t="str">
+        <f t="shared" si="0"/>
+        <v>DTPA</v>
+      </c>
+      <c r="C51" s="1">
+        <v>2</v>
+      </c>
+      <c r="D51" s="1">
+        <v>2</v>
+      </c>
+      <c r="E51" t="s">
+        <v>354</v>
+      </c>
+      <c r="F51" t="s">
+        <v>352</v>
+      </c>
+      <c r="G51" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: '1st dose', vaccine: 'DTPa', fromAgeInMonths: toInteger(2), toAgeInMonths:toInteger(2), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O51" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'DTPa' AND d.vaccine = 'DTPa' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>365</v>
+      </c>
+      <c r="B52" t="str">
+        <f t="shared" si="0"/>
+        <v>DTPA</v>
+      </c>
+      <c r="C52" s="1">
+        <v>4</v>
+      </c>
+      <c r="D52" s="1">
+        <v>4</v>
+      </c>
+      <c r="E52" t="s">
+        <v>355</v>
+      </c>
+      <c r="F52" t="s">
+        <v>352</v>
+      </c>
+      <c r="G52" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: '2nd dose', vaccine: 'DTPa', fromAgeInMonths: toInteger(4), toAgeInMonths:toInteger(4), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O52" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'DTPa' AND d.vaccine = 'DTPa' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>365</v>
+      </c>
+      <c r="B53" t="str">
+        <f t="shared" si="0"/>
+        <v>DTPA</v>
+      </c>
+      <c r="C53" s="1">
+        <v>6</v>
+      </c>
+      <c r="D53" s="1">
+        <v>6</v>
+      </c>
+      <c r="E53" t="s">
+        <v>357</v>
+      </c>
+      <c r="F53" t="s">
+        <v>352</v>
+      </c>
+      <c r="G53" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: '3rd dose', vaccine: 'DTPa', fromAgeInMonths: toInteger(6), toAgeInMonths:toInteger(6), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O53" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'DTPa' AND d.vaccine = 'DTPa' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>365</v>
+      </c>
+      <c r="B54" t="str">
+        <f t="shared" si="0"/>
+        <v>DTPA</v>
+      </c>
+      <c r="C54" s="1">
+        <v>15</v>
+      </c>
+      <c r="D54" s="1">
+        <v>18</v>
+      </c>
+      <c r="E54" t="s">
+        <v>356</v>
+      </c>
+      <c r="F54" t="s">
+        <v>352</v>
+      </c>
+      <c r="G54" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: 'Booster', vaccine: 'DTPa', fromAgeInMonths: toInteger(15), toAgeInMonths:toInteger(18), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O54" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'DTPa' AND d.vaccine = 'DTPa' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>365</v>
+      </c>
+      <c r="B55" t="str">
+        <f t="shared" si="0"/>
+        <v>DTPA</v>
+      </c>
+      <c r="C55" s="1">
+        <v>48</v>
+      </c>
+      <c r="D55" s="1">
+        <v>60</v>
+      </c>
+      <c r="E55" t="s">
+        <v>356</v>
+      </c>
+      <c r="F55" t="s">
+        <v>352</v>
+      </c>
+      <c r="G55" t="str">
+        <f t="shared" si="1"/>
+        <v>(:VaccineDose {name: 'Booster', vaccine: 'DTPa', fromAgeInMonths: toInteger(48), toAgeInMonths:toInteger(60), classification: 'Mandatory'}),</v>
+      </c>
+      <c r="O55" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'DTPa' AND d.vaccine = 'DTPa' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16822055-6D7C-4562-869B-B3AD28812FB9}">
-  <dimension ref="A1:D97"/>
+  <dimension ref="A1:D98"/>
   <sheetViews>
     <sheetView topLeftCell="A79" zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
-      <selection activeCell="D92" sqref="D92:D97"/>
+      <selection activeCell="D98" sqref="D98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2701,7 +4691,7 @@
         <v>165</v>
       </c>
       <c r="D66" t="str">
-        <f t="shared" ref="D66:D97" si="1">"(:Disease {uuid: apoc.create.uuid(), name: '" &amp; B66 &amp;"', inPortuguese: '" &amp; A66 &amp;"'}),"</f>
+        <f t="shared" ref="D66:D98" si="1">"(:Disease {uuid: apoc.create.uuid(), name: '" &amp; B66 &amp;"', inPortuguese: '" &amp; A66 &amp;"'}),"</f>
         <v>(:Disease {uuid: apoc.create.uuid(), name: 'Tendonitis', inPortuguese: 'Tendinite'}),</v>
       </c>
     </row>
@@ -3075,6 +5065,18 @@
       <c r="D97" t="str">
         <f t="shared" si="1"/>
         <v>(:Disease {uuid: apoc.create.uuid(), name: 'Chikungunya ', inPortuguese: 'Chikungunya '}),</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>487</v>
+      </c>
+      <c r="B98" t="s">
+        <v>486</v>
+      </c>
+      <c r="D98" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Disease {uuid: apoc.create.uuid(), name: 'Fibromyalgia', inPortuguese: 'Fibromialgia'}),</v>
       </c>
     </row>
   </sheetData>
@@ -4770,10 +6772,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7A3E379-11D0-4971-86BE-FD970275DE12}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4781,20 +6783,27 @@
     <col min="1" max="1" width="13.77734375" customWidth="1"/>
     <col min="2" max="2" width="13.44140625" customWidth="1"/>
     <col min="3" max="3" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>433</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>432</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="L1" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>290</v>
       </c>
@@ -4805,8 +6814,14 @@
         <f>"(:Symptom {uuid: apoc.create.uuid(), name: '" &amp; B2 &amp;"', inPortuguese: '" &amp; A2 &amp;"'}),"</f>
         <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Cry', inPortuguese: 'Choro'}),</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="L2" t="s">
+        <v>442</v>
+      </c>
+      <c r="M2" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>291</v>
       </c>
@@ -4817,8 +6832,14 @@
         <f t="shared" ref="C3:C26" si="0">"(:Symptom {uuid: apoc.create.uuid(), name: '" &amp; B3 &amp;"', inPortuguese: '" &amp; A3 &amp;"'}),"</f>
         <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Fever', inPortuguese: 'Febre'}),</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="L3" t="s">
+        <v>443</v>
+      </c>
+      <c r="M3" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>292</v>
       </c>
@@ -4829,8 +6850,14 @@
         <f t="shared" si="0"/>
         <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Vomit', inPortuguese: 'Vômito'}),</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="L4" t="s">
+        <v>449</v>
+      </c>
+      <c r="M4" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>406</v>
       </c>
@@ -4841,8 +6868,14 @@
         <f t="shared" si="0"/>
         <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Diarrhea', inPortuguese: 'Diarréia'}),</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="L5" t="s">
+        <v>479</v>
+      </c>
+      <c r="M5" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>294</v>
       </c>
@@ -4853,8 +6886,14 @@
         <f t="shared" si="0"/>
         <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Coryza', inPortuguese: 'Coriza'}),</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="L6" t="s">
+        <v>391</v>
+      </c>
+      <c r="M6" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>295</v>
       </c>
@@ -4865,8 +6904,14 @@
         <f t="shared" si="0"/>
         <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Stress', inPortuguese: 'Estresse'}),</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="L7" t="s">
+        <v>444</v>
+      </c>
+      <c r="M7" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>296</v>
       </c>
@@ -4877,8 +6922,14 @@
         <f t="shared" si="0"/>
         <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Cough', inPortuguese: 'Tosse'}),</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="L8" t="s">
+        <v>445</v>
+      </c>
+      <c r="M8" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>297</v>
       </c>
@@ -4889,8 +6940,14 @@
         <f t="shared" si="0"/>
         <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Sneeze', inPortuguese: 'Espirro'}),</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="L9" t="s">
+        <v>440</v>
+      </c>
+      <c r="M9" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>298</v>
       </c>
@@ -4901,8 +6958,14 @@
         <f t="shared" si="0"/>
         <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Nausea', inPortuguese: 'Náusea'}),</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="L10" t="s">
+        <v>446</v>
+      </c>
+      <c r="M10" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>300</v>
       </c>
@@ -4913,8 +6976,14 @@
         <f t="shared" si="0"/>
         <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Vertigo', inPortuguese: 'Vertigem'}),</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="L11" t="s">
+        <v>450</v>
+      </c>
+      <c r="M11" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>407</v>
       </c>
@@ -4925,8 +6994,14 @@
         <f t="shared" si="0"/>
         <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Choke', inPortuguese: 'Engasgo'}),</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="L12" t="s">
+        <v>451</v>
+      </c>
+      <c r="M12" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>304</v>
       </c>
@@ -4937,20 +7012,37 @@
         <f t="shared" si="0"/>
         <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Weakness', inPortuguese: 'Fraqueza'}),</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="L13" t="s">
+        <v>452</v>
+      </c>
+      <c r="M13" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>408</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="C14" t="str">
+      <c r="C14" s="3" t="str">
         <f t="shared" si="0"/>
         <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Pain', inPortuguese: 'Dor '}),</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="L14" t="s">
+        <v>453</v>
+      </c>
+      <c r="M14" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>410</v>
       </c>
@@ -4961,8 +7053,14 @@
         <f t="shared" si="0"/>
         <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Short of Breath', inPortuguese: 'Falta de Ar'}),</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="L15" t="s">
+        <v>458</v>
+      </c>
+      <c r="M15" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>411</v>
       </c>
@@ -4973,8 +7071,14 @@
         <f t="shared" si="0"/>
         <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Sweating', inPortuguese: 'Sudorese'}),</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="L16" t="s">
+        <v>476</v>
+      </c>
+      <c r="M16" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>413</v>
       </c>
@@ -4985,8 +7089,14 @@
         <f t="shared" si="0"/>
         <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Insomnia ', inPortuguese: 'Insônia'}),</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="L17" t="s">
+        <v>480</v>
+      </c>
+      <c r="M17" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>423</v>
       </c>
@@ -4997,8 +7107,14 @@
         <f t="shared" si="0"/>
         <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Dry Mouth', inPortuguese: 'Boca Seca'}),</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="L18" t="s">
+        <v>482</v>
+      </c>
+      <c r="M18" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>424</v>
       </c>
@@ -5010,7 +7126,7 @@
         <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Hoarseness', inPortuguese: 'Rouquidão '}),</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>420</v>
       </c>
@@ -5021,8 +7137,14 @@
         <f t="shared" si="0"/>
         <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Sense of Taste', inPortuguese: 'Perda do Paladar'}),</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="L20" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>422</v>
       </c>
@@ -5033,8 +7155,14 @@
         <f t="shared" si="0"/>
         <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Bad Breath', inPortuguese: 'Mau Hálito'}),</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="L21" t="s">
+        <v>467</v>
+      </c>
+      <c r="M21" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>421</v>
       </c>
@@ -5045,8 +7173,14 @@
         <f t="shared" si="0"/>
         <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Sense of Smell', inPortuguese: 'Perda do Olfato'}),</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="L22" t="s">
+        <v>468</v>
+      </c>
+      <c r="M22" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>425</v>
       </c>
@@ -5057,8 +7191,14 @@
         <f t="shared" si="0"/>
         <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Apenea', inPortuguese: 'Apenéia'}),</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="L23" t="s">
+        <v>469</v>
+      </c>
+      <c r="M23" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>427</v>
       </c>
@@ -5069,8 +7209,14 @@
         <f t="shared" si="0"/>
         <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Tremor', inPortuguese: 'Tremor'}),</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="L24" t="s">
+        <v>470</v>
+      </c>
+      <c r="M24" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>429</v>
       </c>
@@ -5081,8 +7227,14 @@
         <f t="shared" si="0"/>
         <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Dizziness', inPortuguese: 'Tontura'}),</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="L25" t="s">
+        <v>471</v>
+      </c>
+      <c r="M25" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>431</v>
       </c>
@@ -5093,143 +7245,382 @@
         <f t="shared" si="0"/>
         <v>(:Symptom {uuid: apoc.create.uuid(), name: 'Lack of Appetite', inPortuguese: 'Falta de Apetite'}),</v>
       </c>
+      <c r="L26" t="s">
+        <v>472</v>
+      </c>
+      <c r="M26" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L27" t="s">
+        <v>473</v>
+      </c>
+      <c r="M27" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L28" t="s">
+        <v>475</v>
+      </c>
+      <c r="M28" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L29" t="s">
+        <v>484</v>
+      </c>
+      <c r="M29" t="s">
+        <v>485</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F5CDE23-EAB5-47A7-B33D-96F18BE56CCE}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" customWidth="1"/>
-    <col min="3" max="3" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="17.77734375" customWidth="1"/>
+    <col min="3" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="30" customWidth="1"/>
+    <col min="11" max="11" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>488</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>489</v>
       </c>
       <c r="C1" t="s">
+        <v>510</v>
+      </c>
+      <c r="D1" t="s">
+        <v>542</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>290</v>
+        <v>496</v>
       </c>
       <c r="B2" t="s">
-        <v>307</v>
-      </c>
-      <c r="C2" t="str">
-        <f>"(:Measurement {name: '" &amp; B2 &amp;"', inPortuguese: '" &amp; A2 &amp;"'}),"</f>
-        <v>(:Measurement {name: 'Cry', inPortuguese: 'Choro'}),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C3" t="str">
-        <f t="shared" ref="C3:C18" si="0">"(:Measurement {name: '" &amp; B3 &amp;"', inPortuguese: '" &amp; A3 &amp;"'}),"</f>
-        <v>(:Measurement {name: '', inPortuguese: ''}),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C4" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Measurement {name: '', inPortuguese: ''}),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C5" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Measurement {name: '', inPortuguese: ''}),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C6" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Measurement {name: '', inPortuguese: ''}),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C7" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Measurement {name: '', inPortuguese: ''}),</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C8" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Measurement {name: '', inPortuguese: ''}),</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C9" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Measurement {name: '', inPortuguese: ''}),</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C10" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Measurement {name: '', inPortuguese: ''}),</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C11" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Measurement {name: '', inPortuguese: ''}),</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C12" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Measurement {name: '', inPortuguese: ''}),</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C13" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Measurement {name: '', inPortuguese: ''}),</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C14" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Measurement {name: '', inPortuguese: ''}),</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C15" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Measurement {name: '', inPortuguese: ''}),</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C16" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Measurement {name: '', inPortuguese: ''}),</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C17" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Measurement {name: '', inPortuguese: ''}),</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C18" t="str">
-        <f t="shared" si="0"/>
-        <v>(:Measurement {name: '', inPortuguese: ''}),</v>
+        <v>490</v>
+      </c>
+      <c r="C2" t="s">
+        <v>511</v>
+      </c>
+      <c r="D2" t="s">
+        <v>519</v>
+      </c>
+      <c r="E2" t="str">
+        <f>"(:Measurement {uuid: apoc.create.uuid(), name: '" &amp; B2 &amp;"', inPortuguese: '" &amp; A2 &amp;"', type: '" &amp; C2 &amp; "'}),"</f>
+        <v>(:Measurement {uuid: apoc.create.uuid(), name: 'Height', inPortuguese: 'Altura', type: 'Auto'}),</v>
+      </c>
+      <c r="K2" t="str">
+        <f>"MATCH (meas:Measurement), (unit:MeasurementUnit) WHERE meas.name = '" &amp; B2 &amp;"' AND unit.name = '" &amp; D2 &amp;"' MERGE (meas)-[:IS_MEASURED_IN]-&gt;(unit);"</f>
+        <v>MATCH (meas:Measurement), (unit:MeasurementUnit) WHERE meas.name = 'Height' AND unit.name = 'Centimeter' MERGE (meas)-[:IS_MEASURED_IN]-&gt;(unit);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>497</v>
+      </c>
+      <c r="B3" t="s">
+        <v>463</v>
+      </c>
+      <c r="C3" t="s">
+        <v>511</v>
+      </c>
+      <c r="D3" t="s">
+        <v>525</v>
+      </c>
+      <c r="E3" t="str">
+        <f>"(:Measurement {uuid: apoc.create.uuid(), name: '" &amp; B3 &amp;"', inPortuguese: '" &amp; A3 &amp;"', type: '" &amp; C3 &amp; "'}),"</f>
+        <v>(:Measurement {uuid: apoc.create.uuid(), name: 'Weight', inPortuguese: 'Peso', type: 'Auto'}),</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K17" si="0">"MATCH (meas:Measurement), (unit:MeasurementUnit) WHERE meas.name = '" &amp; B3 &amp;"' AND unit.name = '" &amp; D3 &amp;"' MERGE (meas)-[:IS_MEASURED_IN]-&gt;(unit);"</f>
+        <v>MATCH (meas:Measurement), (unit:MeasurementUnit) WHERE meas.name = 'Weight' AND unit.name = 'Kilogram ' MERGE (meas)-[:IS_MEASURED_IN]-&gt;(unit);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>498</v>
+      </c>
+      <c r="B4" t="s">
+        <v>491</v>
+      </c>
+      <c r="C4" t="s">
+        <v>511</v>
+      </c>
+      <c r="D4" t="s">
+        <v>528</v>
+      </c>
+      <c r="E4" t="str">
+        <f>"(:Measurement {uuid: apoc.create.uuid(), name: '" &amp; B4 &amp;"', inPortuguese: '" &amp; A4 &amp;"', type: '" &amp; C4 &amp; "'}),"</f>
+        <v>(:Measurement {uuid: apoc.create.uuid(), name: 'Systolic Blood Pressure', inPortuguese: 'Pressão Arterial Sistólica', type: 'Auto'}),</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="0"/>
+        <v>MATCH (meas:Measurement), (unit:MeasurementUnit) WHERE meas.name = 'Systolic Blood Pressure' AND unit.name = 'Millimeters of Mercury' MERGE (meas)-[:IS_MEASURED_IN]-&gt;(unit);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>499</v>
+      </c>
+      <c r="B5" t="s">
+        <v>492</v>
+      </c>
+      <c r="C5" t="s">
+        <v>511</v>
+      </c>
+      <c r="D5" t="s">
+        <v>528</v>
+      </c>
+      <c r="E5" t="str">
+        <f>"(:Measurement {uuid: apoc.create.uuid(), name: '" &amp; B5 &amp;"', inPortuguese: '" &amp; A5 &amp;"', type: '" &amp; C5 &amp; "'}),"</f>
+        <v>(:Measurement {uuid: apoc.create.uuid(), name: 'Diastolic Blood Pressure', inPortuguese: 'Pressão Sanguínea Diastólica', type: 'Auto'}),</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="0"/>
+        <v>MATCH (meas:Measurement), (unit:MeasurementUnit) WHERE meas.name = 'Diastolic Blood Pressure' AND unit.name = 'Millimeters of Mercury' MERGE (meas)-[:IS_MEASURED_IN]-&gt;(unit);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>500</v>
+      </c>
+      <c r="B6" t="s">
+        <v>493</v>
+      </c>
+      <c r="C6" t="s">
+        <v>511</v>
+      </c>
+      <c r="D6" t="s">
+        <v>514</v>
+      </c>
+      <c r="E6" t="str">
+        <f>"(:Measurement {uuid: apoc.create.uuid(), name: '" &amp; B6 &amp;"', inPortuguese: '" &amp; A6 &amp;"', type: '" &amp; C6 &amp; "'}),"</f>
+        <v>(:Measurement {uuid: apoc.create.uuid(), name: 'Temperature', inPortuguese: 'Temperatura', type: 'Auto'}),</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="0"/>
+        <v>MATCH (meas:Measurement), (unit:MeasurementUnit) WHERE meas.name = 'Temperature' AND unit.name = 'Celsius' MERGE (meas)-[:IS_MEASURED_IN]-&gt;(unit);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>506</v>
+      </c>
+      <c r="B7" t="s">
+        <v>494</v>
+      </c>
+      <c r="C7" t="s">
+        <v>511</v>
+      </c>
+      <c r="D7" t="s">
+        <v>553</v>
+      </c>
+      <c r="E7" t="str">
+        <f>"(:Measurement {uuid: apoc.create.uuid(), name: '" &amp; B7 &amp;"', inPortuguese: '" &amp; A7 &amp;"', type: '" &amp; C7 &amp; "'}),"</f>
+        <v>(:Measurement {uuid: apoc.create.uuid(), name: 'Sleep', inPortuguese: 'Sono', type: 'Auto'}),</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="0"/>
+        <v>MATCH (meas:Measurement), (unit:MeasurementUnit) WHERE meas.name = 'Sleep' AND unit.name = 'None' MERGE (meas)-[:IS_MEASURED_IN]-&gt;(unit);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>295</v>
+      </c>
+      <c r="B8" t="s">
+        <v>312</v>
+      </c>
+      <c r="C8" t="s">
+        <v>511</v>
+      </c>
+      <c r="D8" t="s">
+        <v>553</v>
+      </c>
+      <c r="E8" t="str">
+        <f>"(:Measurement {uuid: apoc.create.uuid(), name: '" &amp; B8 &amp;"', inPortuguese: '" &amp; A8 &amp;"', type: '" &amp; C8 &amp; "'}),"</f>
+        <v>(:Measurement {uuid: apoc.create.uuid(), name: 'Stress', inPortuguese: 'Estresse', type: 'Auto'}),</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="0"/>
+        <v>MATCH (meas:Measurement), (unit:MeasurementUnit) WHERE meas.name = 'Stress' AND unit.name = 'None' MERGE (meas)-[:IS_MEASURED_IN]-&gt;(unit);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>501</v>
+      </c>
+      <c r="B9" t="s">
+        <v>495</v>
+      </c>
+      <c r="C9" t="s">
+        <v>512</v>
+      </c>
+      <c r="D9" t="s">
+        <v>544</v>
+      </c>
+      <c r="E9" t="str">
+        <f>"(:Measurement {uuid: apoc.create.uuid(), name: '" &amp; B9 &amp;"', inPortuguese: '" &amp; A9 &amp;"', type: '" &amp; C9 &amp; "'}),"</f>
+        <v>(:Measurement {uuid: apoc.create.uuid(), name: 'Glucose', inPortuguese: 'Glicose', type: 'Clinical'}),</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="0"/>
+        <v>MATCH (meas:Measurement), (unit:MeasurementUnit) WHERE meas.name = 'Glucose' AND unit.name = 'Millimoles per Litre' MERGE (meas)-[:IS_MEASURED_IN]-&gt;(unit);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>505</v>
+      </c>
+      <c r="B10" t="s">
+        <v>529</v>
+      </c>
+      <c r="C10" t="s">
+        <v>513</v>
+      </c>
+      <c r="D10" t="s">
+        <v>553</v>
+      </c>
+      <c r="E10" t="str">
+        <f>"(:Measurement {uuid: apoc.create.uuid(), name: '" &amp; B10 &amp;"', inPortuguese: '" &amp; A10 &amp;"', type: '" &amp; C10 &amp; "'}),"</f>
+        <v>(:Measurement {uuid: apoc.create.uuid(), name: 'Apgar Score', inPortuguese: 'Número de Apgar', type: 'Medic'}),</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="0"/>
+        <v>MATCH (meas:Measurement), (unit:MeasurementUnit) WHERE meas.name = 'Apgar Score' AND unit.name = 'None' MERGE (meas)-[:IS_MEASURED_IN]-&gt;(unit);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>502</v>
+      </c>
+      <c r="B11" t="s">
+        <v>507</v>
+      </c>
+      <c r="C11" t="s">
+        <v>513</v>
+      </c>
+      <c r="D11" t="s">
+        <v>519</v>
+      </c>
+      <c r="E11" t="str">
+        <f>"(:Measurement {uuid: apoc.create.uuid(), name: '" &amp; B11 &amp;"', inPortuguese: '" &amp; A11 &amp;"', type: '" &amp; C11 &amp; "'}),"</f>
+        <v>(:Measurement {uuid: apoc.create.uuid(), name: 'Thoracic Circumference', inPortuguese: 'Circunferência Torácica', type: 'Medic'}),</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="0"/>
+        <v>MATCH (meas:Measurement), (unit:MeasurementUnit) WHERE meas.name = 'Thoracic Circumference' AND unit.name = 'Centimeter' MERGE (meas)-[:IS_MEASURED_IN]-&gt;(unit);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>503</v>
+      </c>
+      <c r="B12" t="s">
+        <v>508</v>
+      </c>
+      <c r="C12" t="s">
+        <v>513</v>
+      </c>
+      <c r="D12" t="s">
+        <v>519</v>
+      </c>
+      <c r="E12" t="str">
+        <f>"(:Measurement {uuid: apoc.create.uuid(), name: '" &amp; B12 &amp;"', inPortuguese: '" &amp; A12 &amp;"', type: '" &amp; C12 &amp; "'}),"</f>
+        <v>(:Measurement {uuid: apoc.create.uuid(), name: 'Head Circumference', inPortuguese: 'Circunferência Craniana', type: 'Medic'}),</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="0"/>
+        <v>MATCH (meas:Measurement), (unit:MeasurementUnit) WHERE meas.name = 'Head Circumference' AND unit.name = 'Centimeter' MERGE (meas)-[:IS_MEASURED_IN]-&gt;(unit);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>504</v>
+      </c>
+      <c r="B13" t="s">
+        <v>509</v>
+      </c>
+      <c r="C13" t="s">
+        <v>513</v>
+      </c>
+      <c r="D13" t="s">
+        <v>519</v>
+      </c>
+      <c r="E13" t="str">
+        <f>"(:Measurement {uuid: apoc.create.uuid(), name: '" &amp; B13 &amp;"', inPortuguese: '" &amp; A13 &amp;"', type: '" &amp; C13 &amp; "'}),"</f>
+        <v>(:Measurement {uuid: apoc.create.uuid(), name: 'Abdominal Circumference', inPortuguese: 'Circunferência Abdominal', type: 'Medic'}),</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="0"/>
+        <v>MATCH (meas:Measurement), (unit:MeasurementUnit) WHERE meas.name = 'Abdominal Circumference' AND unit.name = 'Centimeter' MERGE (meas)-[:IS_MEASURED_IN]-&gt;(unit);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>531</v>
+      </c>
+      <c r="B14" t="s">
+        <v>530</v>
+      </c>
+      <c r="C14" t="s">
+        <v>513</v>
+      </c>
+      <c r="D14" t="s">
+        <v>550</v>
+      </c>
+      <c r="E14" t="str">
+        <f>"(:Measurement {uuid: apoc.create.uuid(), name: '" &amp; B14 &amp;"', inPortuguese: '" &amp; A14 &amp;"', type: '" &amp; C14 &amp; "'}),"</f>
+        <v>(:Measurement {uuid: apoc.create.uuid(), name: 'Birth Weight', inPortuguese: 'Peso ao Nascer', type: 'Medic'}),</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="0"/>
+        <v>MATCH (meas:Measurement), (unit:MeasurementUnit) WHERE meas.name = 'Birth Weight' AND unit.name = 'Gram' MERGE (meas)-[:IS_MEASURED_IN]-&gt;(unit);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>533</v>
+      </c>
+      <c r="B15" t="s">
+        <v>532</v>
+      </c>
+      <c r="C15" t="s">
+        <v>513</v>
+      </c>
+      <c r="D15" t="s">
+        <v>519</v>
+      </c>
+      <c r="E15" t="str">
+        <f>"(:Measurement {uuid: apoc.create.uuid(), name: '" &amp; B15 &amp;"', inPortuguese: '" &amp; A15 &amp;"', type: '" &amp; C15 &amp; "'}),"</f>
+        <v>(:Measurement {uuid: apoc.create.uuid(), name: 'Birth Height', inPortuguese: 'Comprimento ao Nascer', type: 'Medic'}),</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="0"/>
+        <v>MATCH (meas:Measurement), (unit:MeasurementUnit) WHERE meas.name = 'Birth Height' AND unit.name = 'Centimeter' MERGE (meas)-[:IS_MEASURED_IN]-&gt;(unit);</v>
       </c>
     </row>
   </sheetData>
@@ -5238,6 +7629,215 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58E23DBB-27F6-4A87-AFAA-C8781EFF9D8C}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>541</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>514</v>
+      </c>
+      <c r="B2" t="s">
+        <v>514</v>
+      </c>
+      <c r="C2" t="s">
+        <v>516</v>
+      </c>
+      <c r="D2" t="str">
+        <f>"(:MeasurementUnit {uuid: apoc.create.uuid(), name: '" &amp; B2 &amp;"', inPortuguese: '" &amp; A2 &amp;"', acronym : '"&amp; C2 &amp; "'}),"</f>
+        <v>(:MeasurementUnit {uuid: apoc.create.uuid(), name: 'Celsius', inPortuguese: 'Celsius', acronym : 'C'}),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>534</v>
+      </c>
+      <c r="B3" t="s">
+        <v>515</v>
+      </c>
+      <c r="C3" t="s">
+        <v>517</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D20" si="0">"(:MeasurementUnit {uuid: apoc.create.uuid(), name: '" &amp; B3 &amp;"', inPortuguese: '" &amp; A3 &amp;"', acronym : '"&amp; C3 &amp; "'}),"</f>
+        <v>(:MeasurementUnit {uuid: apoc.create.uuid(), name: 'Meter', inPortuguese: 'Metro', acronym : 'm'}),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>535</v>
+      </c>
+      <c r="B4" t="s">
+        <v>525</v>
+      </c>
+      <c r="C4" t="s">
+        <v>518</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>(:MeasurementUnit {uuid: apoc.create.uuid(), name: 'Kilogram ', inPortuguese: 'Quilograma', acronym : 'kg'}),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>536</v>
+      </c>
+      <c r="B5" t="s">
+        <v>519</v>
+      </c>
+      <c r="C5" t="s">
+        <v>520</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>(:MeasurementUnit {uuid: apoc.create.uuid(), name: 'Centimeter', inPortuguese: 'Centímetro', acronym : 'cm'}),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>537</v>
+      </c>
+      <c r="B6" t="s">
+        <v>521</v>
+      </c>
+      <c r="C6" t="s">
+        <v>522</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>(:MeasurementUnit {uuid: apoc.create.uuid(), name: 'Liter', inPortuguese: 'Litro', acronym : 'l'}),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>538</v>
+      </c>
+      <c r="B7" t="s">
+        <v>523</v>
+      </c>
+      <c r="C7" t="s">
+        <v>524</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>(:MeasurementUnit {uuid: apoc.create.uuid(), name: 'Milliliter', inPortuguese: 'Mililitro', acronym : 'ml'}),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>539</v>
+      </c>
+      <c r="B8" t="s">
+        <v>526</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>(:MeasurementUnit {uuid: apoc.create.uuid(), name: 'Degree', inPortuguese: 'Grau', acronym : ''}),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>540</v>
+      </c>
+      <c r="B9" t="s">
+        <v>528</v>
+      </c>
+      <c r="C9" t="s">
+        <v>527</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>(:MeasurementUnit {uuid: apoc.create.uuid(), name: 'Millimeters of Mercury', inPortuguese: 'Milímetros de Mercúrio ', acronym : 'mmHg'}),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>547</v>
+      </c>
+      <c r="B10" t="s">
+        <v>544</v>
+      </c>
+      <c r="C10" t="s">
+        <v>543</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>(:MeasurementUnit {uuid: apoc.create.uuid(), name: 'Millimoles per Litre', inPortuguese: 'Milimoles por Litro', acronym : 'mmol/L'}),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>548</v>
+      </c>
+      <c r="B11" t="s">
+        <v>545</v>
+      </c>
+      <c r="C11" t="s">
+        <v>546</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>(:MeasurementUnit {uuid: apoc.create.uuid(), name: 'Milligrams per 100 Millilitres', inPortuguese: 'Miligramas por 100 Mililitros ', acronym : 'mg/dL'}),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>549</v>
+      </c>
+      <c r="B12" t="s">
+        <v>550</v>
+      </c>
+      <c r="C12" t="s">
+        <v>551</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>(:MeasurementUnit {uuid: apoc.create.uuid(), name: 'Gram', inPortuguese: 'Grama', acronym : 'g'}),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>552</v>
+      </c>
+      <c r="B13" t="s">
+        <v>553</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>(:MeasurementUnit {uuid: apoc.create.uuid(), name: 'None', inPortuguese: 'Nenhuma', acronym : ''}),</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8BE5788-872A-43B9-9E25-E8C1A583BFB6}">
   <dimension ref="A1:C20"/>
   <sheetViews>
@@ -5496,7 +8096,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A61B1D1-1498-4062-8FF1-43F1DDC4F5BE}">
   <dimension ref="A1:F37"/>
   <sheetViews>
@@ -6019,1620 +8619,4 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{391AE3A0-7DB7-4C1A-B882-6DBA4383A0D7}">
-  <dimension ref="A1:O55"/>
-  <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:O2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" customWidth="1"/>
-    <col min="3" max="4" width="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="46.44140625" customWidth="1"/>
-    <col min="15" max="15" width="27.21875" customWidth="1"/>
-    <col min="16" max="16" width="9.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="B1" t="s">
-        <v>366</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="O1" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>325</v>
-      </c>
-      <c r="B2" t="str">
-        <f>SUBSTITUTE(UPPER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(A2," ","_"),"ó","o"),"í","i")),"/","_")</f>
-        <v>BCG_ID</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>353</v>
-      </c>
-      <c r="F2" t="s">
-        <v>352</v>
-      </c>
-      <c r="G2" t="str">
-        <f>"(:VaccineDose {name: '" &amp; E2 &amp;"', vaccine: '" &amp; A2 &amp;"', fromAgeInMonths: toInteger(" &amp; C2 &amp;"), toAgeInMonths:toInteger(" &amp; D2 &amp;"), classification: '" &amp; F2 &amp;"'}),"</f>
-        <v>(:VaccineDose {name: 'Unique', vaccine: 'BCG ID', fromAgeInMonths: toInteger(1), toAgeInMonths:toInteger(1), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O2" t="str">
-        <f>"MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '" &amp; A2 &amp; "' AND d.vaccine = '" &amp; A2 &amp; "' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);"</f>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'BCG ID' AND d.vaccine = 'BCG ID' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>326</v>
-      </c>
-      <c r="B3" t="str">
-        <f t="shared" ref="B3:B55" si="0">SUBSTITUTE(UPPER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(A3," ","_"),"ó","o"),"í","i")),"/","_")</f>
-        <v>HEPATITE_B</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>354</v>
-      </c>
-      <c r="F3" t="s">
-        <v>352</v>
-      </c>
-      <c r="G3" t="str">
-        <f t="shared" ref="G3:G55" si="1">"(:VaccineDose {name: '" &amp; E3 &amp;"', vaccine: '" &amp; A3 &amp;"', fromAgeInMonths: toInteger(" &amp; C3 &amp;"), toAgeInMonths:toInteger(" &amp; D3 &amp;"), classification: '" &amp; F3 &amp;"'}),"</f>
-        <v>(:VaccineDose {name: '1st dose', vaccine: 'Hepatite B', fromAgeInMonths: toInteger(1), toAgeInMonths:toInteger(1), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O3" t="str">
-        <f t="shared" ref="O3:O55" si="2">"MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '" &amp; A3 &amp; "' AND d.vaccine = '" &amp; A3 &amp; "' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);"</f>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Hepatite B' AND d.vaccine = 'Hepatite B' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>326</v>
-      </c>
-      <c r="B4" t="str">
-        <f t="shared" si="0"/>
-        <v>HEPATITE_B</v>
-      </c>
-      <c r="C4" s="1">
-        <v>2</v>
-      </c>
-      <c r="D4" s="1">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>355</v>
-      </c>
-      <c r="F4" t="s">
-        <v>352</v>
-      </c>
-      <c r="G4" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '2nd dose', vaccine: 'Hepatite B', fromAgeInMonths: toInteger(2), toAgeInMonths:toInteger(2), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O4" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Hepatite B' AND d.vaccine = 'Hepatite B' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>326</v>
-      </c>
-      <c r="B5" t="str">
-        <f t="shared" si="0"/>
-        <v>HEPATITE_B</v>
-      </c>
-      <c r="C5" s="1">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s">
-        <v>357</v>
-      </c>
-      <c r="F5" t="s">
-        <v>352</v>
-      </c>
-      <c r="G5" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '3rd dose', vaccine: 'Hepatite B', fromAgeInMonths: toInteger(6), toAgeInMonths:toInteger(6), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O5" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Hepatite B' AND d.vaccine = 'Hepatite B' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>364</v>
-      </c>
-      <c r="B6" t="str">
-        <f t="shared" si="0"/>
-        <v>DTPW</v>
-      </c>
-      <c r="C6" s="1">
-        <v>2</v>
-      </c>
-      <c r="D6" s="1">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>354</v>
-      </c>
-      <c r="F6" t="s">
-        <v>352</v>
-      </c>
-      <c r="G6" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '1st dose', vaccine: 'DTPw', fromAgeInMonths: toInteger(2), toAgeInMonths:toInteger(2), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O6" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'DTPw' AND d.vaccine = 'DTPw' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>364</v>
-      </c>
-      <c r="B7" t="str">
-        <f t="shared" si="0"/>
-        <v>DTPW</v>
-      </c>
-      <c r="C7" s="1">
-        <v>4</v>
-      </c>
-      <c r="D7" s="1">
-        <v>4</v>
-      </c>
-      <c r="E7" t="s">
-        <v>355</v>
-      </c>
-      <c r="F7" t="s">
-        <v>352</v>
-      </c>
-      <c r="G7" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '2nd dose', vaccine: 'DTPw', fromAgeInMonths: toInteger(4), toAgeInMonths:toInteger(4), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O7" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'DTPw' AND d.vaccine = 'DTPw' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>364</v>
-      </c>
-      <c r="B8" t="str">
-        <f t="shared" si="0"/>
-        <v>DTPW</v>
-      </c>
-      <c r="C8" s="1">
-        <v>6</v>
-      </c>
-      <c r="D8" s="1">
-        <v>6</v>
-      </c>
-      <c r="E8" t="s">
-        <v>357</v>
-      </c>
-      <c r="F8" t="s">
-        <v>352</v>
-      </c>
-      <c r="G8" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '3rd dose', vaccine: 'DTPw', fromAgeInMonths: toInteger(6), toAgeInMonths:toInteger(6), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O8" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'DTPw' AND d.vaccine = 'DTPw' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>364</v>
-      </c>
-      <c r="B9" t="str">
-        <f t="shared" si="0"/>
-        <v>DTPW</v>
-      </c>
-      <c r="C9" s="1">
-        <v>15</v>
-      </c>
-      <c r="D9" s="1">
-        <v>18</v>
-      </c>
-      <c r="E9" t="s">
-        <v>356</v>
-      </c>
-      <c r="F9" t="s">
-        <v>352</v>
-      </c>
-      <c r="G9" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Booster', vaccine: 'DTPw', fromAgeInMonths: toInteger(15), toAgeInMonths:toInteger(18), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O9" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'DTPw' AND d.vaccine = 'DTPw' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>364</v>
-      </c>
-      <c r="B10" t="str">
-        <f t="shared" si="0"/>
-        <v>DTPW</v>
-      </c>
-      <c r="C10" s="1">
-        <v>48</v>
-      </c>
-      <c r="D10" s="1">
-        <v>60</v>
-      </c>
-      <c r="E10" t="s">
-        <v>356</v>
-      </c>
-      <c r="F10" t="s">
-        <v>352</v>
-      </c>
-      <c r="G10" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Booster', vaccine: 'DTPw', fromAgeInMonths: toInteger(48), toAgeInMonths:toInteger(60), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O10" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'DTPw' AND d.vaccine = 'DTPw' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>367</v>
-      </c>
-      <c r="B11" t="str">
-        <f t="shared" si="0"/>
-        <v>H_INFLUENZAE</v>
-      </c>
-      <c r="C11" s="1">
-        <v>2</v>
-      </c>
-      <c r="D11" s="1">
-        <v>2</v>
-      </c>
-      <c r="E11" t="s">
-        <v>354</v>
-      </c>
-      <c r="F11" t="s">
-        <v>352</v>
-      </c>
-      <c r="G11" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '1st dose', vaccine: 'H Influenzae', fromAgeInMonths: toInteger(2), toAgeInMonths:toInteger(2), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O11" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'H Influenzae' AND d.vaccine = 'H Influenzae' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>367</v>
-      </c>
-      <c r="B12" t="str">
-        <f t="shared" si="0"/>
-        <v>H_INFLUENZAE</v>
-      </c>
-      <c r="C12" s="1">
-        <v>4</v>
-      </c>
-      <c r="D12" s="1">
-        <v>4</v>
-      </c>
-      <c r="E12" t="s">
-        <v>355</v>
-      </c>
-      <c r="F12" t="s">
-        <v>352</v>
-      </c>
-      <c r="G12" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '2nd dose', vaccine: 'H Influenzae', fromAgeInMonths: toInteger(4), toAgeInMonths:toInteger(4), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O12" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'H Influenzae' AND d.vaccine = 'H Influenzae' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>367</v>
-      </c>
-      <c r="B13" t="str">
-        <f t="shared" si="0"/>
-        <v>H_INFLUENZAE</v>
-      </c>
-      <c r="C13" s="1">
-        <v>6</v>
-      </c>
-      <c r="D13" s="1">
-        <v>6</v>
-      </c>
-      <c r="E13" t="s">
-        <v>357</v>
-      </c>
-      <c r="F13" t="s">
-        <v>352</v>
-      </c>
-      <c r="G13" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '3rd dose', vaccine: 'H Influenzae', fromAgeInMonths: toInteger(6), toAgeInMonths:toInteger(6), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O13" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'H Influenzae' AND d.vaccine = 'H Influenzae' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>367</v>
-      </c>
-      <c r="B14" t="str">
-        <f t="shared" si="0"/>
-        <v>H_INFLUENZAE</v>
-      </c>
-      <c r="C14" s="1">
-        <v>15</v>
-      </c>
-      <c r="D14" s="1">
-        <v>18</v>
-      </c>
-      <c r="E14" t="s">
-        <v>356</v>
-      </c>
-      <c r="F14" t="s">
-        <v>352</v>
-      </c>
-      <c r="G14" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Booster', vaccine: 'H Influenzae', fromAgeInMonths: toInteger(15), toAgeInMonths:toInteger(18), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O14" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'H Influenzae' AND d.vaccine = 'H Influenzae' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>327</v>
-      </c>
-      <c r="B15" t="str">
-        <f t="shared" si="0"/>
-        <v>POLIO_VIP</v>
-      </c>
-      <c r="C15" s="1">
-        <v>2</v>
-      </c>
-      <c r="D15" s="1">
-        <v>2</v>
-      </c>
-      <c r="E15" t="s">
-        <v>354</v>
-      </c>
-      <c r="F15" t="s">
-        <v>352</v>
-      </c>
-      <c r="G15" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '1st dose', vaccine: 'Pólio VIP', fromAgeInMonths: toInteger(2), toAgeInMonths:toInteger(2), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O15" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Pólio VIP' AND d.vaccine = 'Pólio VIP' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>327</v>
-      </c>
-      <c r="B16" t="str">
-        <f t="shared" si="0"/>
-        <v>POLIO_VIP</v>
-      </c>
-      <c r="C16" s="1">
-        <v>4</v>
-      </c>
-      <c r="D16" s="1">
-        <v>4</v>
-      </c>
-      <c r="E16" t="s">
-        <v>355</v>
-      </c>
-      <c r="F16" t="s">
-        <v>352</v>
-      </c>
-      <c r="G16" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '2nd dose', vaccine: 'Pólio VIP', fromAgeInMonths: toInteger(4), toAgeInMonths:toInteger(4), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O16" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Pólio VIP' AND d.vaccine = 'Pólio VIP' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>327</v>
-      </c>
-      <c r="B17" t="str">
-        <f t="shared" si="0"/>
-        <v>POLIO_VIP</v>
-      </c>
-      <c r="C17" s="1">
-        <v>6</v>
-      </c>
-      <c r="D17" s="1">
-        <v>6</v>
-      </c>
-      <c r="E17" t="s">
-        <v>357</v>
-      </c>
-      <c r="F17" t="s">
-        <v>352</v>
-      </c>
-      <c r="G17" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '3rd dose', vaccine: 'Pólio VIP', fromAgeInMonths: toInteger(6), toAgeInMonths:toInteger(6), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O17" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Pólio VIP' AND d.vaccine = 'Pólio VIP' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>328</v>
-      </c>
-      <c r="B18" t="str">
-        <f t="shared" si="0"/>
-        <v>POLIO_VOP</v>
-      </c>
-      <c r="C18" s="1">
-        <v>15</v>
-      </c>
-      <c r="D18" s="1">
-        <v>18</v>
-      </c>
-      <c r="E18" t="s">
-        <v>356</v>
-      </c>
-      <c r="F18" t="s">
-        <v>352</v>
-      </c>
-      <c r="G18" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Booster', vaccine: 'Pólio VOP', fromAgeInMonths: toInteger(15), toAgeInMonths:toInteger(18), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O18" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Pólio VOP' AND d.vaccine = 'Pólio VOP' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>328</v>
-      </c>
-      <c r="B19" t="str">
-        <f t="shared" si="0"/>
-        <v>POLIO_VOP</v>
-      </c>
-      <c r="C19" s="1">
-        <v>48</v>
-      </c>
-      <c r="D19" s="1">
-        <v>60</v>
-      </c>
-      <c r="E19" t="s">
-        <v>356</v>
-      </c>
-      <c r="F19" t="s">
-        <v>352</v>
-      </c>
-      <c r="G19" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Booster', vaccine: 'Pólio VOP', fromAgeInMonths: toInteger(48), toAgeInMonths:toInteger(60), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O19" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Pólio VOP' AND d.vaccine = 'Pólio VOP' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>329</v>
-      </c>
-      <c r="B20" t="str">
-        <f t="shared" si="0"/>
-        <v>ROTAVIRUS</v>
-      </c>
-      <c r="C20" s="1">
-        <v>2</v>
-      </c>
-      <c r="D20" s="1">
-        <v>4</v>
-      </c>
-      <c r="E20" t="s">
-        <v>354</v>
-      </c>
-      <c r="F20" t="s">
-        <v>352</v>
-      </c>
-      <c r="G20" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '1st dose', vaccine: 'Rotavírus', fromAgeInMonths: toInteger(2), toAgeInMonths:toInteger(4), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O20" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Rotavírus' AND d.vaccine = 'Rotavírus' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>329</v>
-      </c>
-      <c r="B21" t="str">
-        <f t="shared" si="0"/>
-        <v>ROTAVIRUS</v>
-      </c>
-      <c r="C21" s="1">
-        <v>5</v>
-      </c>
-      <c r="D21" s="1">
-        <v>8</v>
-      </c>
-      <c r="E21" t="s">
-        <v>355</v>
-      </c>
-      <c r="F21" t="s">
-        <v>352</v>
-      </c>
-      <c r="G21" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '2nd dose', vaccine: 'Rotavírus', fromAgeInMonths: toInteger(5), toAgeInMonths:toInteger(8), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O21" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Rotavírus' AND d.vaccine = 'Rotavírus' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>330</v>
-      </c>
-      <c r="B22" t="str">
-        <f t="shared" si="0"/>
-        <v>VPC10</v>
-      </c>
-      <c r="C22" s="1">
-        <v>2</v>
-      </c>
-      <c r="D22" s="1">
-        <v>3</v>
-      </c>
-      <c r="E22" t="s">
-        <v>354</v>
-      </c>
-      <c r="F22" t="s">
-        <v>352</v>
-      </c>
-      <c r="G22" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '1st dose', vaccine: 'VPC10', fromAgeInMonths: toInteger(2), toAgeInMonths:toInteger(3), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O22" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'VPC10' AND d.vaccine = 'VPC10' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>330</v>
-      </c>
-      <c r="B23" t="str">
-        <f t="shared" si="0"/>
-        <v>VPC10</v>
-      </c>
-      <c r="C23" s="1">
-        <v>4</v>
-      </c>
-      <c r="D23" s="1">
-        <v>6</v>
-      </c>
-      <c r="E23" t="s">
-        <v>355</v>
-      </c>
-      <c r="F23" t="s">
-        <v>352</v>
-      </c>
-      <c r="G23" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '2nd dose', vaccine: 'VPC10', fromAgeInMonths: toInteger(4), toAgeInMonths:toInteger(6), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O23" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'VPC10' AND d.vaccine = 'VPC10' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>330</v>
-      </c>
-      <c r="B24" t="str">
-        <f t="shared" si="0"/>
-        <v>VPC10</v>
-      </c>
-      <c r="C24" s="1">
-        <v>12</v>
-      </c>
-      <c r="D24" s="1">
-        <v>15</v>
-      </c>
-      <c r="E24" t="s">
-        <v>356</v>
-      </c>
-      <c r="F24" t="s">
-        <v>352</v>
-      </c>
-      <c r="G24" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Booster', vaccine: 'VPC10', fromAgeInMonths: toInteger(12), toAgeInMonths:toInteger(15), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O24" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'VPC10' AND d.vaccine = 'VPC10' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>331</v>
-      </c>
-      <c r="B25" t="str">
-        <f t="shared" si="0"/>
-        <v>ACWY_C</v>
-      </c>
-      <c r="C25" s="1">
-        <v>3</v>
-      </c>
-      <c r="D25" s="1">
-        <v>5</v>
-      </c>
-      <c r="E25" t="s">
-        <v>354</v>
-      </c>
-      <c r="F25" t="s">
-        <v>352</v>
-      </c>
-      <c r="G25" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '1st dose', vaccine: 'ACWY/C', fromAgeInMonths: toInteger(3), toAgeInMonths:toInteger(5), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O25" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'ACWY/C' AND d.vaccine = 'ACWY/C' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>331</v>
-      </c>
-      <c r="B26" t="str">
-        <f t="shared" si="0"/>
-        <v>ACWY_C</v>
-      </c>
-      <c r="C26" s="1">
-        <v>6</v>
-      </c>
-      <c r="D26" s="1">
-        <v>8</v>
-      </c>
-      <c r="E26" t="s">
-        <v>355</v>
-      </c>
-      <c r="F26" t="s">
-        <v>352</v>
-      </c>
-      <c r="G26" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '2nd dose', vaccine: 'ACWY/C', fromAgeInMonths: toInteger(6), toAgeInMonths:toInteger(8), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O26" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'ACWY/C' AND d.vaccine = 'ACWY/C' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>331</v>
-      </c>
-      <c r="B27" t="str">
-        <f t="shared" si="0"/>
-        <v>ACWY_C</v>
-      </c>
-      <c r="C27" s="1">
-        <v>12</v>
-      </c>
-      <c r="D27" s="1">
-        <v>15</v>
-      </c>
-      <c r="E27" t="s">
-        <v>356</v>
-      </c>
-      <c r="F27" t="s">
-        <v>352</v>
-      </c>
-      <c r="G27" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Booster', vaccine: 'ACWY/C', fromAgeInMonths: toInteger(12), toAgeInMonths:toInteger(15), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O27" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'ACWY/C' AND d.vaccine = 'ACWY/C' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>331</v>
-      </c>
-      <c r="B28" t="str">
-        <f t="shared" si="0"/>
-        <v>ACWY_C</v>
-      </c>
-      <c r="C28" s="1">
-        <v>60</v>
-      </c>
-      <c r="D28" s="1">
-        <v>72</v>
-      </c>
-      <c r="E28" t="s">
-        <v>356</v>
-      </c>
-      <c r="F28" t="s">
-        <v>359</v>
-      </c>
-      <c r="G28" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Booster', vaccine: 'ACWY/C', fromAgeInMonths: toInteger(60), toAgeInMonths:toInteger(72), classification: 'Optional'}),</v>
-      </c>
-      <c r="O28" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'ACWY/C' AND d.vaccine = 'ACWY/C' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>332</v>
-      </c>
-      <c r="B29" t="str">
-        <f t="shared" si="0"/>
-        <v>MENINGOCOCICA_B</v>
-      </c>
-      <c r="C29" s="1">
-        <v>3</v>
-      </c>
-      <c r="D29" s="1">
-        <v>3</v>
-      </c>
-      <c r="E29" t="s">
-        <v>354</v>
-      </c>
-      <c r="F29" t="s">
-        <v>352</v>
-      </c>
-      <c r="G29" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '1st dose', vaccine: 'Meningocócica B', fromAgeInMonths: toInteger(3), toAgeInMonths:toInteger(3), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O29" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Meningocócica B' AND d.vaccine = 'Meningocócica B' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>332</v>
-      </c>
-      <c r="B30" t="str">
-        <f t="shared" si="0"/>
-        <v>MENINGOCOCICA_B</v>
-      </c>
-      <c r="C30" s="1">
-        <v>5</v>
-      </c>
-      <c r="D30" s="1">
-        <v>5</v>
-      </c>
-      <c r="E30" t="s">
-        <v>355</v>
-      </c>
-      <c r="F30" t="s">
-        <v>352</v>
-      </c>
-      <c r="G30" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '2nd dose', vaccine: 'Meningocócica B', fromAgeInMonths: toInteger(5), toAgeInMonths:toInteger(5), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O30" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Meningocócica B' AND d.vaccine = 'Meningocócica B' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>332</v>
-      </c>
-      <c r="B31" t="str">
-        <f t="shared" si="0"/>
-        <v>MENINGOCOCICA_B</v>
-      </c>
-      <c r="C31" s="1">
-        <v>12</v>
-      </c>
-      <c r="D31" s="1">
-        <v>15</v>
-      </c>
-      <c r="E31" t="s">
-        <v>356</v>
-      </c>
-      <c r="F31" t="s">
-        <v>352</v>
-      </c>
-      <c r="G31" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Booster', vaccine: 'Meningocócica B', fromAgeInMonths: toInteger(12), toAgeInMonths:toInteger(15), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O31" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Meningocócica B' AND d.vaccine = 'Meningocócica B' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>333</v>
-      </c>
-      <c r="B32" t="str">
-        <f t="shared" si="0"/>
-        <v>3V</v>
-      </c>
-      <c r="C32" s="1">
-        <v>6</v>
-      </c>
-      <c r="D32" s="1">
-        <v>12</v>
-      </c>
-      <c r="E32" t="s">
-        <v>358</v>
-      </c>
-      <c r="F32" t="s">
-        <v>352</v>
-      </c>
-      <c r="G32" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Annual', vaccine: '3V', fromAgeInMonths: toInteger(6), toAgeInMonths:toInteger(12), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O32" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '3V' AND d.vaccine = '3V' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>333</v>
-      </c>
-      <c r="B33" t="str">
-        <f t="shared" si="0"/>
-        <v>3V</v>
-      </c>
-      <c r="C33" s="1">
-        <v>13</v>
-      </c>
-      <c r="D33" s="1">
-        <v>24</v>
-      </c>
-      <c r="E33" t="s">
-        <v>358</v>
-      </c>
-      <c r="F33" t="s">
-        <v>352</v>
-      </c>
-      <c r="G33" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Annual', vaccine: '3V', fromAgeInMonths: toInteger(13), toAgeInMonths:toInteger(24), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O33" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '3V' AND d.vaccine = '3V' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>333</v>
-      </c>
-      <c r="B34" t="str">
-        <f>SUBSTITUTE(UPPER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(A34," ","_"),"ó","o"),"í","i")),"/","_")</f>
-        <v>3V</v>
-      </c>
-      <c r="C34" s="1">
-        <v>25</v>
-      </c>
-      <c r="D34" s="1">
-        <v>36</v>
-      </c>
-      <c r="E34" t="s">
-        <v>358</v>
-      </c>
-      <c r="F34" t="s">
-        <v>352</v>
-      </c>
-      <c r="G34" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Annual', vaccine: '3V', fromAgeInMonths: toInteger(25), toAgeInMonths:toInteger(36), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O34" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '3V' AND d.vaccine = '3V' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>333</v>
-      </c>
-      <c r="B35" t="str">
-        <f t="shared" si="0"/>
-        <v>3V</v>
-      </c>
-      <c r="C35" s="1">
-        <v>37</v>
-      </c>
-      <c r="D35" s="1">
-        <v>48</v>
-      </c>
-      <c r="E35" t="s">
-        <v>358</v>
-      </c>
-      <c r="F35" t="s">
-        <v>352</v>
-      </c>
-      <c r="G35" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Annual', vaccine: '3V', fromAgeInMonths: toInteger(37), toAgeInMonths:toInteger(48), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O35" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '3V' AND d.vaccine = '3V' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>333</v>
-      </c>
-      <c r="B36" t="str">
-        <f t="shared" si="0"/>
-        <v>3V</v>
-      </c>
-      <c r="C36" s="1">
-        <v>49</v>
-      </c>
-      <c r="D36" s="1">
-        <v>60</v>
-      </c>
-      <c r="E36" t="s">
-        <v>358</v>
-      </c>
-      <c r="F36" t="s">
-        <v>352</v>
-      </c>
-      <c r="G36" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Annual', vaccine: '3V', fromAgeInMonths: toInteger(49), toAgeInMonths:toInteger(60), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O36" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '3V' AND d.vaccine = '3V' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>333</v>
-      </c>
-      <c r="B37" t="str">
-        <f t="shared" si="0"/>
-        <v>3V</v>
-      </c>
-      <c r="C37" s="1">
-        <v>61</v>
-      </c>
-      <c r="D37" s="1">
-        <v>72</v>
-      </c>
-      <c r="E37" t="s">
-        <v>358</v>
-      </c>
-      <c r="F37" t="s">
-        <v>352</v>
-      </c>
-      <c r="G37" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Annual', vaccine: '3V', fromAgeInMonths: toInteger(61), toAgeInMonths:toInteger(72), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O37" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '3V' AND d.vaccine = '3V' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>333</v>
-      </c>
-      <c r="B38" t="str">
-        <f t="shared" si="0"/>
-        <v>3V</v>
-      </c>
-      <c r="C38" s="1">
-        <v>73</v>
-      </c>
-      <c r="D38" s="1">
-        <v>84</v>
-      </c>
-      <c r="E38" t="s">
-        <v>358</v>
-      </c>
-      <c r="F38" t="s">
-        <v>352</v>
-      </c>
-      <c r="G38" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Annual', vaccine: '3V', fromAgeInMonths: toInteger(73), toAgeInMonths:toInteger(84), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O38" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '3V' AND d.vaccine = '3V' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>333</v>
-      </c>
-      <c r="B39" t="str">
-        <f t="shared" si="0"/>
-        <v>3V</v>
-      </c>
-      <c r="C39" s="1">
-        <v>85</v>
-      </c>
-      <c r="D39" s="1">
-        <v>96</v>
-      </c>
-      <c r="E39" t="s">
-        <v>358</v>
-      </c>
-      <c r="F39" t="s">
-        <v>352</v>
-      </c>
-      <c r="G39" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Annual', vaccine: '3V', fromAgeInMonths: toInteger(85), toAgeInMonths:toInteger(96), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O39" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '3V' AND d.vaccine = '3V' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>333</v>
-      </c>
-      <c r="B40" t="str">
-        <f t="shared" si="0"/>
-        <v>3V</v>
-      </c>
-      <c r="C40" s="1">
-        <v>97</v>
-      </c>
-      <c r="D40" s="1">
-        <v>108</v>
-      </c>
-      <c r="E40" t="s">
-        <v>358</v>
-      </c>
-      <c r="F40" t="s">
-        <v>352</v>
-      </c>
-      <c r="G40" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Annual', vaccine: '3V', fromAgeInMonths: toInteger(97), toAgeInMonths:toInteger(108), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O40" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '3V' AND d.vaccine = '3V' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>333</v>
-      </c>
-      <c r="B41" t="str">
-        <f t="shared" si="0"/>
-        <v>3V</v>
-      </c>
-      <c r="C41" s="1">
-        <v>109</v>
-      </c>
-      <c r="D41" s="1">
-        <v>120</v>
-      </c>
-      <c r="E41" t="s">
-        <v>358</v>
-      </c>
-      <c r="F41" t="s">
-        <v>352</v>
-      </c>
-      <c r="G41" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Annual', vaccine: '3V', fromAgeInMonths: toInteger(109), toAgeInMonths:toInteger(120), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O41" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '3V' AND d.vaccine = '3V' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>334</v>
-      </c>
-      <c r="B42" t="str">
-        <f t="shared" si="0"/>
-        <v>FEBRE_AMARELA</v>
-      </c>
-      <c r="C42" s="1">
-        <v>9</v>
-      </c>
-      <c r="D42" s="1">
-        <v>9</v>
-      </c>
-      <c r="E42" t="s">
-        <v>353</v>
-      </c>
-      <c r="F42" t="s">
-        <v>352</v>
-      </c>
-      <c r="G42" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Unique', vaccine: 'Febre amarela', fromAgeInMonths: toInteger(9), toAgeInMonths:toInteger(9), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O42" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Febre amarela' AND d.vaccine = 'Febre amarela' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>335</v>
-      </c>
-      <c r="B43" t="str">
-        <f t="shared" si="0"/>
-        <v>HEPATITE_A</v>
-      </c>
-      <c r="C43" s="1">
-        <v>12</v>
-      </c>
-      <c r="D43" s="1">
-        <v>12</v>
-      </c>
-      <c r="E43" t="s">
-        <v>354</v>
-      </c>
-      <c r="F43" t="s">
-        <v>352</v>
-      </c>
-      <c r="G43" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '1st dose', vaccine: 'Hepatite A', fromAgeInMonths: toInteger(12), toAgeInMonths:toInteger(12), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O43" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Hepatite A' AND d.vaccine = 'Hepatite A' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>335</v>
-      </c>
-      <c r="B44" t="str">
-        <f t="shared" si="0"/>
-        <v>HEPATITE_A</v>
-      </c>
-      <c r="C44" s="1">
-        <v>18</v>
-      </c>
-      <c r="D44" s="1">
-        <v>18</v>
-      </c>
-      <c r="E44" t="s">
-        <v>355</v>
-      </c>
-      <c r="F44" t="s">
-        <v>352</v>
-      </c>
-      <c r="G44" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '2nd dose', vaccine: 'Hepatite A', fromAgeInMonths: toInteger(18), toAgeInMonths:toInteger(18), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O44" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Hepatite A' AND d.vaccine = 'Hepatite A' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>336</v>
-      </c>
-      <c r="B45" t="str">
-        <f t="shared" si="0"/>
-        <v>BCG</v>
-      </c>
-      <c r="C45" s="1">
-        <v>12</v>
-      </c>
-      <c r="D45" s="1">
-        <v>12</v>
-      </c>
-      <c r="E45" t="s">
-        <v>354</v>
-      </c>
-      <c r="F45" t="s">
-        <v>352</v>
-      </c>
-      <c r="G45" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '1st dose', vaccine: 'BCG', fromAgeInMonths: toInteger(12), toAgeInMonths:toInteger(12), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O45" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'BCG' AND d.vaccine = 'BCG' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>336</v>
-      </c>
-      <c r="B46" t="str">
-        <f t="shared" si="0"/>
-        <v>BCG</v>
-      </c>
-      <c r="C46" s="1">
-        <v>15</v>
-      </c>
-      <c r="D46" s="1">
-        <v>24</v>
-      </c>
-      <c r="E46" t="s">
-        <v>355</v>
-      </c>
-      <c r="F46" t="s">
-        <v>352</v>
-      </c>
-      <c r="G46" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '2nd dose', vaccine: 'BCG', fromAgeInMonths: toInteger(15), toAgeInMonths:toInteger(24), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O46" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'BCG' AND d.vaccine = 'BCG' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>337</v>
-      </c>
-      <c r="B47" t="str">
-        <f t="shared" si="0"/>
-        <v>VARICELA</v>
-      </c>
-      <c r="C47" s="1">
-        <v>12</v>
-      </c>
-      <c r="D47" s="1">
-        <v>12</v>
-      </c>
-      <c r="E47" t="s">
-        <v>354</v>
-      </c>
-      <c r="F47" t="s">
-        <v>352</v>
-      </c>
-      <c r="G47" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '1st dose', vaccine: 'Varicela', fromAgeInMonths: toInteger(12), toAgeInMonths:toInteger(12), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O47" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Varicela' AND d.vaccine = 'Varicela' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>337</v>
-      </c>
-      <c r="B48" t="str">
-        <f t="shared" si="0"/>
-        <v>VARICELA</v>
-      </c>
-      <c r="C48" s="1">
-        <v>15</v>
-      </c>
-      <c r="D48" s="1">
-        <v>24</v>
-      </c>
-      <c r="E48" t="s">
-        <v>355</v>
-      </c>
-      <c r="F48" t="s">
-        <v>352</v>
-      </c>
-      <c r="G48" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '2nd dose', vaccine: 'Varicela', fromAgeInMonths: toInteger(15), toAgeInMonths:toInteger(24), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O48" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Varicela' AND d.vaccine = 'Varicela' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>338</v>
-      </c>
-      <c r="B49" t="str">
-        <f t="shared" si="0"/>
-        <v>HPV4</v>
-      </c>
-      <c r="C49" s="1">
-        <v>108</v>
-      </c>
-      <c r="D49" s="1">
-        <v>119</v>
-      </c>
-      <c r="E49" t="s">
-        <v>354</v>
-      </c>
-      <c r="F49" t="s">
-        <v>352</v>
-      </c>
-      <c r="G49" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '1st dose', vaccine: 'HPV4', fromAgeInMonths: toInteger(108), toAgeInMonths:toInteger(119), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O49" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'HPV4' AND d.vaccine = 'HPV4' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>338</v>
-      </c>
-      <c r="B50" t="str">
-        <f t="shared" si="0"/>
-        <v>HPV4</v>
-      </c>
-      <c r="C50" s="1">
-        <v>120</v>
-      </c>
-      <c r="D50" s="1">
-        <v>132</v>
-      </c>
-      <c r="E50" t="s">
-        <v>355</v>
-      </c>
-      <c r="F50" t="s">
-        <v>352</v>
-      </c>
-      <c r="G50" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '2nd dose', vaccine: 'HPV4', fromAgeInMonths: toInteger(120), toAgeInMonths:toInteger(132), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O50" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'HPV4' AND d.vaccine = 'HPV4' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>365</v>
-      </c>
-      <c r="B51" t="str">
-        <f t="shared" si="0"/>
-        <v>DTPA</v>
-      </c>
-      <c r="C51" s="1">
-        <v>2</v>
-      </c>
-      <c r="D51" s="1">
-        <v>2</v>
-      </c>
-      <c r="E51" t="s">
-        <v>354</v>
-      </c>
-      <c r="F51" t="s">
-        <v>352</v>
-      </c>
-      <c r="G51" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '1st dose', vaccine: 'DTPa', fromAgeInMonths: toInteger(2), toAgeInMonths:toInteger(2), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O51" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'DTPa' AND d.vaccine = 'DTPa' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>365</v>
-      </c>
-      <c r="B52" t="str">
-        <f t="shared" si="0"/>
-        <v>DTPA</v>
-      </c>
-      <c r="C52" s="1">
-        <v>4</v>
-      </c>
-      <c r="D52" s="1">
-        <v>4</v>
-      </c>
-      <c r="E52" t="s">
-        <v>355</v>
-      </c>
-      <c r="F52" t="s">
-        <v>352</v>
-      </c>
-      <c r="G52" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '2nd dose', vaccine: 'DTPa', fromAgeInMonths: toInteger(4), toAgeInMonths:toInteger(4), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O52" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'DTPa' AND d.vaccine = 'DTPa' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>365</v>
-      </c>
-      <c r="B53" t="str">
-        <f t="shared" si="0"/>
-        <v>DTPA</v>
-      </c>
-      <c r="C53" s="1">
-        <v>6</v>
-      </c>
-      <c r="D53" s="1">
-        <v>6</v>
-      </c>
-      <c r="E53" t="s">
-        <v>357</v>
-      </c>
-      <c r="F53" t="s">
-        <v>352</v>
-      </c>
-      <c r="G53" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '3rd dose', vaccine: 'DTPa', fromAgeInMonths: toInteger(6), toAgeInMonths:toInteger(6), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O53" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'DTPa' AND d.vaccine = 'DTPa' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>365</v>
-      </c>
-      <c r="B54" t="str">
-        <f t="shared" si="0"/>
-        <v>DTPA</v>
-      </c>
-      <c r="C54" s="1">
-        <v>15</v>
-      </c>
-      <c r="D54" s="1">
-        <v>18</v>
-      </c>
-      <c r="E54" t="s">
-        <v>356</v>
-      </c>
-      <c r="F54" t="s">
-        <v>352</v>
-      </c>
-      <c r="G54" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Booster', vaccine: 'DTPa', fromAgeInMonths: toInteger(15), toAgeInMonths:toInteger(18), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O54" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'DTPa' AND d.vaccine = 'DTPa' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>365</v>
-      </c>
-      <c r="B55" t="str">
-        <f t="shared" si="0"/>
-        <v>DTPA</v>
-      </c>
-      <c r="C55" s="1">
-        <v>48</v>
-      </c>
-      <c r="D55" s="1">
-        <v>60</v>
-      </c>
-      <c r="E55" t="s">
-        <v>356</v>
-      </c>
-      <c r="F55" t="s">
-        <v>352</v>
-      </c>
-      <c r="G55" t="str">
-        <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Booster', vaccine: 'DTPa', fromAgeInMonths: toInteger(48), toAgeInMonths:toInteger(60), classification: 'Mandatory'}),</v>
-      </c>
-      <c r="O55" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'DTPa' AND d.vaccine = 'DTPa' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
refactor: :construction: refactoring measurement features
</commit_message>
<xml_diff>
--- a/poc.xlsx
+++ b/poc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\renatospaka\dev\heykid\draft\poc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79091F93-C39E-4C35-8A63-2783EC58BAE0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A97A57D-18FD-4AC7-A090-887BB3969848}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="disease" sheetId="3" r:id="rId1"/>
@@ -20,14 +20,15 @@
     <sheet name="measurement" sheetId="8" r:id="rId5"/>
     <sheet name="measurement unit" sheetId="10" r:id="rId6"/>
     <sheet name="event" sheetId="1" r:id="rId7"/>
-    <sheet name="specialty" sheetId="2" r:id="rId8"/>
-    <sheet name="vaccine" sheetId="6" r:id="rId9"/>
-    <sheet name="vaccine dose" sheetId="7" r:id="rId10"/>
+    <sheet name="milestone" sheetId="11" r:id="rId8"/>
+    <sheet name="specialty" sheetId="2" r:id="rId9"/>
+    <sheet name="vaccine" sheetId="6" r:id="rId10"/>
+    <sheet name="vaccine dose" sheetId="7" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">disease!$A$1:$D$101</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">intolerance!$A$1:$D$50</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'vaccine dose'!$A$1:$F$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'vaccine dose'!$A$1:$F$55</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="574">
   <si>
     <t>Query</t>
   </si>
@@ -1761,6 +1762,15 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>Primeiro Dente</t>
+  </si>
+  <si>
+    <t>Balbuciar</t>
+  </si>
+  <si>
+    <t>Chamar os Pais</t>
   </si>
 </sst>
 </file>
@@ -3318,6 +3328,531 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A61B1D1-1498-4062-8FF1-43F1DDC4F5BE}">
+  <dimension ref="A1:F37"/>
+  <sheetViews>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="41.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="50.109375" customWidth="1"/>
+    <col min="8" max="8" width="34" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C1" t="s">
+        <v>349</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B2" t="str">
+        <f>SUBSTITUTE(UPPER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(A2," ","_"),"ó","o"),"í","i")),"/","_")</f>
+        <v>BCG_ID</v>
+      </c>
+      <c r="C2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D2" t="s">
+        <v>342</v>
+      </c>
+      <c r="E2" t="s">
+        <v>341</v>
+      </c>
+      <c r="F2" t="str">
+        <f>"(:Vaccine {name: '" &amp; A2 &amp;"', description: '" &amp; C2 &amp;"', dosage: '" &amp; D2 &amp;"', classification: '" &amp; E2 &amp;"'}),"</f>
+        <v>(:Vaccine {name: 'BCG ID', description: 'Tuberculose', dosage: 'Unique', classification: 'Mandatory'}),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>315</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B18" si="0">SUBSTITUTE(UPPER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(A3," ","_"),"ó","o"),"í","i")),"/","_")</f>
+        <v>HEPATITE_B</v>
+      </c>
+      <c r="C3" t="s">
+        <v>315</v>
+      </c>
+      <c r="D3" t="s">
+        <v>351</v>
+      </c>
+      <c r="E3" t="s">
+        <v>341</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F18" si="1">"(:Vaccine {name: '" &amp; A3 &amp;"', description: '" &amp; C3 &amp;"', dosage: '" &amp; D3 &amp;"', classification: '" &amp; E3 &amp;"'}),"</f>
+        <v>(:Vaccine {name: 'Hepatite B', description: 'Hepatite B', dosage: 'Dose', classification: 'Mandatory'}),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>353</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>DTPW</v>
+      </c>
+      <c r="C4" t="s">
+        <v>328</v>
+      </c>
+      <c r="D4" t="s">
+        <v>351</v>
+      </c>
+      <c r="E4" t="s">
+        <v>341</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Vaccine {name: 'DTPw', description: 'Tríplice bacteriana (difteria, tétano e coqueluche)', dosage: 'Dose', classification: 'Mandatory'}),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>356</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>H_INFLUENZAE</v>
+      </c>
+      <c r="C5" t="s">
+        <v>329</v>
+      </c>
+      <c r="D5" t="s">
+        <v>351</v>
+      </c>
+      <c r="E5" t="s">
+        <v>341</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Vaccine {name: 'H Influenzae', description: 'Haemophilus influenzae, tipo B', dosage: 'Dose', classification: 'Mandatory'}),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>316</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>POLIO_VIP</v>
+      </c>
+      <c r="C6" t="s">
+        <v>330</v>
+      </c>
+      <c r="D6" t="s">
+        <v>351</v>
+      </c>
+      <c r="E6" t="s">
+        <v>341</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Vaccine {name: 'Pólio VIP', description: 'Vacina Inativada Poliomielite', dosage: 'Dose', classification: 'Mandatory'}),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>317</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>POLIO_VOP</v>
+      </c>
+      <c r="C7" t="s">
+        <v>331</v>
+      </c>
+      <c r="D7" t="s">
+        <v>345</v>
+      </c>
+      <c r="E7" t="s">
+        <v>341</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Vaccine {name: 'Pólio VOP', description: 'Vacina Oral Poliomielite', dosage: 'Booster', classification: 'Mandatory'}),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>318</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>ROTAVIRUS</v>
+      </c>
+      <c r="C8" t="s">
+        <v>318</v>
+      </c>
+      <c r="D8" t="s">
+        <v>351</v>
+      </c>
+      <c r="E8" t="s">
+        <v>341</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Vaccine {name: 'Rotavírus', description: 'Rotavírus', dosage: 'Dose', classification: 'Mandatory'}),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>319</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>VPC10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D9" t="s">
+        <v>351</v>
+      </c>
+      <c r="E9" t="s">
+        <v>341</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Vaccine {name: 'VPC10', description: 'Pneumocócicas conjugadas', dosage: 'Dose', classification: 'Mandatory'}),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>320</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>ACWY_C</v>
+      </c>
+      <c r="C10" t="s">
+        <v>333</v>
+      </c>
+      <c r="D10" t="s">
+        <v>351</v>
+      </c>
+      <c r="E10" t="s">
+        <v>348</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Vaccine {name: 'ACWY/C', description: 'Meningocócicas conjugadas ACWY/C', dosage: 'Dose', classification: 'Optional'}),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>321</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>MENINGOCOCICA_B</v>
+      </c>
+      <c r="C11" t="s">
+        <v>321</v>
+      </c>
+      <c r="D11" t="s">
+        <v>351</v>
+      </c>
+      <c r="E11" t="s">
+        <v>341</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Vaccine {name: 'Meningocócica B', description: 'Meningocócica B', dosage: 'Dose', classification: 'Mandatory'}),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>322</v>
+      </c>
+      <c r="B12" t="str">
+        <f>"_" &amp;A12</f>
+        <v>_3V</v>
+      </c>
+      <c r="C12" t="s">
+        <v>334</v>
+      </c>
+      <c r="D12" t="s">
+        <v>347</v>
+      </c>
+      <c r="E12" t="s">
+        <v>341</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Vaccine {name: '3V', description: 'Influenza, gripe', dosage: 'Annual', classification: 'Mandatory'}),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>323</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>FEBRE_AMARELA</v>
+      </c>
+      <c r="C13" t="s">
+        <v>335</v>
+      </c>
+      <c r="D13" t="s">
+        <v>342</v>
+      </c>
+      <c r="E13" t="s">
+        <v>341</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Vaccine {name: 'Febre amarela', description: 'Febre amarela (atenuada)', dosage: 'Unique', classification: 'Mandatory'}),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>324</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>HEPATITE_A</v>
+      </c>
+      <c r="C14" t="s">
+        <v>324</v>
+      </c>
+      <c r="D14" t="s">
+        <v>351</v>
+      </c>
+      <c r="E14" t="s">
+        <v>341</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Vaccine {name: 'Hepatite A', description: 'Hepatite A', dosage: 'Dose', classification: 'Mandatory'}),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>325</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>BCG</v>
+      </c>
+      <c r="C15" t="s">
+        <v>336</v>
+      </c>
+      <c r="D15" t="s">
+        <v>351</v>
+      </c>
+      <c r="E15" t="s">
+        <v>341</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Vaccine {name: 'BCG', description: 'Tríplice viral (sarampo, caxumba e rubéola)', dosage: 'Dose', classification: 'Mandatory'}),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>326</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>VARICELA</v>
+      </c>
+      <c r="C16" t="s">
+        <v>337</v>
+      </c>
+      <c r="D16" t="s">
+        <v>351</v>
+      </c>
+      <c r="E16" t="s">
+        <v>341</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Vaccine {name: 'Varicela', description: 'Varicela (catapora)', dosage: 'Dose', classification: 'Mandatory'}),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>327</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>HPV4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>338</v>
+      </c>
+      <c r="D17" t="s">
+        <v>351</v>
+      </c>
+      <c r="E17" t="s">
+        <v>341</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Vaccine {name: 'HPV4', description: 'HPV', dosage: 'Dose', classification: 'Mandatory'}),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>354</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>DTPA</v>
+      </c>
+      <c r="C18" t="s">
+        <v>328</v>
+      </c>
+      <c r="D18" t="s">
+        <v>351</v>
+      </c>
+      <c r="E18" t="s">
+        <v>341</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="1"/>
+        <v>(:Vaccine {name: 'DTPa', description: 'Tríplice bacteriana (difteria, tétano e coqueluche)', dosage: 'Dose', classification: 'Mandatory'}),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F21" t="str">
+        <f t="shared" ref="F21:F37" si="2">"MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '" &amp; A2 &amp; "' AND d.vaccine = '" &amp; A2 &amp; "' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);"</f>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'BCG ID' AND d.vaccine = 'BCG ID' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F22" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Hepatite B' AND d.vaccine = 'Hepatite B' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F23" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'DTPw' AND d.vaccine = 'DTPw' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F24" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'H Influenzae' AND d.vaccine = 'H Influenzae' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F25" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Pólio VIP' AND d.vaccine = 'Pólio VIP' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F26" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Pólio VOP' AND d.vaccine = 'Pólio VOP' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F27" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Rotavírus' AND d.vaccine = 'Rotavírus' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F28" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'VPC10' AND d.vaccine = 'VPC10' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F29" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'ACWY/C' AND d.vaccine = 'ACWY/C' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F30" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Meningocócica B' AND d.vaccine = 'Meningocócica B' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F31" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '3V' AND d.vaccine = '3V' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F32" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Febre amarela' AND d.vaccine = 'Febre amarela' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F33" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Hepatite A' AND d.vaccine = 'Hepatite A' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F34" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'BCG' AND d.vaccine = 'BCG' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F35" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Varicela' AND d.vaccine = 'Varicela' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F36" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'HPV4' AND d.vaccine = 'HPV4' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+    <row r="37" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F37" t="str">
+        <f t="shared" si="2"/>
+        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'DTPa' AND d.vaccine = 'DTPa' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{391AE3A0-7DB7-4C1A-B882-6DBA4383A0D7}">
   <dimension ref="A1:O55"/>
   <sheetViews>
@@ -7479,7 +8014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58E23DBB-27F6-4A87-AFAA-C8781EFF9D8C}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
+    <sheetView zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -7689,7 +8224,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7913,6 +8448,168 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE4D6E2-6BDE-4AC5-843C-AEB3BD0CAE9C}">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="30.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>569</v>
+      </c>
+      <c r="B1" t="s">
+        <v>570</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>571</v>
+      </c>
+      <c r="B2" t="s">
+        <v>540</v>
+      </c>
+      <c r="D2" t="str">
+        <f>"(:Milestone {uuid: apoc.create.uuid(), name: '" &amp; B2 &amp;"', inPortuguese: '" &amp; A2 &amp;"'}),"</f>
+        <v>(:Milestone {uuid: apoc.create.uuid(), name: 'Surgery', inPortuguese: 'Primeiro Dente'}),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>572</v>
+      </c>
+      <c r="B3" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>573</v>
+      </c>
+      <c r="B4" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>554</v>
+      </c>
+      <c r="B5" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>555</v>
+      </c>
+      <c r="B6" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>545</v>
+      </c>
+      <c r="B7" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>556</v>
+      </c>
+      <c r="B8" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>557</v>
+      </c>
+      <c r="B9" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>558</v>
+      </c>
+      <c r="B10" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>559</v>
+      </c>
+      <c r="B11" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>297</v>
+      </c>
+      <c r="B12" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>298</v>
+      </c>
+      <c r="B13" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>300</v>
+      </c>
+      <c r="B14" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>560</v>
+      </c>
+      <c r="B15" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>566</v>
+      </c>
+      <c r="B16" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>567</v>
+      </c>
+      <c r="B17" t="s">
+        <v>565</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8BE5788-872A-43B9-9E25-E8C1A583BFB6}">
   <dimension ref="A1:C20"/>
   <sheetViews>
@@ -8169,529 +8866,4 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A61B1D1-1498-4062-8FF1-43F1DDC4F5BE}">
-  <dimension ref="A1:F37"/>
-  <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="41.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="50.109375" customWidth="1"/>
-    <col min="8" max="8" width="34" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>313</v>
-      </c>
-      <c r="B1" t="s">
-        <v>355</v>
-      </c>
-      <c r="C1" t="s">
-        <v>349</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="F1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>314</v>
-      </c>
-      <c r="B2" t="str">
-        <f>SUBSTITUTE(UPPER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(A2," ","_"),"ó","o"),"í","i")),"/","_")</f>
-        <v>BCG_ID</v>
-      </c>
-      <c r="C2" t="s">
-        <v>174</v>
-      </c>
-      <c r="D2" t="s">
-        <v>342</v>
-      </c>
-      <c r="E2" t="s">
-        <v>341</v>
-      </c>
-      <c r="F2" t="str">
-        <f>"(:Vaccine {name: '" &amp; A2 &amp;"', description: '" &amp; C2 &amp;"', dosage: '" &amp; D2 &amp;"', classification: '" &amp; E2 &amp;"'}),"</f>
-        <v>(:Vaccine {name: 'BCG ID', description: 'Tuberculose', dosage: 'Unique', classification: 'Mandatory'}),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>315</v>
-      </c>
-      <c r="B3" t="str">
-        <f t="shared" ref="B3:B18" si="0">SUBSTITUTE(UPPER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(A3," ","_"),"ó","o"),"í","i")),"/","_")</f>
-        <v>HEPATITE_B</v>
-      </c>
-      <c r="C3" t="s">
-        <v>315</v>
-      </c>
-      <c r="D3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E3" t="s">
-        <v>341</v>
-      </c>
-      <c r="F3" t="str">
-        <f t="shared" ref="F3:F18" si="1">"(:Vaccine {name: '" &amp; A3 &amp;"', description: '" &amp; C3 &amp;"', dosage: '" &amp; D3 &amp;"', classification: '" &amp; E3 &amp;"'}),"</f>
-        <v>(:Vaccine {name: 'Hepatite B', description: 'Hepatite B', dosage: 'Dose', classification: 'Mandatory'}),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>353</v>
-      </c>
-      <c r="B4" t="str">
-        <f t="shared" si="0"/>
-        <v>DTPW</v>
-      </c>
-      <c r="C4" t="s">
-        <v>328</v>
-      </c>
-      <c r="D4" t="s">
-        <v>351</v>
-      </c>
-      <c r="E4" t="s">
-        <v>341</v>
-      </c>
-      <c r="F4" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Vaccine {name: 'DTPw', description: 'Tríplice bacteriana (difteria, tétano e coqueluche)', dosage: 'Dose', classification: 'Mandatory'}),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>356</v>
-      </c>
-      <c r="B5" t="str">
-        <f t="shared" si="0"/>
-        <v>H_INFLUENZAE</v>
-      </c>
-      <c r="C5" t="s">
-        <v>329</v>
-      </c>
-      <c r="D5" t="s">
-        <v>351</v>
-      </c>
-      <c r="E5" t="s">
-        <v>341</v>
-      </c>
-      <c r="F5" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Vaccine {name: 'H Influenzae', description: 'Haemophilus influenzae, tipo B', dosage: 'Dose', classification: 'Mandatory'}),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>316</v>
-      </c>
-      <c r="B6" t="str">
-        <f t="shared" si="0"/>
-        <v>POLIO_VIP</v>
-      </c>
-      <c r="C6" t="s">
-        <v>330</v>
-      </c>
-      <c r="D6" t="s">
-        <v>351</v>
-      </c>
-      <c r="E6" t="s">
-        <v>341</v>
-      </c>
-      <c r="F6" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Vaccine {name: 'Pólio VIP', description: 'Vacina Inativada Poliomielite', dosage: 'Dose', classification: 'Mandatory'}),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>317</v>
-      </c>
-      <c r="B7" t="str">
-        <f t="shared" si="0"/>
-        <v>POLIO_VOP</v>
-      </c>
-      <c r="C7" t="s">
-        <v>331</v>
-      </c>
-      <c r="D7" t="s">
-        <v>345</v>
-      </c>
-      <c r="E7" t="s">
-        <v>341</v>
-      </c>
-      <c r="F7" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Vaccine {name: 'Pólio VOP', description: 'Vacina Oral Poliomielite', dosage: 'Booster', classification: 'Mandatory'}),</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>318</v>
-      </c>
-      <c r="B8" t="str">
-        <f t="shared" si="0"/>
-        <v>ROTAVIRUS</v>
-      </c>
-      <c r="C8" t="s">
-        <v>318</v>
-      </c>
-      <c r="D8" t="s">
-        <v>351</v>
-      </c>
-      <c r="E8" t="s">
-        <v>341</v>
-      </c>
-      <c r="F8" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Vaccine {name: 'Rotavírus', description: 'Rotavírus', dosage: 'Dose', classification: 'Mandatory'}),</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>319</v>
-      </c>
-      <c r="B9" t="str">
-        <f t="shared" si="0"/>
-        <v>VPC10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>332</v>
-      </c>
-      <c r="D9" t="s">
-        <v>351</v>
-      </c>
-      <c r="E9" t="s">
-        <v>341</v>
-      </c>
-      <c r="F9" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Vaccine {name: 'VPC10', description: 'Pneumocócicas conjugadas', dosage: 'Dose', classification: 'Mandatory'}),</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>320</v>
-      </c>
-      <c r="B10" t="str">
-        <f t="shared" si="0"/>
-        <v>ACWY_C</v>
-      </c>
-      <c r="C10" t="s">
-        <v>333</v>
-      </c>
-      <c r="D10" t="s">
-        <v>351</v>
-      </c>
-      <c r="E10" t="s">
-        <v>348</v>
-      </c>
-      <c r="F10" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Vaccine {name: 'ACWY/C', description: 'Meningocócicas conjugadas ACWY/C', dosage: 'Dose', classification: 'Optional'}),</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>321</v>
-      </c>
-      <c r="B11" t="str">
-        <f t="shared" si="0"/>
-        <v>MENINGOCOCICA_B</v>
-      </c>
-      <c r="C11" t="s">
-        <v>321</v>
-      </c>
-      <c r="D11" t="s">
-        <v>351</v>
-      </c>
-      <c r="E11" t="s">
-        <v>341</v>
-      </c>
-      <c r="F11" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Vaccine {name: 'Meningocócica B', description: 'Meningocócica B', dosage: 'Dose', classification: 'Mandatory'}),</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>322</v>
-      </c>
-      <c r="B12" t="str">
-        <f>"_" &amp;A12</f>
-        <v>_3V</v>
-      </c>
-      <c r="C12" t="s">
-        <v>334</v>
-      </c>
-      <c r="D12" t="s">
-        <v>347</v>
-      </c>
-      <c r="E12" t="s">
-        <v>341</v>
-      </c>
-      <c r="F12" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Vaccine {name: '3V', description: 'Influenza, gripe', dosage: 'Annual', classification: 'Mandatory'}),</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>323</v>
-      </c>
-      <c r="B13" t="str">
-        <f t="shared" si="0"/>
-        <v>FEBRE_AMARELA</v>
-      </c>
-      <c r="C13" t="s">
-        <v>335</v>
-      </c>
-      <c r="D13" t="s">
-        <v>342</v>
-      </c>
-      <c r="E13" t="s">
-        <v>341</v>
-      </c>
-      <c r="F13" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Vaccine {name: 'Febre amarela', description: 'Febre amarela (atenuada)', dosage: 'Unique', classification: 'Mandatory'}),</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>324</v>
-      </c>
-      <c r="B14" t="str">
-        <f t="shared" si="0"/>
-        <v>HEPATITE_A</v>
-      </c>
-      <c r="C14" t="s">
-        <v>324</v>
-      </c>
-      <c r="D14" t="s">
-        <v>351</v>
-      </c>
-      <c r="E14" t="s">
-        <v>341</v>
-      </c>
-      <c r="F14" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Vaccine {name: 'Hepatite A', description: 'Hepatite A', dosage: 'Dose', classification: 'Mandatory'}),</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>325</v>
-      </c>
-      <c r="B15" t="str">
-        <f t="shared" si="0"/>
-        <v>BCG</v>
-      </c>
-      <c r="C15" t="s">
-        <v>336</v>
-      </c>
-      <c r="D15" t="s">
-        <v>351</v>
-      </c>
-      <c r="E15" t="s">
-        <v>341</v>
-      </c>
-      <c r="F15" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Vaccine {name: 'BCG', description: 'Tríplice viral (sarampo, caxumba e rubéola)', dosage: 'Dose', classification: 'Mandatory'}),</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>326</v>
-      </c>
-      <c r="B16" t="str">
-        <f t="shared" si="0"/>
-        <v>VARICELA</v>
-      </c>
-      <c r="C16" t="s">
-        <v>337</v>
-      </c>
-      <c r="D16" t="s">
-        <v>351</v>
-      </c>
-      <c r="E16" t="s">
-        <v>341</v>
-      </c>
-      <c r="F16" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Vaccine {name: 'Varicela', description: 'Varicela (catapora)', dosage: 'Dose', classification: 'Mandatory'}),</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>327</v>
-      </c>
-      <c r="B17" t="str">
-        <f t="shared" si="0"/>
-        <v>HPV4</v>
-      </c>
-      <c r="C17" t="s">
-        <v>338</v>
-      </c>
-      <c r="D17" t="s">
-        <v>351</v>
-      </c>
-      <c r="E17" t="s">
-        <v>341</v>
-      </c>
-      <c r="F17" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Vaccine {name: 'HPV4', description: 'HPV', dosage: 'Dose', classification: 'Mandatory'}),</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>354</v>
-      </c>
-      <c r="B18" t="str">
-        <f t="shared" si="0"/>
-        <v>DTPA</v>
-      </c>
-      <c r="C18" t="s">
-        <v>328</v>
-      </c>
-      <c r="D18" t="s">
-        <v>351</v>
-      </c>
-      <c r="E18" t="s">
-        <v>341</v>
-      </c>
-      <c r="F18" t="str">
-        <f t="shared" si="1"/>
-        <v>(:Vaccine {name: 'DTPa', description: 'Tríplice bacteriana (difteria, tétano e coqueluche)', dosage: 'Dose', classification: 'Mandatory'}),</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F20" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F21" t="str">
-        <f t="shared" ref="F21:F37" si="2">"MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '" &amp; A2 &amp; "' AND d.vaccine = '" &amp; A2 &amp; "' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);"</f>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'BCG ID' AND d.vaccine = 'BCG ID' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F22" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Hepatite B' AND d.vaccine = 'Hepatite B' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F23" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'DTPw' AND d.vaccine = 'DTPw' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F24" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'H Influenzae' AND d.vaccine = 'H Influenzae' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F25" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Pólio VIP' AND d.vaccine = 'Pólio VIP' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F26" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Pólio VOP' AND d.vaccine = 'Pólio VOP' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F27" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Rotavírus' AND d.vaccine = 'Rotavírus' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F28" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'VPC10' AND d.vaccine = 'VPC10' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F29" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'ACWY/C' AND d.vaccine = 'ACWY/C' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F30" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Meningocócica B' AND d.vaccine = 'Meningocócica B' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F31" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '3V' AND d.vaccine = '3V' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F32" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Febre amarela' AND d.vaccine = 'Febre amarela' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F33" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Hepatite A' AND d.vaccine = 'Hepatite A' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F34" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'BCG' AND d.vaccine = 'BCG' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F35" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Varicela' AND d.vaccine = 'Varicela' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="36" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F36" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'HPV4' AND d.vaccine = 'HPV4' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-    <row r="37" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F37" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'DTPa' AND d.vaccine = 'DTPa' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
refactor: :recycle: change layout of vaccination features
</commit_message>
<xml_diff>
--- a/poc.xlsx
+++ b/poc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\renatospaka\dev\heykid\draft\poc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A97A57D-18FD-4AC7-A090-887BB3969848}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53CCDD07-3290-455E-A5DC-3A963D314E8C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="disease" sheetId="3" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="619">
   <si>
     <t>Query</t>
   </si>
@@ -1771,6 +1771,141 @@
   </si>
   <si>
     <t>Chamar os Pais</t>
+  </si>
+  <si>
+    <t>Fase</t>
+  </si>
+  <si>
+    <t>Neonatal</t>
+  </si>
+  <si>
+    <t>1ª Infância</t>
+  </si>
+  <si>
+    <t>Stage</t>
+  </si>
+  <si>
+    <t>Adolescência</t>
+  </si>
+  <si>
+    <t>Newborn</t>
+  </si>
+  <si>
+    <t>Toddler</t>
+  </si>
+  <si>
+    <t>Preschool</t>
+  </si>
+  <si>
+    <t>Bebê</t>
+  </si>
+  <si>
+    <t>Pré Escola</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Idade Escolar </t>
+  </si>
+  <si>
+    <t>Engatinhar</t>
+  </si>
+  <si>
+    <t>Segurar coisas</t>
+  </si>
+  <si>
+    <t>Virar</t>
+  </si>
+  <si>
+    <t>Sentar</t>
+  </si>
+  <si>
+    <t>Andar</t>
+  </si>
+  <si>
+    <t>Falar</t>
+  </si>
+  <si>
+    <t>Primeiro Sorriso</t>
+  </si>
+  <si>
+    <t>Reconhece Pai e Mãe</t>
+  </si>
+  <si>
+    <t>Reconhece a Si Próprio</t>
+  </si>
+  <si>
+    <t>Ficar em Pé</t>
+  </si>
+  <si>
+    <t>Desfralde</t>
+  </si>
+  <si>
+    <t>Alimentos Sólidos</t>
+  </si>
+  <si>
+    <t>Desmame</t>
+  </si>
+  <si>
+    <t>First Tooth</t>
+  </si>
+  <si>
+    <t>Babble</t>
+  </si>
+  <si>
+    <t>Call the Parents</t>
+  </si>
+  <si>
+    <t>Crawl</t>
+  </si>
+  <si>
+    <t>Turn</t>
+  </si>
+  <si>
+    <t>Sit</t>
+  </si>
+  <si>
+    <t>Weaning</t>
+  </si>
+  <si>
+    <t>Walk</t>
+  </si>
+  <si>
+    <t>Speak</t>
+  </si>
+  <si>
+    <t>First Smile</t>
+  </si>
+  <si>
+    <t>Recognizes Father and Mother</t>
+  </si>
+  <si>
+    <t>Recognize Himself</t>
+  </si>
+  <si>
+    <t>Stand Up</t>
+  </si>
+  <si>
+    <t>Solid Food</t>
+  </si>
+  <si>
+    <t>Holding Things</t>
+  </si>
+  <si>
+    <t>Use Toilet</t>
+  </si>
+  <si>
+    <t>Controle da Cabeça</t>
+  </si>
+  <si>
+    <t>Head Control</t>
+  </si>
+  <si>
+    <t>Infant</t>
+  </si>
+  <si>
+    <t>School Age</t>
+  </si>
+  <si>
+    <t>Adolescence</t>
   </si>
 </sst>
 </file>
@@ -2102,7 +2237,7 @@
   <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3331,8 +3466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A61B1D1-1498-4062-8FF1-43F1DDC4F5BE}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3856,8 +3991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{391AE3A0-7DB7-4C1A-B882-6DBA4383A0D7}">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:O2"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3918,8 +4053,8 @@
         <v>341</v>
       </c>
       <c r="G2" t="str">
-        <f>"(:VaccineDose {name: '" &amp; E2 &amp;"', vaccine: '" &amp; A2 &amp;"', fromAgeInMonths: toInteger(" &amp; C2 &amp;"), toAgeInMonths:toInteger(" &amp; D2 &amp;"), classification: '" &amp; F2 &amp;"'}),"</f>
-        <v>(:VaccineDose {name: 'Unique', vaccine: 'BCG ID', fromAgeInMonths: toInteger(1), toAgeInMonths:toInteger(1), classification: 'Mandatory'}),</v>
+        <f>"(:VaccineDose {name: '" &amp; E2 &amp;"', vaccineName: '" &amp; A2 &amp;"', fromAgeInMonths: toInteger(" &amp; C2 &amp;"), toAgeInMonths:toInteger(" &amp; D2 &amp;"), classification: '" &amp; F2 &amp;"'}),"</f>
+        <v>(:VaccineDose {name: 'Unique', vaccineName: 'BCG ID', fromAgeInMonths: toInteger(1), toAgeInMonths:toInteger(1), classification: 'Mandatory'}),</v>
       </c>
       <c r="O2" t="str">
         <f>"MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '" &amp; A2 &amp; "' AND d.vaccine = '" &amp; A2 &amp; "' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);"</f>
@@ -3947,8 +4082,8 @@
         <v>341</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G55" si="1">"(:VaccineDose {name: '" &amp; E3 &amp;"', vaccine: '" &amp; A3 &amp;"', fromAgeInMonths: toInteger(" &amp; C3 &amp;"), toAgeInMonths:toInteger(" &amp; D3 &amp;"), classification: '" &amp; F3 &amp;"'}),"</f>
-        <v>(:VaccineDose {name: '1st dose', vaccine: 'Hepatite B', fromAgeInMonths: toInteger(1), toAgeInMonths:toInteger(1), classification: 'Mandatory'}),</v>
+        <f t="shared" ref="G3:G55" si="1">"(:VaccineDose {name: '" &amp; E3 &amp;"', vaccineName: '" &amp; A3 &amp;"', fromAgeInMonths: toInteger(" &amp; C3 &amp;"), toAgeInMonths:toInteger(" &amp; D3 &amp;"), classification: '" &amp; F3 &amp;"'}),"</f>
+        <v>(:VaccineDose {name: '1st dose', vaccineName: 'Hepatite B', fromAgeInMonths: toInteger(1), toAgeInMonths:toInteger(1), classification: 'Mandatory'}),</v>
       </c>
       <c r="O3" t="str">
         <f t="shared" ref="O3:O55" si="2">"MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '" &amp; A3 &amp; "' AND d.vaccine = '" &amp; A3 &amp; "' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);"</f>
@@ -3977,7 +4112,7 @@
       </c>
       <c r="G4" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '2nd dose', vaccine: 'Hepatite B', fromAgeInMonths: toInteger(2), toAgeInMonths:toInteger(2), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: '2nd dose', vaccineName: 'Hepatite B', fromAgeInMonths: toInteger(2), toAgeInMonths:toInteger(2), classification: 'Mandatory'}),</v>
       </c>
       <c r="O4" t="str">
         <f t="shared" si="2"/>
@@ -4006,7 +4141,7 @@
       </c>
       <c r="G5" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '3rd dose', vaccine: 'Hepatite B', fromAgeInMonths: toInteger(6), toAgeInMonths:toInteger(6), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: '3rd dose', vaccineName: 'Hepatite B', fromAgeInMonths: toInteger(6), toAgeInMonths:toInteger(6), classification: 'Mandatory'}),</v>
       </c>
       <c r="O5" t="str">
         <f t="shared" si="2"/>
@@ -4035,7 +4170,7 @@
       </c>
       <c r="G6" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '1st dose', vaccine: 'DTPw', fromAgeInMonths: toInteger(2), toAgeInMonths:toInteger(2), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: '1st dose', vaccineName: 'DTPw', fromAgeInMonths: toInteger(2), toAgeInMonths:toInteger(2), classification: 'Mandatory'}),</v>
       </c>
       <c r="O6" t="str">
         <f t="shared" si="2"/>
@@ -4064,7 +4199,7 @@
       </c>
       <c r="G7" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '2nd dose', vaccine: 'DTPw', fromAgeInMonths: toInteger(4), toAgeInMonths:toInteger(4), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: '2nd dose', vaccineName: 'DTPw', fromAgeInMonths: toInteger(4), toAgeInMonths:toInteger(4), classification: 'Mandatory'}),</v>
       </c>
       <c r="O7" t="str">
         <f t="shared" si="2"/>
@@ -4093,7 +4228,7 @@
       </c>
       <c r="G8" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '3rd dose', vaccine: 'DTPw', fromAgeInMonths: toInteger(6), toAgeInMonths:toInteger(6), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: '3rd dose', vaccineName: 'DTPw', fromAgeInMonths: toInteger(6), toAgeInMonths:toInteger(6), classification: 'Mandatory'}),</v>
       </c>
       <c r="O8" t="str">
         <f t="shared" si="2"/>
@@ -4122,7 +4257,7 @@
       </c>
       <c r="G9" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Booster', vaccine: 'DTPw', fromAgeInMonths: toInteger(15), toAgeInMonths:toInteger(18), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: 'Booster', vaccineName: 'DTPw', fromAgeInMonths: toInteger(15), toAgeInMonths:toInteger(18), classification: 'Mandatory'}),</v>
       </c>
       <c r="O9" t="str">
         <f t="shared" si="2"/>
@@ -4151,7 +4286,7 @@
       </c>
       <c r="G10" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Booster', vaccine: 'DTPw', fromAgeInMonths: toInteger(48), toAgeInMonths:toInteger(60), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: 'Booster', vaccineName: 'DTPw', fromAgeInMonths: toInteger(48), toAgeInMonths:toInteger(60), classification: 'Mandatory'}),</v>
       </c>
       <c r="O10" t="str">
         <f t="shared" si="2"/>
@@ -4180,7 +4315,7 @@
       </c>
       <c r="G11" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '1st dose', vaccine: 'H Influenzae', fromAgeInMonths: toInteger(2), toAgeInMonths:toInteger(2), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: '1st dose', vaccineName: 'H Influenzae', fromAgeInMonths: toInteger(2), toAgeInMonths:toInteger(2), classification: 'Mandatory'}),</v>
       </c>
       <c r="O11" t="str">
         <f t="shared" si="2"/>
@@ -4209,7 +4344,7 @@
       </c>
       <c r="G12" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '2nd dose', vaccine: 'H Influenzae', fromAgeInMonths: toInteger(4), toAgeInMonths:toInteger(4), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: '2nd dose', vaccineName: 'H Influenzae', fromAgeInMonths: toInteger(4), toAgeInMonths:toInteger(4), classification: 'Mandatory'}),</v>
       </c>
       <c r="O12" t="str">
         <f t="shared" si="2"/>
@@ -4238,7 +4373,7 @@
       </c>
       <c r="G13" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '3rd dose', vaccine: 'H Influenzae', fromAgeInMonths: toInteger(6), toAgeInMonths:toInteger(6), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: '3rd dose', vaccineName: 'H Influenzae', fromAgeInMonths: toInteger(6), toAgeInMonths:toInteger(6), classification: 'Mandatory'}),</v>
       </c>
       <c r="O13" t="str">
         <f t="shared" si="2"/>
@@ -4267,7 +4402,7 @@
       </c>
       <c r="G14" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Booster', vaccine: 'H Influenzae', fromAgeInMonths: toInteger(15), toAgeInMonths:toInteger(18), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: 'Booster', vaccineName: 'H Influenzae', fromAgeInMonths: toInteger(15), toAgeInMonths:toInteger(18), classification: 'Mandatory'}),</v>
       </c>
       <c r="O14" t="str">
         <f t="shared" si="2"/>
@@ -4296,7 +4431,7 @@
       </c>
       <c r="G15" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '1st dose', vaccine: 'Pólio VIP', fromAgeInMonths: toInteger(2), toAgeInMonths:toInteger(2), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: '1st dose', vaccineName: 'Pólio VIP', fromAgeInMonths: toInteger(2), toAgeInMonths:toInteger(2), classification: 'Mandatory'}),</v>
       </c>
       <c r="O15" t="str">
         <f t="shared" si="2"/>
@@ -4325,7 +4460,7 @@
       </c>
       <c r="G16" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '2nd dose', vaccine: 'Pólio VIP', fromAgeInMonths: toInteger(4), toAgeInMonths:toInteger(4), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: '2nd dose', vaccineName: 'Pólio VIP', fromAgeInMonths: toInteger(4), toAgeInMonths:toInteger(4), classification: 'Mandatory'}),</v>
       </c>
       <c r="O16" t="str">
         <f t="shared" si="2"/>
@@ -4354,7 +4489,7 @@
       </c>
       <c r="G17" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '3rd dose', vaccine: 'Pólio VIP', fromAgeInMonths: toInteger(6), toAgeInMonths:toInteger(6), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: '3rd dose', vaccineName: 'Pólio VIP', fromAgeInMonths: toInteger(6), toAgeInMonths:toInteger(6), classification: 'Mandatory'}),</v>
       </c>
       <c r="O17" t="str">
         <f t="shared" si="2"/>
@@ -4383,7 +4518,7 @@
       </c>
       <c r="G18" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Booster', vaccine: 'Pólio VOP', fromAgeInMonths: toInteger(15), toAgeInMonths:toInteger(18), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: 'Booster', vaccineName: 'Pólio VOP', fromAgeInMonths: toInteger(15), toAgeInMonths:toInteger(18), classification: 'Mandatory'}),</v>
       </c>
       <c r="O18" t="str">
         <f t="shared" si="2"/>
@@ -4412,7 +4547,7 @@
       </c>
       <c r="G19" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Booster', vaccine: 'Pólio VOP', fromAgeInMonths: toInteger(48), toAgeInMonths:toInteger(60), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: 'Booster', vaccineName: 'Pólio VOP', fromAgeInMonths: toInteger(48), toAgeInMonths:toInteger(60), classification: 'Mandatory'}),</v>
       </c>
       <c r="O19" t="str">
         <f t="shared" si="2"/>
@@ -4441,7 +4576,7 @@
       </c>
       <c r="G20" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '1st dose', vaccine: 'Rotavírus', fromAgeInMonths: toInteger(2), toAgeInMonths:toInteger(4), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: '1st dose', vaccineName: 'Rotavírus', fromAgeInMonths: toInteger(2), toAgeInMonths:toInteger(4), classification: 'Mandatory'}),</v>
       </c>
       <c r="O20" t="str">
         <f t="shared" si="2"/>
@@ -4470,7 +4605,7 @@
       </c>
       <c r="G21" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '2nd dose', vaccine: 'Rotavírus', fromAgeInMonths: toInteger(5), toAgeInMonths:toInteger(8), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: '2nd dose', vaccineName: 'Rotavírus', fromAgeInMonths: toInteger(5), toAgeInMonths:toInteger(8), classification: 'Mandatory'}),</v>
       </c>
       <c r="O21" t="str">
         <f t="shared" si="2"/>
@@ -4499,7 +4634,7 @@
       </c>
       <c r="G22" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '1st dose', vaccine: 'VPC10', fromAgeInMonths: toInteger(2), toAgeInMonths:toInteger(3), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: '1st dose', vaccineName: 'VPC10', fromAgeInMonths: toInteger(2), toAgeInMonths:toInteger(3), classification: 'Mandatory'}),</v>
       </c>
       <c r="O22" t="str">
         <f t="shared" si="2"/>
@@ -4528,7 +4663,7 @@
       </c>
       <c r="G23" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '2nd dose', vaccine: 'VPC10', fromAgeInMonths: toInteger(4), toAgeInMonths:toInteger(6), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: '2nd dose', vaccineName: 'VPC10', fromAgeInMonths: toInteger(4), toAgeInMonths:toInteger(6), classification: 'Mandatory'}),</v>
       </c>
       <c r="O23" t="str">
         <f t="shared" si="2"/>
@@ -4557,7 +4692,7 @@
       </c>
       <c r="G24" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Booster', vaccine: 'VPC10', fromAgeInMonths: toInteger(12), toAgeInMonths:toInteger(15), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: 'Booster', vaccineName: 'VPC10', fromAgeInMonths: toInteger(12), toAgeInMonths:toInteger(15), classification: 'Mandatory'}),</v>
       </c>
       <c r="O24" t="str">
         <f t="shared" si="2"/>
@@ -4586,7 +4721,7 @@
       </c>
       <c r="G25" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '1st dose', vaccine: 'ACWY/C', fromAgeInMonths: toInteger(3), toAgeInMonths:toInteger(5), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: '1st dose', vaccineName: 'ACWY/C', fromAgeInMonths: toInteger(3), toAgeInMonths:toInteger(5), classification: 'Mandatory'}),</v>
       </c>
       <c r="O25" t="str">
         <f t="shared" si="2"/>
@@ -4615,7 +4750,7 @@
       </c>
       <c r="G26" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '2nd dose', vaccine: 'ACWY/C', fromAgeInMonths: toInteger(6), toAgeInMonths:toInteger(8), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: '2nd dose', vaccineName: 'ACWY/C', fromAgeInMonths: toInteger(6), toAgeInMonths:toInteger(8), classification: 'Mandatory'}),</v>
       </c>
       <c r="O26" t="str">
         <f t="shared" si="2"/>
@@ -4644,7 +4779,7 @@
       </c>
       <c r="G27" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Booster', vaccine: 'ACWY/C', fromAgeInMonths: toInteger(12), toAgeInMonths:toInteger(15), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: 'Booster', vaccineName: 'ACWY/C', fromAgeInMonths: toInteger(12), toAgeInMonths:toInteger(15), classification: 'Mandatory'}),</v>
       </c>
       <c r="O27" t="str">
         <f t="shared" si="2"/>
@@ -4673,7 +4808,7 @@
       </c>
       <c r="G28" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Booster', vaccine: 'ACWY/C', fromAgeInMonths: toInteger(60), toAgeInMonths:toInteger(72), classification: 'Optional'}),</v>
+        <v>(:VaccineDose {name: 'Booster', vaccineName: 'ACWY/C', fromAgeInMonths: toInteger(60), toAgeInMonths:toInteger(72), classification: 'Optional'}),</v>
       </c>
       <c r="O28" t="str">
         <f t="shared" si="2"/>
@@ -4702,7 +4837,7 @@
       </c>
       <c r="G29" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '1st dose', vaccine: 'Meningocócica B', fromAgeInMonths: toInteger(3), toAgeInMonths:toInteger(3), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: '1st dose', vaccineName: 'Meningocócica B', fromAgeInMonths: toInteger(3), toAgeInMonths:toInteger(3), classification: 'Mandatory'}),</v>
       </c>
       <c r="O29" t="str">
         <f t="shared" si="2"/>
@@ -4731,7 +4866,7 @@
       </c>
       <c r="G30" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '2nd dose', vaccine: 'Meningocócica B', fromAgeInMonths: toInteger(5), toAgeInMonths:toInteger(5), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: '2nd dose', vaccineName: 'Meningocócica B', fromAgeInMonths: toInteger(5), toAgeInMonths:toInteger(5), classification: 'Mandatory'}),</v>
       </c>
       <c r="O30" t="str">
         <f t="shared" si="2"/>
@@ -4760,7 +4895,7 @@
       </c>
       <c r="G31" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Booster', vaccine: 'Meningocócica B', fromAgeInMonths: toInteger(12), toAgeInMonths:toInteger(15), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: 'Booster', vaccineName: 'Meningocócica B', fromAgeInMonths: toInteger(12), toAgeInMonths:toInteger(15), classification: 'Mandatory'}),</v>
       </c>
       <c r="O31" t="str">
         <f t="shared" si="2"/>
@@ -4789,7 +4924,7 @@
       </c>
       <c r="G32" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Annual', vaccine: '3V', fromAgeInMonths: toInteger(6), toAgeInMonths:toInteger(12), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: 'Annual', vaccineName: '3V', fromAgeInMonths: toInteger(6), toAgeInMonths:toInteger(12), classification: 'Mandatory'}),</v>
       </c>
       <c r="O32" t="str">
         <f t="shared" si="2"/>
@@ -4818,7 +4953,7 @@
       </c>
       <c r="G33" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Annual', vaccine: '3V', fromAgeInMonths: toInteger(13), toAgeInMonths:toInteger(24), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: 'Annual', vaccineName: '3V', fromAgeInMonths: toInteger(13), toAgeInMonths:toInteger(24), classification: 'Mandatory'}),</v>
       </c>
       <c r="O33" t="str">
         <f t="shared" si="2"/>
@@ -4847,7 +4982,7 @@
       </c>
       <c r="G34" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Annual', vaccine: '3V', fromAgeInMonths: toInteger(25), toAgeInMonths:toInteger(36), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: 'Annual', vaccineName: '3V', fromAgeInMonths: toInteger(25), toAgeInMonths:toInteger(36), classification: 'Mandatory'}),</v>
       </c>
       <c r="O34" t="str">
         <f t="shared" si="2"/>
@@ -4876,7 +5011,7 @@
       </c>
       <c r="G35" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Annual', vaccine: '3V', fromAgeInMonths: toInteger(37), toAgeInMonths:toInteger(48), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: 'Annual', vaccineName: '3V', fromAgeInMonths: toInteger(37), toAgeInMonths:toInteger(48), classification: 'Mandatory'}),</v>
       </c>
       <c r="O35" t="str">
         <f t="shared" si="2"/>
@@ -4905,7 +5040,7 @@
       </c>
       <c r="G36" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Annual', vaccine: '3V', fromAgeInMonths: toInteger(49), toAgeInMonths:toInteger(60), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: 'Annual', vaccineName: '3V', fromAgeInMonths: toInteger(49), toAgeInMonths:toInteger(60), classification: 'Mandatory'}),</v>
       </c>
       <c r="O36" t="str">
         <f t="shared" si="2"/>
@@ -4934,7 +5069,7 @@
       </c>
       <c r="G37" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Annual', vaccine: '3V', fromAgeInMonths: toInteger(61), toAgeInMonths:toInteger(72), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: 'Annual', vaccineName: '3V', fromAgeInMonths: toInteger(61), toAgeInMonths:toInteger(72), classification: 'Mandatory'}),</v>
       </c>
       <c r="O37" t="str">
         <f t="shared" si="2"/>
@@ -4963,7 +5098,7 @@
       </c>
       <c r="G38" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Annual', vaccine: '3V', fromAgeInMonths: toInteger(73), toAgeInMonths:toInteger(84), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: 'Annual', vaccineName: '3V', fromAgeInMonths: toInteger(73), toAgeInMonths:toInteger(84), classification: 'Mandatory'}),</v>
       </c>
       <c r="O38" t="str">
         <f t="shared" si="2"/>
@@ -4992,7 +5127,7 @@
       </c>
       <c r="G39" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Annual', vaccine: '3V', fromAgeInMonths: toInteger(85), toAgeInMonths:toInteger(96), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: 'Annual', vaccineName: '3V', fromAgeInMonths: toInteger(85), toAgeInMonths:toInteger(96), classification: 'Mandatory'}),</v>
       </c>
       <c r="O39" t="str">
         <f t="shared" si="2"/>
@@ -5021,7 +5156,7 @@
       </c>
       <c r="G40" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Annual', vaccine: '3V', fromAgeInMonths: toInteger(97), toAgeInMonths:toInteger(108), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: 'Annual', vaccineName: '3V', fromAgeInMonths: toInteger(97), toAgeInMonths:toInteger(108), classification: 'Mandatory'}),</v>
       </c>
       <c r="O40" t="str">
         <f t="shared" si="2"/>
@@ -5050,7 +5185,7 @@
       </c>
       <c r="G41" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Annual', vaccine: '3V', fromAgeInMonths: toInteger(109), toAgeInMonths:toInteger(120), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: 'Annual', vaccineName: '3V', fromAgeInMonths: toInteger(109), toAgeInMonths:toInteger(120), classification: 'Mandatory'}),</v>
       </c>
       <c r="O41" t="str">
         <f t="shared" si="2"/>
@@ -5079,7 +5214,7 @@
       </c>
       <c r="G42" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Unique', vaccine: 'Febre amarela', fromAgeInMonths: toInteger(9), toAgeInMonths:toInteger(9), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: 'Unique', vaccineName: 'Febre amarela', fromAgeInMonths: toInteger(9), toAgeInMonths:toInteger(9), classification: 'Mandatory'}),</v>
       </c>
       <c r="O42" t="str">
         <f t="shared" si="2"/>
@@ -5108,7 +5243,7 @@
       </c>
       <c r="G43" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '1st dose', vaccine: 'Hepatite A', fromAgeInMonths: toInteger(12), toAgeInMonths:toInteger(12), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: '1st dose', vaccineName: 'Hepatite A', fromAgeInMonths: toInteger(12), toAgeInMonths:toInteger(12), classification: 'Mandatory'}),</v>
       </c>
       <c r="O43" t="str">
         <f t="shared" si="2"/>
@@ -5137,7 +5272,7 @@
       </c>
       <c r="G44" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '2nd dose', vaccine: 'Hepatite A', fromAgeInMonths: toInteger(18), toAgeInMonths:toInteger(18), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: '2nd dose', vaccineName: 'Hepatite A', fromAgeInMonths: toInteger(18), toAgeInMonths:toInteger(18), classification: 'Mandatory'}),</v>
       </c>
       <c r="O44" t="str">
         <f t="shared" si="2"/>
@@ -5166,7 +5301,7 @@
       </c>
       <c r="G45" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '1st dose', vaccine: 'BCG', fromAgeInMonths: toInteger(12), toAgeInMonths:toInteger(12), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: '1st dose', vaccineName: 'BCG', fromAgeInMonths: toInteger(12), toAgeInMonths:toInteger(12), classification: 'Mandatory'}),</v>
       </c>
       <c r="O45" t="str">
         <f t="shared" si="2"/>
@@ -5195,7 +5330,7 @@
       </c>
       <c r="G46" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '2nd dose', vaccine: 'BCG', fromAgeInMonths: toInteger(15), toAgeInMonths:toInteger(24), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: '2nd dose', vaccineName: 'BCG', fromAgeInMonths: toInteger(15), toAgeInMonths:toInteger(24), classification: 'Mandatory'}),</v>
       </c>
       <c r="O46" t="str">
         <f t="shared" si="2"/>
@@ -5224,7 +5359,7 @@
       </c>
       <c r="G47" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '1st dose', vaccine: 'Varicela', fromAgeInMonths: toInteger(12), toAgeInMonths:toInteger(12), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: '1st dose', vaccineName: 'Varicela', fromAgeInMonths: toInteger(12), toAgeInMonths:toInteger(12), classification: 'Mandatory'}),</v>
       </c>
       <c r="O47" t="str">
         <f t="shared" si="2"/>
@@ -5253,7 +5388,7 @@
       </c>
       <c r="G48" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '2nd dose', vaccine: 'Varicela', fromAgeInMonths: toInteger(15), toAgeInMonths:toInteger(24), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: '2nd dose', vaccineName: 'Varicela', fromAgeInMonths: toInteger(15), toAgeInMonths:toInteger(24), classification: 'Mandatory'}),</v>
       </c>
       <c r="O48" t="str">
         <f t="shared" si="2"/>
@@ -5282,7 +5417,7 @@
       </c>
       <c r="G49" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '1st dose', vaccine: 'HPV4', fromAgeInMonths: toInteger(108), toAgeInMonths:toInteger(119), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: '1st dose', vaccineName: 'HPV4', fromAgeInMonths: toInteger(108), toAgeInMonths:toInteger(119), classification: 'Mandatory'}),</v>
       </c>
       <c r="O49" t="str">
         <f t="shared" si="2"/>
@@ -5311,7 +5446,7 @@
       </c>
       <c r="G50" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '2nd dose', vaccine: 'HPV4', fromAgeInMonths: toInteger(120), toAgeInMonths:toInteger(132), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: '2nd dose', vaccineName: 'HPV4', fromAgeInMonths: toInteger(120), toAgeInMonths:toInteger(132), classification: 'Mandatory'}),</v>
       </c>
       <c r="O50" t="str">
         <f t="shared" si="2"/>
@@ -5340,7 +5475,7 @@
       </c>
       <c r="G51" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '1st dose', vaccine: 'DTPa', fromAgeInMonths: toInteger(2), toAgeInMonths:toInteger(2), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: '1st dose', vaccineName: 'DTPa', fromAgeInMonths: toInteger(2), toAgeInMonths:toInteger(2), classification: 'Mandatory'}),</v>
       </c>
       <c r="O51" t="str">
         <f t="shared" si="2"/>
@@ -5369,7 +5504,7 @@
       </c>
       <c r="G52" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '2nd dose', vaccine: 'DTPa', fromAgeInMonths: toInteger(4), toAgeInMonths:toInteger(4), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: '2nd dose', vaccineName: 'DTPa', fromAgeInMonths: toInteger(4), toAgeInMonths:toInteger(4), classification: 'Mandatory'}),</v>
       </c>
       <c r="O52" t="str">
         <f t="shared" si="2"/>
@@ -5398,7 +5533,7 @@
       </c>
       <c r="G53" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: '3rd dose', vaccine: 'DTPa', fromAgeInMonths: toInteger(6), toAgeInMonths:toInteger(6), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: '3rd dose', vaccineName: 'DTPa', fromAgeInMonths: toInteger(6), toAgeInMonths:toInteger(6), classification: 'Mandatory'}),</v>
       </c>
       <c r="O53" t="str">
         <f t="shared" si="2"/>
@@ -5427,7 +5562,7 @@
       </c>
       <c r="G54" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Booster', vaccine: 'DTPa', fromAgeInMonths: toInteger(15), toAgeInMonths:toInteger(18), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: 'Booster', vaccineName: 'DTPa', fromAgeInMonths: toInteger(15), toAgeInMonths:toInteger(18), classification: 'Mandatory'}),</v>
       </c>
       <c r="O54" t="str">
         <f t="shared" si="2"/>
@@ -5456,7 +5591,7 @@
       </c>
       <c r="G55" t="str">
         <f t="shared" si="1"/>
-        <v>(:VaccineDose {name: 'Booster', vaccine: 'DTPa', fromAgeInMonths: toInteger(48), toAgeInMonths:toInteger(60), classification: 'Mandatory'}),</v>
+        <v>(:VaccineDose {name: 'Booster', vaccineName: 'DTPa', fromAgeInMonths: toInteger(48), toAgeInMonths:toInteger(60), classification: 'Mandatory'}),</v>
       </c>
       <c r="O55" t="str">
         <f t="shared" si="2"/>
@@ -5473,7 +5608,7 @@
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8449,163 +8584,332 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE4D6E2-6BDE-4AC5-843C-AEB3BD0CAE9C}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="14" customWidth="1"/>
+    <col min="1" max="3" width="15.88671875" customWidth="1"/>
     <col min="4" max="4" width="30.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>569</v>
       </c>
       <c r="B1" t="s">
         <v>570</v>
       </c>
+      <c r="C1" t="s">
+        <v>574</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="K1" t="s">
+        <v>569</v>
+      </c>
+      <c r="L1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>571</v>
       </c>
       <c r="B2" t="s">
-        <v>540</v>
+        <v>598</v>
+      </c>
+      <c r="C2" t="s">
+        <v>616</v>
       </c>
       <c r="D2" t="str">
-        <f>"(:Milestone {uuid: apoc.create.uuid(), name: '" &amp; B2 &amp;"', inPortuguese: '" &amp; A2 &amp;"'}),"</f>
-        <v>(:Milestone {uuid: apoc.create.uuid(), name: 'Surgery', inPortuguese: 'Primeiro Dente'}),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <f>"(:Milestone {uuid: apoc.create.uuid(), name: '" &amp; B2 &amp;"', inPortuguese: '" &amp; A2 &amp;"', stage: '" &amp; C2 &amp;"'}),"</f>
+        <v>(:Milestone {uuid: apoc.create.uuid(), name: 'First Tooth', inPortuguese: 'Primeiro Dente', stage: 'Infant'}),</v>
+      </c>
+      <c r="K2" t="s">
+        <v>575</v>
+      </c>
+      <c r="L2" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>572</v>
       </c>
       <c r="B3" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>599</v>
+      </c>
+      <c r="C3" t="s">
+        <v>616</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D18" si="0">"(:Milestone {uuid: apoc.create.uuid(), name: '" &amp; B3 &amp;"', inPortuguese: '" &amp; A3 &amp;"', stage: '" &amp; C3 &amp;"'}),"</f>
+        <v>(:Milestone {uuid: apoc.create.uuid(), name: 'Babble', inPortuguese: 'Balbuciar', stage: 'Infant'}),</v>
+      </c>
+      <c r="K3" t="s">
+        <v>582</v>
+      </c>
+      <c r="L3" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>573</v>
       </c>
       <c r="B4" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>600</v>
+      </c>
+      <c r="C4" t="s">
+        <v>580</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Milestone {uuid: apoc.create.uuid(), name: 'Call the Parents', inPortuguese: 'Chamar os Pais', stage: 'Toddler'}),</v>
+      </c>
+      <c r="K4" t="s">
+        <v>576</v>
+      </c>
+      <c r="L4" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>554</v>
+        <v>585</v>
       </c>
       <c r="B5" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>601</v>
+      </c>
+      <c r="C5" t="s">
+        <v>580</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Milestone {uuid: apoc.create.uuid(), name: 'Crawl', inPortuguese: 'Engatinhar', stage: 'Toddler'}),</v>
+      </c>
+      <c r="K5" t="s">
+        <v>583</v>
+      </c>
+      <c r="L5" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>555</v>
+        <v>586</v>
       </c>
       <c r="B6" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>612</v>
+      </c>
+      <c r="C6" t="s">
+        <v>580</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Milestone {uuid: apoc.create.uuid(), name: 'Holding Things', inPortuguese: 'Segurar coisas', stage: 'Toddler'}),</v>
+      </c>
+      <c r="K6" t="s">
+        <v>584</v>
+      </c>
+      <c r="L6" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>545</v>
+        <v>614</v>
       </c>
       <c r="B7" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>615</v>
+      </c>
+      <c r="C7" t="s">
+        <v>580</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Milestone {uuid: apoc.create.uuid(), name: 'Head Control', inPortuguese: 'Controle da Cabeça', stage: 'Toddler'}),</v>
+      </c>
+      <c r="K7" t="s">
+        <v>578</v>
+      </c>
+      <c r="L7" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>556</v>
+        <v>587</v>
       </c>
       <c r="B8" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>602</v>
+      </c>
+      <c r="C8" t="s">
+        <v>616</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Milestone {uuid: apoc.create.uuid(), name: 'Turn', inPortuguese: 'Virar', stage: 'Infant'}),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>557</v>
+        <v>588</v>
       </c>
       <c r="B9" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>603</v>
+      </c>
+      <c r="C9" t="s">
+        <v>580</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Milestone {uuid: apoc.create.uuid(), name: 'Sit', inPortuguese: 'Sentar', stage: 'Toddler'}),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>558</v>
+        <v>597</v>
       </c>
       <c r="B10" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>604</v>
+      </c>
+      <c r="C10" t="s">
+        <v>580</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Milestone {uuid: apoc.create.uuid(), name: 'Weaning', inPortuguese: 'Desmame', stage: 'Toddler'}),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>559</v>
+        <v>589</v>
       </c>
       <c r="B11" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>605</v>
+      </c>
+      <c r="C11" t="s">
+        <v>580</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Milestone {uuid: apoc.create.uuid(), name: 'Walk', inPortuguese: 'Andar', stage: 'Toddler'}),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>297</v>
+        <v>590</v>
       </c>
       <c r="B12" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>606</v>
+      </c>
+      <c r="C12" t="s">
+        <v>581</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Milestone {uuid: apoc.create.uuid(), name: 'Speak', inPortuguese: 'Falar', stage: 'Preschool'}),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>298</v>
+        <v>591</v>
       </c>
       <c r="B13" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>607</v>
+      </c>
+      <c r="C13" t="s">
+        <v>616</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Milestone {uuid: apoc.create.uuid(), name: 'First Smile', inPortuguese: 'Primeiro Sorriso', stage: 'Infant'}),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>300</v>
+        <v>592</v>
       </c>
       <c r="B14" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>608</v>
+      </c>
+      <c r="C14" t="s">
+        <v>616</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Milestone {uuid: apoc.create.uuid(), name: 'Recognizes Father and Mother', inPortuguese: 'Reconhece Pai e Mãe', stage: 'Infant'}),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>560</v>
+        <v>593</v>
       </c>
       <c r="B15" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>609</v>
+      </c>
+      <c r="C15" t="s">
+        <v>616</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Milestone {uuid: apoc.create.uuid(), name: 'Recognize Himself', inPortuguese: 'Reconhece a Si Próprio', stage: 'Infant'}),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>566</v>
+        <v>594</v>
       </c>
       <c r="B16" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+        <v>610</v>
+      </c>
+      <c r="C16" t="s">
+        <v>580</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Milestone {uuid: apoc.create.uuid(), name: 'Stand Up', inPortuguese: 'Ficar em Pé', stage: 'Toddler'}),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>567</v>
+        <v>595</v>
       </c>
       <c r="B17" t="s">
-        <v>565</v>
+        <v>613</v>
+      </c>
+      <c r="C17" t="s">
+        <v>580</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Milestone {uuid: apoc.create.uuid(), name: 'Use Toilet', inPortuguese: 'Desfralde', stage: 'Toddler'}),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>596</v>
+      </c>
+      <c r="B18" t="s">
+        <v>611</v>
+      </c>
+      <c r="C18" t="s">
+        <v>580</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>(:Milestone {uuid: apoc.create.uuid(), name: 'Solid Food', inPortuguese: 'Alimentos Sólidos', stage: 'Toddler'}),</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>